<commit_message>
numbers working to end of ri2
</commit_message>
<xml_diff>
--- a/ftest/data/fm24/Worked_Example_Calculation_Net_Loss_Pre_Cat_Simple_Complex_Test_Case_working.xlsx
+++ b/ftest/data/fm24/Worked_Example_Calculation_Net_Loss_Pre_Cat_Simple_Complex_Test_Case_working.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="-12" windowWidth="18972" windowHeight="5916" activeTab="3"/>
+    <workbookView xWindow="-12" yWindow="-12" windowWidth="18972" windowHeight="5916" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="9" r:id="rId1"/>
@@ -1087,6 +1087,21 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1115,21 +1130,6 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1631,8 +1631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V33"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14:R14"/>
+    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2925,11 +2925,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U166"/>
   <sheetViews>
-    <sheetView zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <pane xSplit="4" ySplit="7" topLeftCell="E17" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
+      <pane xSplit="4" ySplit="7" topLeftCell="E53" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="K25" sqref="K25:N25"/>
+      <selection pane="bottomRight" activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3085,11 +3085,11 @@
       <c r="U7" s="10"/>
     </row>
     <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="112" t="s">
+      <c r="A8" s="117" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="113"/>
-      <c r="C8" s="114"/>
+      <c r="B8" s="118"/>
+      <c r="C8" s="119"/>
       <c r="D8" s="33" t="s">
         <v>38</v>
       </c>
@@ -3154,9 +3154,9 @@
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A9" s="115"/>
-      <c r="B9" s="116"/>
-      <c r="C9" s="117"/>
+      <c r="A9" s="120"/>
+      <c r="B9" s="121"/>
+      <c r="C9" s="122"/>
       <c r="D9" s="33" t="s">
         <v>39</v>
       </c>
@@ -3221,9 +3221,9 @@
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A10" s="115"/>
-      <c r="B10" s="116"/>
-      <c r="C10" s="117"/>
+      <c r="A10" s="120"/>
+      <c r="B10" s="121"/>
+      <c r="C10" s="122"/>
       <c r="D10" s="33" t="s">
         <v>40</v>
       </c>
@@ -3288,9 +3288,9 @@
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A11" s="118"/>
-      <c r="B11" s="119"/>
-      <c r="C11" s="120"/>
+      <c r="A11" s="123"/>
+      <c r="B11" s="124"/>
+      <c r="C11" s="125"/>
       <c r="D11" s="9" t="s">
         <v>37</v>
       </c>
@@ -3375,13 +3375,13 @@
       <c r="U12" s="10"/>
     </row>
     <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="111" t="s">
+      <c r="A13" s="116" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="111" t="s">
+      <c r="B13" s="116" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="111"/>
+      <c r="C13" s="116"/>
       <c r="D13" s="34" t="s">
         <v>49</v>
       </c>
@@ -3424,9 +3424,9 @@
       </c>
     </row>
     <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="111"/>
-      <c r="B14" s="111"/>
-      <c r="C14" s="111"/>
+      <c r="A14" s="116"/>
+      <c r="B14" s="116"/>
+      <c r="C14" s="116"/>
       <c r="D14" s="34" t="s">
         <v>50</v>
       </c>
@@ -3479,9 +3479,9 @@
       <c r="U14" s="40"/>
     </row>
     <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="111"/>
-      <c r="B15" s="111"/>
-      <c r="C15" s="111"/>
+      <c r="A15" s="116"/>
+      <c r="B15" s="116"/>
+      <c r="C15" s="116"/>
       <c r="D15" s="34" t="s">
         <v>51</v>
       </c>
@@ -3534,11 +3534,11 @@
       <c r="U15" s="40"/>
     </row>
     <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="111"/>
-      <c r="B16" s="112" t="s">
+      <c r="A16" s="116"/>
+      <c r="B16" s="117" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="114"/>
+      <c r="C16" s="119"/>
       <c r="D16" s="33" t="s">
         <v>38</v>
       </c>
@@ -3603,9 +3603,9 @@
       </c>
     </row>
     <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="111"/>
-      <c r="B17" s="115"/>
-      <c r="C17" s="117"/>
+      <c r="A17" s="116"/>
+      <c r="B17" s="120"/>
+      <c r="C17" s="122"/>
       <c r="D17" s="33" t="s">
         <v>39</v>
       </c>
@@ -3670,9 +3670,9 @@
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A18" s="111"/>
-      <c r="B18" s="115"/>
-      <c r="C18" s="117"/>
+      <c r="A18" s="116"/>
+      <c r="B18" s="120"/>
+      <c r="C18" s="122"/>
       <c r="D18" s="33" t="s">
         <v>40</v>
       </c>
@@ -3737,9 +3737,9 @@
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A19" s="111"/>
-      <c r="B19" s="118"/>
-      <c r="C19" s="120"/>
+      <c r="A19" s="116"/>
+      <c r="B19" s="123"/>
+      <c r="C19" s="125"/>
       <c r="D19" s="35" t="s">
         <v>47</v>
       </c>
@@ -3844,13 +3844,13 @@
       <c r="U21" s="10"/>
     </row>
     <row r="22" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="111" t="s">
+      <c r="A22" s="116" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="111" t="s">
+      <c r="B22" s="116" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="121" t="s">
+      <c r="C22" s="113" t="s">
         <v>56</v>
       </c>
       <c r="D22" s="9" t="s">
@@ -3905,9 +3905,9 @@
       <c r="U22" s="10"/>
     </row>
     <row r="23" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="111"/>
-      <c r="B23" s="111"/>
-      <c r="C23" s="121"/>
+      <c r="A23" s="116"/>
+      <c r="B23" s="116"/>
+      <c r="C23" s="113"/>
       <c r="D23" s="9" t="s">
         <v>32</v>
       </c>
@@ -3960,9 +3960,9 @@
       <c r="U23" s="10"/>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A24" s="111"/>
-      <c r="B24" s="111"/>
-      <c r="C24" s="121"/>
+      <c r="A24" s="116"/>
+      <c r="B24" s="116"/>
+      <c r="C24" s="113"/>
       <c r="D24" s="9" t="s">
         <v>30</v>
       </c>
@@ -4015,9 +4015,9 @@
       <c r="U24" s="10"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A25" s="111"/>
-      <c r="B25" s="111"/>
-      <c r="C25" s="121"/>
+      <c r="A25" s="116"/>
+      <c r="B25" s="116"/>
+      <c r="C25" s="113"/>
       <c r="D25" s="36" t="s">
         <v>53</v>
       </c>
@@ -4070,9 +4070,9 @@
       <c r="U25" s="10"/>
     </row>
     <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="111"/>
-      <c r="B26" s="111"/>
-      <c r="C26" s="121" t="s">
+      <c r="A26" s="116"/>
+      <c r="B26" s="116"/>
+      <c r="C26" s="113" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="9" t="s">
@@ -4127,9 +4127,9 @@
       <c r="U26" s="10"/>
     </row>
     <row r="27" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="111"/>
-      <c r="B27" s="111"/>
-      <c r="C27" s="121"/>
+      <c r="A27" s="116"/>
+      <c r="B27" s="116"/>
+      <c r="C27" s="113"/>
       <c r="D27" s="36" t="s">
         <v>58</v>
       </c>
@@ -4191,11 +4191,11 @@
       <c r="U27" s="42"/>
     </row>
     <row r="28" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="111"/>
-      <c r="B28" s="111" t="s">
+      <c r="A28" s="116"/>
+      <c r="B28" s="116" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="121" t="s">
+      <c r="C28" s="113" t="s">
         <v>21</v>
       </c>
       <c r="D28" s="9" t="s">
@@ -4229,9 +4229,9 @@
       <c r="U28" s="10"/>
     </row>
     <row r="29" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="111"/>
-      <c r="B29" s="111"/>
-      <c r="C29" s="121"/>
+      <c r="A29" s="116"/>
+      <c r="B29" s="116"/>
+      <c r="C29" s="113"/>
       <c r="D29" s="36" t="s">
         <v>59</v>
       </c>
@@ -4293,9 +4293,9 @@
       <c r="U29" s="10"/>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A30" s="111"/>
-      <c r="B30" s="111"/>
-      <c r="C30" s="121" t="s">
+      <c r="A30" s="116"/>
+      <c r="B30" s="116"/>
+      <c r="C30" s="113" t="s">
         <v>57</v>
       </c>
       <c r="D30" s="9" t="s">
@@ -4329,9 +4329,9 @@
       <c r="U30" s="10"/>
     </row>
     <row r="31" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="111"/>
-      <c r="B31" s="111"/>
-      <c r="C31" s="121"/>
+      <c r="A31" s="116"/>
+      <c r="B31" s="116"/>
+      <c r="C31" s="113"/>
       <c r="D31" s="35" t="s">
         <v>60</v>
       </c>
@@ -4438,13 +4438,13 @@
       <c r="U33" s="10"/>
     </row>
     <row r="34" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="124" t="s">
+      <c r="A34" s="114" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="111" t="s">
+      <c r="B34" s="116" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="121" t="s">
+      <c r="C34" s="113" t="s">
         <v>16</v>
       </c>
       <c r="D34" s="9" t="s">
@@ -4487,9 +4487,9 @@
       <c r="U34" s="10"/>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A35" s="125"/>
-      <c r="B35" s="111"/>
-      <c r="C35" s="121"/>
+      <c r="A35" s="115"/>
+      <c r="B35" s="116"/>
+      <c r="C35" s="113"/>
       <c r="D35" s="9" t="s">
         <v>14</v>
       </c>
@@ -4530,9 +4530,9 @@
       <c r="U35" s="10"/>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A36" s="125"/>
-      <c r="B36" s="111"/>
-      <c r="C36" s="121"/>
+      <c r="A36" s="115"/>
+      <c r="B36" s="116"/>
+      <c r="C36" s="113"/>
       <c r="D36" s="9" t="s">
         <v>36</v>
       </c>
@@ -4573,9 +4573,9 @@
       <c r="U36" s="10"/>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A37" s="125"/>
-      <c r="B37" s="111"/>
-      <c r="C37" s="121"/>
+      <c r="A37" s="115"/>
+      <c r="B37" s="116"/>
+      <c r="C37" s="113"/>
       <c r="D37" s="9" t="s">
         <v>22</v>
       </c>
@@ -4616,9 +4616,9 @@
       <c r="U37" s="10"/>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A38" s="125"/>
-      <c r="B38" s="111"/>
-      <c r="C38" s="121"/>
+      <c r="A38" s="115"/>
+      <c r="B38" s="116"/>
+      <c r="C38" s="113"/>
       <c r="D38" s="48" t="s">
         <v>61</v>
       </c>
@@ -4671,9 +4671,9 @@
       <c r="U38" s="10"/>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A39" s="125"/>
-      <c r="B39" s="111"/>
-      <c r="C39" s="121"/>
+      <c r="A39" s="115"/>
+      <c r="B39" s="116"/>
+      <c r="C39" s="113"/>
       <c r="D39" s="9" t="s">
         <v>21</v>
       </c>
@@ -4714,9 +4714,9 @@
       <c r="U39" s="10"/>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A40" s="125"/>
-      <c r="B40" s="111"/>
-      <c r="C40" s="121"/>
+      <c r="A40" s="115"/>
+      <c r="B40" s="116"/>
+      <c r="C40" s="113"/>
       <c r="D40" s="48" t="s">
         <v>62</v>
       </c>
@@ -4769,9 +4769,9 @@
       <c r="U40" s="10"/>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A41" s="125"/>
-      <c r="B41" s="111"/>
-      <c r="C41" s="121"/>
+      <c r="A41" s="115"/>
+      <c r="B41" s="116"/>
+      <c r="C41" s="113"/>
       <c r="D41" s="9" t="s">
         <v>23</v>
       </c>
@@ -4812,9 +4812,9 @@
       <c r="U41" s="10"/>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A42" s="125"/>
-      <c r="B42" s="111"/>
-      <c r="C42" s="121"/>
+      <c r="A42" s="115"/>
+      <c r="B42" s="116"/>
+      <c r="C42" s="113"/>
       <c r="D42" s="48" t="s">
         <v>63</v>
       </c>
@@ -4867,9 +4867,9 @@
       <c r="U42" s="10"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A43" s="125"/>
-      <c r="B43" s="111"/>
-      <c r="C43" s="121"/>
+      <c r="A43" s="115"/>
+      <c r="B43" s="116"/>
+      <c r="C43" s="113"/>
       <c r="D43" s="9" t="s">
         <v>20</v>
       </c>
@@ -4910,9 +4910,9 @@
       <c r="U43" s="10"/>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A44" s="125"/>
-      <c r="B44" s="111"/>
-      <c r="C44" s="121"/>
+      <c r="A44" s="115"/>
+      <c r="B44" s="116"/>
+      <c r="C44" s="113"/>
       <c r="D44" s="9" t="s">
         <v>24</v>
       </c>
@@ -4953,9 +4953,9 @@
       <c r="U44" s="10"/>
     </row>
     <row r="45" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A45" s="125"/>
-      <c r="B45" s="111"/>
-      <c r="C45" s="121"/>
+      <c r="A45" s="115"/>
+      <c r="B45" s="116"/>
+      <c r="C45" s="113"/>
       <c r="D45" s="49" t="s">
         <v>64</v>
       </c>
@@ -5020,9 +5020,9 @@
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A46" s="125"/>
-      <c r="B46" s="111"/>
-      <c r="C46" s="121"/>
+      <c r="A46" s="115"/>
+      <c r="B46" s="116"/>
+      <c r="C46" s="113"/>
       <c r="D46" s="36" t="s">
         <v>65</v>
       </c>
@@ -5087,11 +5087,11 @@
       </c>
     </row>
     <row r="47" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="125"/>
-      <c r="B47" s="111" t="s">
+      <c r="A47" s="115"/>
+      <c r="B47" s="116" t="s">
         <v>71</v>
       </c>
-      <c r="C47" s="121" t="s">
+      <c r="C47" s="113" t="s">
         <v>15</v>
       </c>
       <c r="D47" s="10"/>
@@ -5114,9 +5114,9 @@
       <c r="U47" s="10"/>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A48" s="125"/>
-      <c r="B48" s="111"/>
-      <c r="C48" s="121"/>
+      <c r="A48" s="115"/>
+      <c r="B48" s="116"/>
+      <c r="C48" s="113"/>
       <c r="D48" s="9" t="s">
         <v>25</v>
       </c>
@@ -5142,9 +5142,9 @@
       <c r="U48" s="10"/>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A49" s="125"/>
-      <c r="B49" s="111"/>
-      <c r="C49" s="121"/>
+      <c r="A49" s="115"/>
+      <c r="B49" s="116"/>
+      <c r="C49" s="113"/>
       <c r="D49" s="9" t="s">
         <v>14</v>
       </c>
@@ -5170,9 +5170,9 @@
       <c r="U49" s="10"/>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A50" s="125"/>
-      <c r="B50" s="111"/>
-      <c r="C50" s="121"/>
+      <c r="A50" s="115"/>
+      <c r="B50" s="116"/>
+      <c r="C50" s="113"/>
       <c r="D50" s="9" t="s">
         <v>36</v>
       </c>
@@ -5198,9 +5198,9 @@
       <c r="U50" s="10"/>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A51" s="125"/>
-      <c r="B51" s="111"/>
-      <c r="C51" s="121"/>
+      <c r="A51" s="115"/>
+      <c r="B51" s="116"/>
+      <c r="C51" s="113"/>
       <c r="D51" s="9" t="s">
         <v>22</v>
       </c>
@@ -5226,9 +5226,9 @@
       <c r="U51" s="10"/>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A52" s="125"/>
-      <c r="B52" s="111"/>
-      <c r="C52" s="121"/>
+      <c r="A52" s="115"/>
+      <c r="B52" s="116"/>
+      <c r="C52" s="113"/>
       <c r="D52" s="48" t="s">
         <v>61</v>
       </c>
@@ -5260,9 +5260,9 @@
       <c r="U52" s="10"/>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A53" s="125"/>
-      <c r="B53" s="111"/>
-      <c r="C53" s="121"/>
+      <c r="A53" s="115"/>
+      <c r="B53" s="116"/>
+      <c r="C53" s="113"/>
       <c r="D53" s="9" t="s">
         <v>21</v>
       </c>
@@ -5288,9 +5288,9 @@
       <c r="U53" s="10"/>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A54" s="125"/>
-      <c r="B54" s="111"/>
-      <c r="C54" s="121"/>
+      <c r="A54" s="115"/>
+      <c r="B54" s="116"/>
+      <c r="C54" s="113"/>
       <c r="D54" s="48" t="s">
         <v>62</v>
       </c>
@@ -5322,9 +5322,9 @@
       <c r="U54" s="10"/>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A55" s="125"/>
-      <c r="B55" s="111"/>
-      <c r="C55" s="121"/>
+      <c r="A55" s="115"/>
+      <c r="B55" s="116"/>
+      <c r="C55" s="113"/>
       <c r="D55" s="9" t="s">
         <v>23</v>
       </c>
@@ -5350,9 +5350,9 @@
       <c r="U55" s="10"/>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A56" s="125"/>
-      <c r="B56" s="111"/>
-      <c r="C56" s="121"/>
+      <c r="A56" s="115"/>
+      <c r="B56" s="116"/>
+      <c r="C56" s="113"/>
       <c r="D56" s="48" t="s">
         <v>63</v>
       </c>
@@ -5384,9 +5384,9 @@
       <c r="U56" s="10"/>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A57" s="125"/>
-      <c r="B57" s="111"/>
-      <c r="C57" s="121"/>
+      <c r="A57" s="115"/>
+      <c r="B57" s="116"/>
+      <c r="C57" s="113"/>
       <c r="D57" s="9" t="s">
         <v>20</v>
       </c>
@@ -5412,9 +5412,9 @@
       <c r="U57" s="10"/>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A58" s="125"/>
-      <c r="B58" s="111"/>
-      <c r="C58" s="121"/>
+      <c r="A58" s="115"/>
+      <c r="B58" s="116"/>
+      <c r="C58" s="113"/>
       <c r="D58" s="9" t="s">
         <v>24</v>
       </c>
@@ -5440,9 +5440,9 @@
       <c r="U58" s="10"/>
     </row>
     <row r="59" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A59" s="125"/>
-      <c r="B59" s="111"/>
-      <c r="C59" s="121"/>
+      <c r="A59" s="115"/>
+      <c r="B59" s="116"/>
+      <c r="C59" s="113"/>
       <c r="D59" s="49" t="s">
         <v>64</v>
       </c>
@@ -5507,9 +5507,9 @@
       </c>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A60" s="125"/>
-      <c r="B60" s="111"/>
-      <c r="C60" s="121"/>
+      <c r="A60" s="115"/>
+      <c r="B60" s="116"/>
+      <c r="C60" s="113"/>
       <c r="D60" s="36" t="s">
         <v>66</v>
       </c>
@@ -5574,13 +5574,13 @@
       </c>
     </row>
     <row r="61" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="124" t="s">
+      <c r="A61" s="114" t="s">
         <v>69</v>
       </c>
-      <c r="B61" s="111" t="s">
+      <c r="B61" s="116" t="s">
         <v>72</v>
       </c>
-      <c r="C61" s="122" t="s">
+      <c r="C61" s="111" t="s">
         <v>73</v>
       </c>
       <c r="D61" s="10"/>
@@ -5603,9 +5603,9 @@
       <c r="U61" s="10"/>
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A62" s="125"/>
-      <c r="B62" s="111"/>
-      <c r="C62" s="123"/>
+      <c r="A62" s="115"/>
+      <c r="B62" s="116"/>
+      <c r="C62" s="112"/>
       <c r="D62" s="9" t="s">
         <v>25</v>
       </c>
@@ -5646,9 +5646,9 @@
       <c r="U62" s="10"/>
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A63" s="125"/>
-      <c r="B63" s="111"/>
-      <c r="C63" s="123"/>
+      <c r="A63" s="115"/>
+      <c r="B63" s="116"/>
+      <c r="C63" s="112"/>
       <c r="D63" s="9" t="s">
         <v>14</v>
       </c>
@@ -5689,9 +5689,9 @@
       <c r="U63" s="10"/>
     </row>
     <row r="64" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A64" s="125"/>
-      <c r="B64" s="111"/>
-      <c r="C64" s="123"/>
+      <c r="A64" s="115"/>
+      <c r="B64" s="116"/>
+      <c r="C64" s="112"/>
       <c r="D64" s="9" t="s">
         <v>36</v>
       </c>
@@ -5732,9 +5732,9 @@
       <c r="U64" s="10"/>
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A65" s="125"/>
-      <c r="B65" s="111"/>
-      <c r="C65" s="123"/>
+      <c r="A65" s="115"/>
+      <c r="B65" s="116"/>
+      <c r="C65" s="112"/>
       <c r="D65" s="9" t="s">
         <v>22</v>
       </c>
@@ -5775,9 +5775,9 @@
       <c r="U65" s="10"/>
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A66" s="125"/>
-      <c r="B66" s="111"/>
-      <c r="C66" s="123"/>
+      <c r="A66" s="115"/>
+      <c r="B66" s="116"/>
+      <c r="C66" s="112"/>
       <c r="D66" s="48" t="s">
         <v>61</v>
       </c>
@@ -5830,9 +5830,9 @@
       <c r="U66" s="10"/>
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A67" s="125"/>
-      <c r="B67" s="111"/>
-      <c r="C67" s="123"/>
+      <c r="A67" s="115"/>
+      <c r="B67" s="116"/>
+      <c r="C67" s="112"/>
       <c r="D67" s="9" t="s">
         <v>21</v>
       </c>
@@ -5873,9 +5873,9 @@
       <c r="U67" s="10"/>
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A68" s="125"/>
-      <c r="B68" s="111"/>
-      <c r="C68" s="123"/>
+      <c r="A68" s="115"/>
+      <c r="B68" s="116"/>
+      <c r="C68" s="112"/>
       <c r="D68" s="48" t="s">
         <v>62</v>
       </c>
@@ -5928,9 +5928,9 @@
       <c r="U68" s="10"/>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A69" s="125"/>
-      <c r="B69" s="111"/>
-      <c r="C69" s="123"/>
+      <c r="A69" s="115"/>
+      <c r="B69" s="116"/>
+      <c r="C69" s="112"/>
       <c r="D69" s="9" t="s">
         <v>23</v>
       </c>
@@ -5971,9 +5971,9 @@
       <c r="U69" s="10"/>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A70" s="125"/>
-      <c r="B70" s="111"/>
-      <c r="C70" s="123"/>
+      <c r="A70" s="115"/>
+      <c r="B70" s="116"/>
+      <c r="C70" s="112"/>
       <c r="D70" s="48" t="s">
         <v>63</v>
       </c>
@@ -6038,9 +6038,9 @@
       </c>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A71" s="125"/>
-      <c r="B71" s="111"/>
-      <c r="C71" s="123"/>
+      <c r="A71" s="115"/>
+      <c r="B71" s="116"/>
+      <c r="C71" s="112"/>
       <c r="D71" s="9" t="s">
         <v>20</v>
       </c>
@@ -6081,9 +6081,9 @@
       <c r="U71" s="10"/>
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A72" s="125"/>
-      <c r="B72" s="111"/>
-      <c r="C72" s="123"/>
+      <c r="A72" s="115"/>
+      <c r="B72" s="116"/>
+      <c r="C72" s="112"/>
       <c r="D72" s="9" t="s">
         <v>24</v>
       </c>
@@ -6109,9 +6109,9 @@
       </c>
     </row>
     <row r="73" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A73" s="125"/>
-      <c r="B73" s="111"/>
-      <c r="C73" s="123"/>
+      <c r="A73" s="115"/>
+      <c r="B73" s="116"/>
+      <c r="C73" s="112"/>
       <c r="D73" s="49" t="s">
         <v>64</v>
       </c>
@@ -6176,9 +6176,9 @@
       </c>
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A74" s="125"/>
-      <c r="B74" s="111"/>
-      <c r="C74" s="121" t="s">
+      <c r="A74" s="115"/>
+      <c r="B74" s="116"/>
+      <c r="C74" s="113" t="s">
         <v>74</v>
       </c>
       <c r="D74" s="10"/>
@@ -6201,9 +6201,9 @@
       <c r="U74" s="10"/>
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A75" s="125"/>
-      <c r="B75" s="111"/>
-      <c r="C75" s="121"/>
+      <c r="A75" s="115"/>
+      <c r="B75" s="116"/>
+      <c r="C75" s="113"/>
       <c r="D75" s="9" t="s">
         <v>25</v>
       </c>
@@ -6238,9 +6238,9 @@
       <c r="U75" s="10"/>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A76" s="125"/>
-      <c r="B76" s="111"/>
-      <c r="C76" s="121"/>
+      <c r="A76" s="115"/>
+      <c r="B76" s="116"/>
+      <c r="C76" s="113"/>
       <c r="D76" s="9" t="s">
         <v>14</v>
       </c>
@@ -6275,9 +6275,9 @@
       <c r="U76" s="10"/>
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A77" s="125"/>
-      <c r="B77" s="111"/>
-      <c r="C77" s="121"/>
+      <c r="A77" s="115"/>
+      <c r="B77" s="116"/>
+      <c r="C77" s="113"/>
       <c r="D77" s="9" t="s">
         <v>36</v>
       </c>
@@ -6312,9 +6312,9 @@
       <c r="U77" s="10"/>
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A78" s="125"/>
-      <c r="B78" s="111"/>
-      <c r="C78" s="121"/>
+      <c r="A78" s="115"/>
+      <c r="B78" s="116"/>
+      <c r="C78" s="113"/>
       <c r="D78" s="9" t="s">
         <v>22</v>
       </c>
@@ -6349,9 +6349,9 @@
       <c r="U78" s="10"/>
     </row>
     <row r="79" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A79" s="125"/>
-      <c r="B79" s="111"/>
-      <c r="C79" s="121"/>
+      <c r="A79" s="115"/>
+      <c r="B79" s="116"/>
+      <c r="C79" s="113"/>
       <c r="D79" s="48" t="s">
         <v>61</v>
       </c>
@@ -6404,9 +6404,9 @@
       <c r="U79" s="10"/>
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A80" s="125"/>
-      <c r="B80" s="111"/>
-      <c r="C80" s="121"/>
+      <c r="A80" s="115"/>
+      <c r="B80" s="116"/>
+      <c r="C80" s="113"/>
       <c r="D80" s="9" t="s">
         <v>21</v>
       </c>
@@ -6441,9 +6441,9 @@
       <c r="U80" s="10"/>
     </row>
     <row r="81" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A81" s="125"/>
-      <c r="B81" s="111"/>
-      <c r="C81" s="121"/>
+      <c r="A81" s="115"/>
+      <c r="B81" s="116"/>
+      <c r="C81" s="113"/>
       <c r="D81" s="48" t="s">
         <v>62</v>
       </c>
@@ -6496,9 +6496,9 @@
       <c r="U81" s="10"/>
     </row>
     <row r="82" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A82" s="125"/>
-      <c r="B82" s="111"/>
-      <c r="C82" s="121"/>
+      <c r="A82" s="115"/>
+      <c r="B82" s="116"/>
+      <c r="C82" s="113"/>
       <c r="D82" s="9" t="s">
         <v>23</v>
       </c>
@@ -6533,9 +6533,9 @@
       <c r="U82" s="10"/>
     </row>
     <row r="83" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A83" s="125"/>
-      <c r="B83" s="111"/>
-      <c r="C83" s="121"/>
+      <c r="A83" s="115"/>
+      <c r="B83" s="116"/>
+      <c r="C83" s="113"/>
       <c r="D83" s="48" t="s">
         <v>63</v>
       </c>
@@ -6600,9 +6600,9 @@
       </c>
     </row>
     <row r="84" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A84" s="125"/>
-      <c r="B84" s="111"/>
-      <c r="C84" s="121"/>
+      <c r="A84" s="115"/>
+      <c r="B84" s="116"/>
+      <c r="C84" s="113"/>
       <c r="D84" s="9" t="s">
         <v>20</v>
       </c>
@@ -6637,9 +6637,9 @@
       <c r="U84" s="10"/>
     </row>
     <row r="85" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A85" s="125"/>
-      <c r="B85" s="111"/>
-      <c r="C85" s="121"/>
+      <c r="A85" s="115"/>
+      <c r="B85" s="116"/>
+      <c r="C85" s="113"/>
       <c r="D85" s="9" t="s">
         <v>24</v>
       </c>
@@ -6665,9 +6665,9 @@
       </c>
     </row>
     <row r="86" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A86" s="125"/>
-      <c r="B86" s="111"/>
-      <c r="C86" s="121"/>
+      <c r="A86" s="115"/>
+      <c r="B86" s="116"/>
+      <c r="C86" s="113"/>
       <c r="D86" s="49" t="s">
         <v>64</v>
       </c>
@@ -6732,9 +6732,9 @@
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A87" s="125"/>
-      <c r="B87" s="111"/>
-      <c r="C87" s="121"/>
+      <c r="A87" s="115"/>
+      <c r="B87" s="116"/>
+      <c r="C87" s="113"/>
       <c r="D87" s="36" t="s">
         <v>68</v>
       </c>
@@ -6799,11 +6799,11 @@
       </c>
     </row>
     <row r="88" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="125"/>
-      <c r="B88" s="111" t="s">
+      <c r="A88" s="115"/>
+      <c r="B88" s="116" t="s">
         <v>75</v>
       </c>
-      <c r="C88" s="122" t="s">
+      <c r="C88" s="111" t="s">
         <v>76</v>
       </c>
       <c r="D88" s="10"/>
@@ -6826,9 +6826,9 @@
       <c r="U88" s="10"/>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A89" s="125"/>
-      <c r="B89" s="111"/>
-      <c r="C89" s="123"/>
+      <c r="A89" s="115"/>
+      <c r="B89" s="116"/>
+      <c r="C89" s="112"/>
       <c r="D89" s="9" t="s">
         <v>25</v>
       </c>
@@ -6881,9 +6881,9 @@
       <c r="U89" s="10"/>
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A90" s="125"/>
-      <c r="B90" s="111"/>
-      <c r="C90" s="123"/>
+      <c r="A90" s="115"/>
+      <c r="B90" s="116"/>
+      <c r="C90" s="112"/>
       <c r="D90" s="9" t="s">
         <v>14</v>
       </c>
@@ -6936,9 +6936,9 @@
       <c r="U90" s="10"/>
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A91" s="125"/>
-      <c r="B91" s="111"/>
-      <c r="C91" s="123"/>
+      <c r="A91" s="115"/>
+      <c r="B91" s="116"/>
+      <c r="C91" s="112"/>
       <c r="D91" s="9" t="s">
         <v>36</v>
       </c>
@@ -6987,9 +6987,9 @@
       <c r="S91" s="61"/>
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A92" s="125"/>
-      <c r="B92" s="111"/>
-      <c r="C92" s="123"/>
+      <c r="A92" s="115"/>
+      <c r="B92" s="116"/>
+      <c r="C92" s="112"/>
       <c r="D92" s="9" t="s">
         <v>22</v>
       </c>
@@ -7038,9 +7038,9 @@
       <c r="S92" s="61"/>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A93" s="125"/>
-      <c r="B93" s="111"/>
-      <c r="C93" s="123"/>
+      <c r="A93" s="115"/>
+      <c r="B93" s="116"/>
+      <c r="C93" s="112"/>
       <c r="D93" s="48" t="s">
         <v>61</v>
       </c>
@@ -7089,9 +7089,9 @@
       <c r="S93" s="10"/>
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A94" s="125"/>
-      <c r="B94" s="111"/>
-      <c r="C94" s="123"/>
+      <c r="A94" s="115"/>
+      <c r="B94" s="116"/>
+      <c r="C94" s="112"/>
       <c r="D94" s="9" t="s">
         <v>21</v>
       </c>
@@ -7140,9 +7140,9 @@
       <c r="S94" s="61"/>
     </row>
     <row r="95" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A95" s="125"/>
-      <c r="B95" s="111"/>
-      <c r="C95" s="123"/>
+      <c r="A95" s="115"/>
+      <c r="B95" s="116"/>
+      <c r="C95" s="112"/>
       <c r="D95" s="48" t="s">
         <v>62</v>
       </c>
@@ -7191,9 +7191,9 @@
       <c r="S95" s="10"/>
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A96" s="125"/>
-      <c r="B96" s="111"/>
-      <c r="C96" s="123"/>
+      <c r="A96" s="115"/>
+      <c r="B96" s="116"/>
+      <c r="C96" s="112"/>
       <c r="D96" s="9" t="s">
         <v>23</v>
       </c>
@@ -7242,9 +7242,9 @@
       <c r="S96" s="61"/>
     </row>
     <row r="97" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A97" s="125"/>
-      <c r="B97" s="111"/>
-      <c r="C97" s="123"/>
+      <c r="A97" s="115"/>
+      <c r="B97" s="116"/>
+      <c r="C97" s="112"/>
       <c r="D97" s="48" t="s">
         <v>63</v>
       </c>
@@ -7306,9 +7306,9 @@
       </c>
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A98" s="125"/>
-      <c r="B98" s="111"/>
-      <c r="C98" s="123"/>
+      <c r="A98" s="115"/>
+      <c r="B98" s="116"/>
+      <c r="C98" s="112"/>
       <c r="D98" s="9" t="s">
         <v>20</v>
       </c>
@@ -7357,9 +7357,9 @@
       <c r="S98" s="61"/>
     </row>
     <row r="99" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A99" s="125"/>
-      <c r="B99" s="111"/>
-      <c r="C99" s="123"/>
+      <c r="A99" s="115"/>
+      <c r="B99" s="116"/>
+      <c r="C99" s="112"/>
       <c r="D99" s="9" t="s">
         <v>24</v>
       </c>
@@ -7382,9 +7382,9 @@
       </c>
     </row>
     <row r="100" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A100" s="125"/>
-      <c r="B100" s="111"/>
-      <c r="C100" s="123"/>
+      <c r="A100" s="115"/>
+      <c r="B100" s="116"/>
+      <c r="C100" s="112"/>
       <c r="D100" s="49" t="s">
         <v>64</v>
       </c>
@@ -7449,9 +7449,9 @@
       </c>
     </row>
     <row r="101" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A101" s="125"/>
-      <c r="B101" s="111"/>
-      <c r="C101" s="122" t="s">
+      <c r="A101" s="115"/>
+      <c r="B101" s="116"/>
+      <c r="C101" s="111" t="s">
         <v>77</v>
       </c>
       <c r="I101" s="10"/>
@@ -7463,9 +7463,9 @@
       <c r="U101" s="10"/>
     </row>
     <row r="102" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A102" s="125"/>
-      <c r="B102" s="111"/>
-      <c r="C102" s="123"/>
+      <c r="A102" s="115"/>
+      <c r="B102" s="116"/>
+      <c r="C102" s="112"/>
       <c r="D102" s="9" t="s">
         <v>25</v>
       </c>
@@ -7518,9 +7518,9 @@
       <c r="U102" s="10"/>
     </row>
     <row r="103" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A103" s="125"/>
-      <c r="B103" s="111"/>
-      <c r="C103" s="123"/>
+      <c r="A103" s="115"/>
+      <c r="B103" s="116"/>
+      <c r="C103" s="112"/>
       <c r="D103" s="9" t="s">
         <v>14</v>
       </c>
@@ -7573,9 +7573,9 @@
       <c r="U103" s="10"/>
     </row>
     <row r="104" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A104" s="125"/>
-      <c r="B104" s="111"/>
-      <c r="C104" s="123"/>
+      <c r="A104" s="115"/>
+      <c r="B104" s="116"/>
+      <c r="C104" s="112"/>
       <c r="D104" s="9" t="s">
         <v>36</v>
       </c>
@@ -7624,9 +7624,9 @@
       <c r="S104" s="61"/>
     </row>
     <row r="105" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A105" s="125"/>
-      <c r="B105" s="111"/>
-      <c r="C105" s="123"/>
+      <c r="A105" s="115"/>
+      <c r="B105" s="116"/>
+      <c r="C105" s="112"/>
       <c r="D105" s="9" t="s">
         <v>22</v>
       </c>
@@ -7675,9 +7675,9 @@
       <c r="S105" s="61"/>
     </row>
     <row r="106" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A106" s="125"/>
-      <c r="B106" s="111"/>
-      <c r="C106" s="123"/>
+      <c r="A106" s="115"/>
+      <c r="B106" s="116"/>
+      <c r="C106" s="112"/>
       <c r="D106" s="48" t="s">
         <v>61</v>
       </c>
@@ -7726,9 +7726,9 @@
       <c r="S106" s="10"/>
     </row>
     <row r="107" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A107" s="125"/>
-      <c r="B107" s="111"/>
-      <c r="C107" s="123"/>
+      <c r="A107" s="115"/>
+      <c r="B107" s="116"/>
+      <c r="C107" s="112"/>
       <c r="D107" s="9" t="s">
         <v>21</v>
       </c>
@@ -7777,9 +7777,9 @@
       <c r="S107" s="61"/>
     </row>
     <row r="108" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A108" s="125"/>
-      <c r="B108" s="111"/>
-      <c r="C108" s="123"/>
+      <c r="A108" s="115"/>
+      <c r="B108" s="116"/>
+      <c r="C108" s="112"/>
       <c r="D108" s="48" t="s">
         <v>62</v>
       </c>
@@ -7828,9 +7828,9 @@
       <c r="S108" s="10"/>
     </row>
     <row r="109" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A109" s="125"/>
-      <c r="B109" s="111"/>
-      <c r="C109" s="123"/>
+      <c r="A109" s="115"/>
+      <c r="B109" s="116"/>
+      <c r="C109" s="112"/>
       <c r="D109" s="9" t="s">
         <v>23</v>
       </c>
@@ -7879,9 +7879,9 @@
       <c r="S109" s="61"/>
     </row>
     <row r="110" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A110" s="125"/>
-      <c r="B110" s="111"/>
-      <c r="C110" s="123"/>
+      <c r="A110" s="115"/>
+      <c r="B110" s="116"/>
+      <c r="C110" s="112"/>
       <c r="D110" s="48" t="s">
         <v>63</v>
       </c>
@@ -7943,9 +7943,9 @@
       </c>
     </row>
     <row r="111" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A111" s="125"/>
-      <c r="B111" s="111"/>
-      <c r="C111" s="123"/>
+      <c r="A111" s="115"/>
+      <c r="B111" s="116"/>
+      <c r="C111" s="112"/>
       <c r="D111" s="9" t="s">
         <v>20</v>
       </c>
@@ -7994,9 +7994,9 @@
       <c r="S111" s="61"/>
     </row>
     <row r="112" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A112" s="125"/>
-      <c r="B112" s="111"/>
-      <c r="C112" s="123"/>
+      <c r="A112" s="115"/>
+      <c r="B112" s="116"/>
+      <c r="C112" s="112"/>
       <c r="D112" s="9" t="s">
         <v>24</v>
       </c>
@@ -8019,9 +8019,9 @@
       </c>
     </row>
     <row r="113" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A113" s="125"/>
-      <c r="B113" s="111"/>
-      <c r="C113" s="123"/>
+      <c r="A113" s="115"/>
+      <c r="B113" s="116"/>
+      <c r="C113" s="112"/>
       <c r="D113" s="49" t="s">
         <v>64</v>
       </c>
@@ -8086,11 +8086,11 @@
       </c>
     </row>
     <row r="114" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="124" t="s">
+      <c r="A114" s="114" t="s">
         <v>69</v>
       </c>
-      <c r="B114" s="111"/>
-      <c r="C114" s="122" t="s">
+      <c r="B114" s="116"/>
+      <c r="C114" s="111" t="s">
         <v>78</v>
       </c>
       <c r="I114" s="10"/>
@@ -8102,9 +8102,9 @@
       <c r="U114" s="10"/>
     </row>
     <row r="115" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A115" s="125"/>
-      <c r="B115" s="111"/>
-      <c r="C115" s="123"/>
+      <c r="A115" s="115"/>
+      <c r="B115" s="116"/>
+      <c r="C115" s="112"/>
       <c r="D115" s="9" t="s">
         <v>25</v>
       </c>
@@ -8157,9 +8157,9 @@
       <c r="U115" s="10"/>
     </row>
     <row r="116" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A116" s="125"/>
-      <c r="B116" s="111"/>
-      <c r="C116" s="123"/>
+      <c r="A116" s="115"/>
+      <c r="B116" s="116"/>
+      <c r="C116" s="112"/>
       <c r="D116" s="9" t="s">
         <v>14</v>
       </c>
@@ -8212,9 +8212,9 @@
       <c r="U116" s="10"/>
     </row>
     <row r="117" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A117" s="125"/>
-      <c r="B117" s="111"/>
-      <c r="C117" s="123"/>
+      <c r="A117" s="115"/>
+      <c r="B117" s="116"/>
+      <c r="C117" s="112"/>
       <c r="D117" s="9" t="s">
         <v>36</v>
       </c>
@@ -8263,9 +8263,9 @@
       <c r="S117" s="61"/>
     </row>
     <row r="118" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A118" s="125"/>
-      <c r="B118" s="111"/>
-      <c r="C118" s="123"/>
+      <c r="A118" s="115"/>
+      <c r="B118" s="116"/>
+      <c r="C118" s="112"/>
       <c r="D118" s="9" t="s">
         <v>22</v>
       </c>
@@ -8314,9 +8314,9 @@
       <c r="S118" s="61"/>
     </row>
     <row r="119" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A119" s="125"/>
-      <c r="B119" s="111"/>
-      <c r="C119" s="123"/>
+      <c r="A119" s="115"/>
+      <c r="B119" s="116"/>
+      <c r="C119" s="112"/>
       <c r="D119" s="48" t="s">
         <v>61</v>
       </c>
@@ -8365,9 +8365,9 @@
       <c r="S119" s="10"/>
     </row>
     <row r="120" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A120" s="125"/>
-      <c r="B120" s="111"/>
-      <c r="C120" s="123"/>
+      <c r="A120" s="115"/>
+      <c r="B120" s="116"/>
+      <c r="C120" s="112"/>
       <c r="D120" s="9" t="s">
         <v>21</v>
       </c>
@@ -8416,9 +8416,9 @@
       <c r="S120" s="61"/>
     </row>
     <row r="121" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A121" s="125"/>
-      <c r="B121" s="111"/>
-      <c r="C121" s="123"/>
+      <c r="A121" s="115"/>
+      <c r="B121" s="116"/>
+      <c r="C121" s="112"/>
       <c r="D121" s="48" t="s">
         <v>62</v>
       </c>
@@ -8467,9 +8467,9 @@
       <c r="S121" s="10"/>
     </row>
     <row r="122" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A122" s="125"/>
-      <c r="B122" s="111"/>
-      <c r="C122" s="123"/>
+      <c r="A122" s="115"/>
+      <c r="B122" s="116"/>
+      <c r="C122" s="112"/>
       <c r="D122" s="9" t="s">
         <v>23</v>
       </c>
@@ -8518,9 +8518,9 @@
       <c r="S122" s="61"/>
     </row>
     <row r="123" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A123" s="125"/>
-      <c r="B123" s="111"/>
-      <c r="C123" s="123"/>
+      <c r="A123" s="115"/>
+      <c r="B123" s="116"/>
+      <c r="C123" s="112"/>
       <c r="D123" s="48" t="s">
         <v>63</v>
       </c>
@@ -8582,9 +8582,9 @@
       </c>
     </row>
     <row r="124" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A124" s="125"/>
-      <c r="B124" s="111"/>
-      <c r="C124" s="123"/>
+      <c r="A124" s="115"/>
+      <c r="B124" s="116"/>
+      <c r="C124" s="112"/>
       <c r="D124" s="9" t="s">
         <v>20</v>
       </c>
@@ -8633,9 +8633,9 @@
       <c r="S124" s="61"/>
     </row>
     <row r="125" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A125" s="125"/>
-      <c r="B125" s="111"/>
-      <c r="C125" s="123"/>
+      <c r="A125" s="115"/>
+      <c r="B125" s="116"/>
+      <c r="C125" s="112"/>
       <c r="D125" s="9" t="s">
         <v>24</v>
       </c>
@@ -8658,9 +8658,9 @@
       </c>
     </row>
     <row r="126" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A126" s="125"/>
-      <c r="B126" s="111"/>
-      <c r="C126" s="123"/>
+      <c r="A126" s="115"/>
+      <c r="B126" s="116"/>
+      <c r="C126" s="112"/>
       <c r="D126" s="49" t="s">
         <v>64</v>
       </c>
@@ -8725,9 +8725,9 @@
       </c>
     </row>
     <row r="127" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A127" s="125"/>
-      <c r="B127" s="111"/>
-      <c r="C127" s="122" t="s">
+      <c r="A127" s="115"/>
+      <c r="B127" s="116"/>
+      <c r="C127" s="111" t="s">
         <v>79</v>
       </c>
       <c r="I127" s="10"/>
@@ -8739,9 +8739,9 @@
       <c r="U127" s="10"/>
     </row>
     <row r="128" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A128" s="125"/>
-      <c r="B128" s="111"/>
-      <c r="C128" s="123"/>
+      <c r="A128" s="115"/>
+      <c r="B128" s="116"/>
+      <c r="C128" s="112"/>
       <c r="D128" s="9" t="s">
         <v>25</v>
       </c>
@@ -8794,9 +8794,9 @@
       <c r="U128" s="10"/>
     </row>
     <row r="129" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A129" s="125"/>
-      <c r="B129" s="111"/>
-      <c r="C129" s="123"/>
+      <c r="A129" s="115"/>
+      <c r="B129" s="116"/>
+      <c r="C129" s="112"/>
       <c r="D129" s="9" t="s">
         <v>14</v>
       </c>
@@ -8849,9 +8849,9 @@
       <c r="U129" s="10"/>
     </row>
     <row r="130" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A130" s="125"/>
-      <c r="B130" s="111"/>
-      <c r="C130" s="123"/>
+      <c r="A130" s="115"/>
+      <c r="B130" s="116"/>
+      <c r="C130" s="112"/>
       <c r="D130" s="9" t="s">
         <v>36</v>
       </c>
@@ -8900,9 +8900,9 @@
       <c r="S130" s="61"/>
     </row>
     <row r="131" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A131" s="125"/>
-      <c r="B131" s="111"/>
-      <c r="C131" s="123"/>
+      <c r="A131" s="115"/>
+      <c r="B131" s="116"/>
+      <c r="C131" s="112"/>
       <c r="D131" s="9" t="s">
         <v>22</v>
       </c>
@@ -8951,9 +8951,9 @@
       <c r="S131" s="61"/>
     </row>
     <row r="132" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A132" s="125"/>
-      <c r="B132" s="111"/>
-      <c r="C132" s="123"/>
+      <c r="A132" s="115"/>
+      <c r="B132" s="116"/>
+      <c r="C132" s="112"/>
       <c r="D132" s="48" t="s">
         <v>61</v>
       </c>
@@ -9002,9 +9002,9 @@
       <c r="S132" s="10"/>
     </row>
     <row r="133" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A133" s="125"/>
-      <c r="B133" s="111"/>
-      <c r="C133" s="123"/>
+      <c r="A133" s="115"/>
+      <c r="B133" s="116"/>
+      <c r="C133" s="112"/>
       <c r="D133" s="9" t="s">
         <v>21</v>
       </c>
@@ -9053,9 +9053,9 @@
       <c r="S133" s="61"/>
     </row>
     <row r="134" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A134" s="125"/>
-      <c r="B134" s="111"/>
-      <c r="C134" s="123"/>
+      <c r="A134" s="115"/>
+      <c r="B134" s="116"/>
+      <c r="C134" s="112"/>
       <c r="D134" s="48" t="s">
         <v>62</v>
       </c>
@@ -9104,9 +9104,9 @@
       <c r="S134" s="10"/>
     </row>
     <row r="135" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A135" s="125"/>
-      <c r="B135" s="111"/>
-      <c r="C135" s="123"/>
+      <c r="A135" s="115"/>
+      <c r="B135" s="116"/>
+      <c r="C135" s="112"/>
       <c r="D135" s="9" t="s">
         <v>23</v>
       </c>
@@ -9155,9 +9155,9 @@
       <c r="S135" s="61"/>
     </row>
     <row r="136" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A136" s="125"/>
-      <c r="B136" s="111"/>
-      <c r="C136" s="123"/>
+      <c r="A136" s="115"/>
+      <c r="B136" s="116"/>
+      <c r="C136" s="112"/>
       <c r="D136" s="48" t="s">
         <v>63</v>
       </c>
@@ -9219,9 +9219,9 @@
       </c>
     </row>
     <row r="137" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A137" s="125"/>
-      <c r="B137" s="111"/>
-      <c r="C137" s="123"/>
+      <c r="A137" s="115"/>
+      <c r="B137" s="116"/>
+      <c r="C137" s="112"/>
       <c r="D137" s="9" t="s">
         <v>20</v>
       </c>
@@ -9270,9 +9270,9 @@
       <c r="S137" s="61"/>
     </row>
     <row r="138" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A138" s="125"/>
-      <c r="B138" s="111"/>
-      <c r="C138" s="123"/>
+      <c r="A138" s="115"/>
+      <c r="B138" s="116"/>
+      <c r="C138" s="112"/>
       <c r="D138" s="9" t="s">
         <v>24</v>
       </c>
@@ -9295,9 +9295,9 @@
       </c>
     </row>
     <row r="139" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A139" s="125"/>
-      <c r="B139" s="111"/>
-      <c r="C139" s="123"/>
+      <c r="A139" s="115"/>
+      <c r="B139" s="116"/>
+      <c r="C139" s="112"/>
       <c r="D139" s="49" t="s">
         <v>64</v>
       </c>
@@ -9362,9 +9362,9 @@
       </c>
     </row>
     <row r="140" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A140" s="125"/>
-      <c r="B140" s="111"/>
-      <c r="C140" s="121" t="s">
+      <c r="A140" s="115"/>
+      <c r="B140" s="116"/>
+      <c r="C140" s="113" t="s">
         <v>80</v>
       </c>
       <c r="I140" s="10"/>
@@ -9376,9 +9376,9 @@
       <c r="U140" s="10"/>
     </row>
     <row r="141" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A141" s="125"/>
-      <c r="B141" s="111"/>
-      <c r="C141" s="121"/>
+      <c r="A141" s="115"/>
+      <c r="B141" s="116"/>
+      <c r="C141" s="113"/>
       <c r="D141" s="9" t="s">
         <v>25</v>
       </c>
@@ -9431,9 +9431,9 @@
       <c r="U141" s="10"/>
     </row>
     <row r="142" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A142" s="125"/>
-      <c r="B142" s="111"/>
-      <c r="C142" s="121"/>
+      <c r="A142" s="115"/>
+      <c r="B142" s="116"/>
+      <c r="C142" s="113"/>
       <c r="D142" s="9" t="s">
         <v>14</v>
       </c>
@@ -9486,9 +9486,9 @@
       <c r="U142" s="10"/>
     </row>
     <row r="143" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A143" s="125"/>
-      <c r="B143" s="111"/>
-      <c r="C143" s="121"/>
+      <c r="A143" s="115"/>
+      <c r="B143" s="116"/>
+      <c r="C143" s="113"/>
       <c r="D143" s="9" t="s">
         <v>36</v>
       </c>
@@ -9537,9 +9537,9 @@
       <c r="S143" s="61"/>
     </row>
     <row r="144" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A144" s="125"/>
-      <c r="B144" s="111"/>
-      <c r="C144" s="121"/>
+      <c r="A144" s="115"/>
+      <c r="B144" s="116"/>
+      <c r="C144" s="113"/>
       <c r="D144" s="9" t="s">
         <v>22</v>
       </c>
@@ -9588,9 +9588,9 @@
       <c r="S144" s="61"/>
     </row>
     <row r="145" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A145" s="125"/>
-      <c r="B145" s="111"/>
-      <c r="C145" s="121"/>
+      <c r="A145" s="115"/>
+      <c r="B145" s="116"/>
+      <c r="C145" s="113"/>
       <c r="D145" s="48" t="s">
         <v>61</v>
       </c>
@@ -9639,9 +9639,9 @@
       <c r="S145" s="10"/>
     </row>
     <row r="146" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A146" s="125"/>
-      <c r="B146" s="111"/>
-      <c r="C146" s="121"/>
+      <c r="A146" s="115"/>
+      <c r="B146" s="116"/>
+      <c r="C146" s="113"/>
       <c r="D146" s="9" t="s">
         <v>21</v>
       </c>
@@ -9690,9 +9690,9 @@
       <c r="S146" s="61"/>
     </row>
     <row r="147" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A147" s="125"/>
-      <c r="B147" s="111"/>
-      <c r="C147" s="121"/>
+      <c r="A147" s="115"/>
+      <c r="B147" s="116"/>
+      <c r="C147" s="113"/>
       <c r="D147" s="48" t="s">
         <v>62</v>
       </c>
@@ -9741,9 +9741,9 @@
       <c r="S147" s="10"/>
     </row>
     <row r="148" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A148" s="125"/>
-      <c r="B148" s="111"/>
-      <c r="C148" s="121"/>
+      <c r="A148" s="115"/>
+      <c r="B148" s="116"/>
+      <c r="C148" s="113"/>
       <c r="D148" s="9" t="s">
         <v>23</v>
       </c>
@@ -9792,9 +9792,9 @@
       <c r="S148" s="61"/>
     </row>
     <row r="149" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A149" s="125"/>
-      <c r="B149" s="111"/>
-      <c r="C149" s="121"/>
+      <c r="A149" s="115"/>
+      <c r="B149" s="116"/>
+      <c r="C149" s="113"/>
       <c r="D149" s="48" t="s">
         <v>63</v>
       </c>
@@ -9856,9 +9856,9 @@
       </c>
     </row>
     <row r="150" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A150" s="125"/>
-      <c r="B150" s="111"/>
-      <c r="C150" s="121"/>
+      <c r="A150" s="115"/>
+      <c r="B150" s="116"/>
+      <c r="C150" s="113"/>
       <c r="D150" s="9" t="s">
         <v>20</v>
       </c>
@@ -9907,9 +9907,9 @@
       <c r="S150" s="61"/>
     </row>
     <row r="151" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A151" s="125"/>
-      <c r="B151" s="111"/>
-      <c r="C151" s="121"/>
+      <c r="A151" s="115"/>
+      <c r="B151" s="116"/>
+      <c r="C151" s="113"/>
       <c r="D151" s="9" t="s">
         <v>24</v>
       </c>
@@ -9932,9 +9932,9 @@
       </c>
     </row>
     <row r="152" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A152" s="125"/>
-      <c r="B152" s="111"/>
-      <c r="C152" s="121"/>
+      <c r="A152" s="115"/>
+      <c r="B152" s="116"/>
+      <c r="C152" s="113"/>
       <c r="D152" s="49" t="s">
         <v>64</v>
       </c>
@@ -9999,9 +9999,9 @@
       </c>
     </row>
     <row r="153" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A153" s="125"/>
-      <c r="B153" s="111"/>
-      <c r="C153" s="121"/>
+      <c r="A153" s="115"/>
+      <c r="B153" s="116"/>
+      <c r="C153" s="113"/>
       <c r="D153" s="52" t="s">
         <v>67</v>
       </c>
@@ -10103,6 +10103,17 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A22:A31"/>
+    <mergeCell ref="A8:C11"/>
+    <mergeCell ref="B13:C15"/>
+    <mergeCell ref="B22:B27"/>
+    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="B16:C19"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C30:C31"/>
     <mergeCell ref="C127:C139"/>
     <mergeCell ref="C140:C153"/>
     <mergeCell ref="A34:A60"/>
@@ -10119,17 +10130,6 @@
     <mergeCell ref="C34:C46"/>
     <mergeCell ref="B47:B60"/>
     <mergeCell ref="C47:C60"/>
-    <mergeCell ref="A22:A31"/>
-    <mergeCell ref="A8:C11"/>
-    <mergeCell ref="B13:C15"/>
-    <mergeCell ref="B22:B27"/>
-    <mergeCell ref="A13:A19"/>
-    <mergeCell ref="B16:C19"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C30:C31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="58" fitToHeight="5" orientation="landscape" r:id="rId1"/>
@@ -10145,8 +10145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView topLeftCell="A112" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K104" sqref="K104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13916,7 +13916,7 @@
         <v>4</v>
       </c>
       <c r="K103" s="95">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="L103" s="95">
         <v>0</v>
@@ -14564,7 +14564,7 @@
         <v>2</v>
       </c>
       <c r="K133" s="95">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="L133" s="95">
         <v>2</v>

</xml_diff>

<commit_message>
added test case for 2 layer at level 1 issue
</commit_message>
<xml_diff>
--- a/ftest/data/fm24/Worked_Example_Calculation_Net_Loss_Pre_Cat_Simple_Complex_Test_Case_working.xlsx
+++ b/ftest/data/fm24/Worked_Example_Calculation_Net_Loss_Pre_Cat_Simple_Complex_Test_Case_working.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\git\ktest\ftest\data\fm24\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{517EFDF6-F67A-4F6C-A1B5-3A43AB482AD9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="-12" windowWidth="18972" windowHeight="5916" activeTab="2"/>
+    <workbookView xWindow="-12" yWindow="-12" windowWidth="18972" windowHeight="5916" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="9" r:id="rId1"/>
@@ -463,7 +464,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0000%"/>
@@ -1087,21 +1088,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1130,6 +1116,21 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1477,7 +1478,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1628,7 +1629,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V33"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -2922,14 +2923,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U166"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <pane xSplit="4" ySplit="7" topLeftCell="E53" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
+      <pane xSplit="4" ySplit="7" topLeftCell="E62" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="O4" sqref="O4"/>
+      <selection pane="bottomRight" activeCell="J89" sqref="J89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3085,11 +3086,11 @@
       <c r="U7" s="10"/>
     </row>
     <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="117" t="s">
+      <c r="A8" s="112" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="118"/>
-      <c r="C8" s="119"/>
+      <c r="B8" s="113"/>
+      <c r="C8" s="114"/>
       <c r="D8" s="33" t="s">
         <v>38</v>
       </c>
@@ -3154,9 +3155,9 @@
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A9" s="120"/>
-      <c r="B9" s="121"/>
-      <c r="C9" s="122"/>
+      <c r="A9" s="115"/>
+      <c r="B9" s="116"/>
+      <c r="C9" s="117"/>
       <c r="D9" s="33" t="s">
         <v>39</v>
       </c>
@@ -3221,9 +3222,9 @@
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A10" s="120"/>
-      <c r="B10" s="121"/>
-      <c r="C10" s="122"/>
+      <c r="A10" s="115"/>
+      <c r="B10" s="116"/>
+      <c r="C10" s="117"/>
       <c r="D10" s="33" t="s">
         <v>40</v>
       </c>
@@ -3288,9 +3289,9 @@
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A11" s="123"/>
-      <c r="B11" s="124"/>
-      <c r="C11" s="125"/>
+      <c r="A11" s="118"/>
+      <c r="B11" s="119"/>
+      <c r="C11" s="120"/>
       <c r="D11" s="9" t="s">
         <v>37</v>
       </c>
@@ -3375,13 +3376,13 @@
       <c r="U12" s="10"/>
     </row>
     <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="116" t="s">
+      <c r="A13" s="111" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="116" t="s">
+      <c r="B13" s="111" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="116"/>
+      <c r="C13" s="111"/>
       <c r="D13" s="34" t="s">
         <v>49</v>
       </c>
@@ -3424,9 +3425,9 @@
       </c>
     </row>
     <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="116"/>
-      <c r="B14" s="116"/>
-      <c r="C14" s="116"/>
+      <c r="A14" s="111"/>
+      <c r="B14" s="111"/>
+      <c r="C14" s="111"/>
       <c r="D14" s="34" t="s">
         <v>50</v>
       </c>
@@ -3479,9 +3480,9 @@
       <c r="U14" s="40"/>
     </row>
     <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="116"/>
-      <c r="B15" s="116"/>
-      <c r="C15" s="116"/>
+      <c r="A15" s="111"/>
+      <c r="B15" s="111"/>
+      <c r="C15" s="111"/>
       <c r="D15" s="34" t="s">
         <v>51</v>
       </c>
@@ -3534,11 +3535,11 @@
       <c r="U15" s="40"/>
     </row>
     <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="116"/>
-      <c r="B16" s="117" t="s">
+      <c r="A16" s="111"/>
+      <c r="B16" s="112" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="119"/>
+      <c r="C16" s="114"/>
       <c r="D16" s="33" t="s">
         <v>38</v>
       </c>
@@ -3603,9 +3604,9 @@
       </c>
     </row>
     <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="116"/>
-      <c r="B17" s="120"/>
-      <c r="C17" s="122"/>
+      <c r="A17" s="111"/>
+      <c r="B17" s="115"/>
+      <c r="C17" s="117"/>
       <c r="D17" s="33" t="s">
         <v>39</v>
       </c>
@@ -3670,9 +3671,9 @@
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A18" s="116"/>
-      <c r="B18" s="120"/>
-      <c r="C18" s="122"/>
+      <c r="A18" s="111"/>
+      <c r="B18" s="115"/>
+      <c r="C18" s="117"/>
       <c r="D18" s="33" t="s">
         <v>40</v>
       </c>
@@ -3737,9 +3738,9 @@
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A19" s="116"/>
-      <c r="B19" s="123"/>
-      <c r="C19" s="125"/>
+      <c r="A19" s="111"/>
+      <c r="B19" s="118"/>
+      <c r="C19" s="120"/>
       <c r="D19" s="35" t="s">
         <v>47</v>
       </c>
@@ -3844,13 +3845,13 @@
       <c r="U21" s="10"/>
     </row>
     <row r="22" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="116" t="s">
+      <c r="A22" s="111" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="116" t="s">
+      <c r="B22" s="111" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="113" t="s">
+      <c r="C22" s="121" t="s">
         <v>56</v>
       </c>
       <c r="D22" s="9" t="s">
@@ -3905,9 +3906,9 @@
       <c r="U22" s="10"/>
     </row>
     <row r="23" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="116"/>
-      <c r="B23" s="116"/>
-      <c r="C23" s="113"/>
+      <c r="A23" s="111"/>
+      <c r="B23" s="111"/>
+      <c r="C23" s="121"/>
       <c r="D23" s="9" t="s">
         <v>32</v>
       </c>
@@ -3960,9 +3961,9 @@
       <c r="U23" s="10"/>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A24" s="116"/>
-      <c r="B24" s="116"/>
-      <c r="C24" s="113"/>
+      <c r="A24" s="111"/>
+      <c r="B24" s="111"/>
+      <c r="C24" s="121"/>
       <c r="D24" s="9" t="s">
         <v>30</v>
       </c>
@@ -4015,9 +4016,9 @@
       <c r="U24" s="10"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A25" s="116"/>
-      <c r="B25" s="116"/>
-      <c r="C25" s="113"/>
+      <c r="A25" s="111"/>
+      <c r="B25" s="111"/>
+      <c r="C25" s="121"/>
       <c r="D25" s="36" t="s">
         <v>53</v>
       </c>
@@ -4070,9 +4071,9 @@
       <c r="U25" s="10"/>
     </row>
     <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="116"/>
-      <c r="B26" s="116"/>
-      <c r="C26" s="113" t="s">
+      <c r="A26" s="111"/>
+      <c r="B26" s="111"/>
+      <c r="C26" s="121" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="9" t="s">
@@ -4127,9 +4128,9 @@
       <c r="U26" s="10"/>
     </row>
     <row r="27" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="116"/>
-      <c r="B27" s="116"/>
-      <c r="C27" s="113"/>
+      <c r="A27" s="111"/>
+      <c r="B27" s="111"/>
+      <c r="C27" s="121"/>
       <c r="D27" s="36" t="s">
         <v>58</v>
       </c>
@@ -4191,11 +4192,11 @@
       <c r="U27" s="42"/>
     </row>
     <row r="28" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="116"/>
-      <c r="B28" s="116" t="s">
+      <c r="A28" s="111"/>
+      <c r="B28" s="111" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="113" t="s">
+      <c r="C28" s="121" t="s">
         <v>21</v>
       </c>
       <c r="D28" s="9" t="s">
@@ -4229,9 +4230,9 @@
       <c r="U28" s="10"/>
     </row>
     <row r="29" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="116"/>
-      <c r="B29" s="116"/>
-      <c r="C29" s="113"/>
+      <c r="A29" s="111"/>
+      <c r="B29" s="111"/>
+      <c r="C29" s="121"/>
       <c r="D29" s="36" t="s">
         <v>59</v>
       </c>
@@ -4293,9 +4294,9 @@
       <c r="U29" s="10"/>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A30" s="116"/>
-      <c r="B30" s="116"/>
-      <c r="C30" s="113" t="s">
+      <c r="A30" s="111"/>
+      <c r="B30" s="111"/>
+      <c r="C30" s="121" t="s">
         <v>57</v>
       </c>
       <c r="D30" s="9" t="s">
@@ -4329,9 +4330,9 @@
       <c r="U30" s="10"/>
     </row>
     <row r="31" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="116"/>
-      <c r="B31" s="116"/>
-      <c r="C31" s="113"/>
+      <c r="A31" s="111"/>
+      <c r="B31" s="111"/>
+      <c r="C31" s="121"/>
       <c r="D31" s="35" t="s">
         <v>60</v>
       </c>
@@ -4438,13 +4439,13 @@
       <c r="U33" s="10"/>
     </row>
     <row r="34" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="114" t="s">
+      <c r="A34" s="124" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="116" t="s">
+      <c r="B34" s="111" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="113" t="s">
+      <c r="C34" s="121" t="s">
         <v>16</v>
       </c>
       <c r="D34" s="9" t="s">
@@ -4487,9 +4488,9 @@
       <c r="U34" s="10"/>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A35" s="115"/>
-      <c r="B35" s="116"/>
-      <c r="C35" s="113"/>
+      <c r="A35" s="125"/>
+      <c r="B35" s="111"/>
+      <c r="C35" s="121"/>
       <c r="D35" s="9" t="s">
         <v>14</v>
       </c>
@@ -4530,9 +4531,9 @@
       <c r="U35" s="10"/>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A36" s="115"/>
-      <c r="B36" s="116"/>
-      <c r="C36" s="113"/>
+      <c r="A36" s="125"/>
+      <c r="B36" s="111"/>
+      <c r="C36" s="121"/>
       <c r="D36" s="9" t="s">
         <v>36</v>
       </c>
@@ -4573,9 +4574,9 @@
       <c r="U36" s="10"/>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A37" s="115"/>
-      <c r="B37" s="116"/>
-      <c r="C37" s="113"/>
+      <c r="A37" s="125"/>
+      <c r="B37" s="111"/>
+      <c r="C37" s="121"/>
       <c r="D37" s="9" t="s">
         <v>22</v>
       </c>
@@ -4616,9 +4617,9 @@
       <c r="U37" s="10"/>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A38" s="115"/>
-      <c r="B38" s="116"/>
-      <c r="C38" s="113"/>
+      <c r="A38" s="125"/>
+      <c r="B38" s="111"/>
+      <c r="C38" s="121"/>
       <c r="D38" s="48" t="s">
         <v>61</v>
       </c>
@@ -4671,9 +4672,9 @@
       <c r="U38" s="10"/>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A39" s="115"/>
-      <c r="B39" s="116"/>
-      <c r="C39" s="113"/>
+      <c r="A39" s="125"/>
+      <c r="B39" s="111"/>
+      <c r="C39" s="121"/>
       <c r="D39" s="9" t="s">
         <v>21</v>
       </c>
@@ -4714,9 +4715,9 @@
       <c r="U39" s="10"/>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A40" s="115"/>
-      <c r="B40" s="116"/>
-      <c r="C40" s="113"/>
+      <c r="A40" s="125"/>
+      <c r="B40" s="111"/>
+      <c r="C40" s="121"/>
       <c r="D40" s="48" t="s">
         <v>62</v>
       </c>
@@ -4769,9 +4770,9 @@
       <c r="U40" s="10"/>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A41" s="115"/>
-      <c r="B41" s="116"/>
-      <c r="C41" s="113"/>
+      <c r="A41" s="125"/>
+      <c r="B41" s="111"/>
+      <c r="C41" s="121"/>
       <c r="D41" s="9" t="s">
         <v>23</v>
       </c>
@@ -4812,9 +4813,9 @@
       <c r="U41" s="10"/>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A42" s="115"/>
-      <c r="B42" s="116"/>
-      <c r="C42" s="113"/>
+      <c r="A42" s="125"/>
+      <c r="B42" s="111"/>
+      <c r="C42" s="121"/>
       <c r="D42" s="48" t="s">
         <v>63</v>
       </c>
@@ -4867,9 +4868,9 @@
       <c r="U42" s="10"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A43" s="115"/>
-      <c r="B43" s="116"/>
-      <c r="C43" s="113"/>
+      <c r="A43" s="125"/>
+      <c r="B43" s="111"/>
+      <c r="C43" s="121"/>
       <c r="D43" s="9" t="s">
         <v>20</v>
       </c>
@@ -4910,9 +4911,9 @@
       <c r="U43" s="10"/>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A44" s="115"/>
-      <c r="B44" s="116"/>
-      <c r="C44" s="113"/>
+      <c r="A44" s="125"/>
+      <c r="B44" s="111"/>
+      <c r="C44" s="121"/>
       <c r="D44" s="9" t="s">
         <v>24</v>
       </c>
@@ -4953,9 +4954,9 @@
       <c r="U44" s="10"/>
     </row>
     <row r="45" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A45" s="115"/>
-      <c r="B45" s="116"/>
-      <c r="C45" s="113"/>
+      <c r="A45" s="125"/>
+      <c r="B45" s="111"/>
+      <c r="C45" s="121"/>
       <c r="D45" s="49" t="s">
         <v>64</v>
       </c>
@@ -5020,9 +5021,9 @@
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A46" s="115"/>
-      <c r="B46" s="116"/>
-      <c r="C46" s="113"/>
+      <c r="A46" s="125"/>
+      <c r="B46" s="111"/>
+      <c r="C46" s="121"/>
       <c r="D46" s="36" t="s">
         <v>65</v>
       </c>
@@ -5087,11 +5088,11 @@
       </c>
     </row>
     <row r="47" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="115"/>
-      <c r="B47" s="116" t="s">
+      <c r="A47" s="125"/>
+      <c r="B47" s="111" t="s">
         <v>71</v>
       </c>
-      <c r="C47" s="113" t="s">
+      <c r="C47" s="121" t="s">
         <v>15</v>
       </c>
       <c r="D47" s="10"/>
@@ -5114,9 +5115,9 @@
       <c r="U47" s="10"/>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A48" s="115"/>
-      <c r="B48" s="116"/>
-      <c r="C48" s="113"/>
+      <c r="A48" s="125"/>
+      <c r="B48" s="111"/>
+      <c r="C48" s="121"/>
       <c r="D48" s="9" t="s">
         <v>25</v>
       </c>
@@ -5142,9 +5143,9 @@
       <c r="U48" s="10"/>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A49" s="115"/>
-      <c r="B49" s="116"/>
-      <c r="C49" s="113"/>
+      <c r="A49" s="125"/>
+      <c r="B49" s="111"/>
+      <c r="C49" s="121"/>
       <c r="D49" s="9" t="s">
         <v>14</v>
       </c>
@@ -5170,9 +5171,9 @@
       <c r="U49" s="10"/>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A50" s="115"/>
-      <c r="B50" s="116"/>
-      <c r="C50" s="113"/>
+      <c r="A50" s="125"/>
+      <c r="B50" s="111"/>
+      <c r="C50" s="121"/>
       <c r="D50" s="9" t="s">
         <v>36</v>
       </c>
@@ -5198,9 +5199,9 @@
       <c r="U50" s="10"/>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A51" s="115"/>
-      <c r="B51" s="116"/>
-      <c r="C51" s="113"/>
+      <c r="A51" s="125"/>
+      <c r="B51" s="111"/>
+      <c r="C51" s="121"/>
       <c r="D51" s="9" t="s">
         <v>22</v>
       </c>
@@ -5226,9 +5227,9 @@
       <c r="U51" s="10"/>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A52" s="115"/>
-      <c r="B52" s="116"/>
-      <c r="C52" s="113"/>
+      <c r="A52" s="125"/>
+      <c r="B52" s="111"/>
+      <c r="C52" s="121"/>
       <c r="D52" s="48" t="s">
         <v>61</v>
       </c>
@@ -5260,9 +5261,9 @@
       <c r="U52" s="10"/>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A53" s="115"/>
-      <c r="B53" s="116"/>
-      <c r="C53" s="113"/>
+      <c r="A53" s="125"/>
+      <c r="B53" s="111"/>
+      <c r="C53" s="121"/>
       <c r="D53" s="9" t="s">
         <v>21</v>
       </c>
@@ -5288,9 +5289,9 @@
       <c r="U53" s="10"/>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A54" s="115"/>
-      <c r="B54" s="116"/>
-      <c r="C54" s="113"/>
+      <c r="A54" s="125"/>
+      <c r="B54" s="111"/>
+      <c r="C54" s="121"/>
       <c r="D54" s="48" t="s">
         <v>62</v>
       </c>
@@ -5322,9 +5323,9 @@
       <c r="U54" s="10"/>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A55" s="115"/>
-      <c r="B55" s="116"/>
-      <c r="C55" s="113"/>
+      <c r="A55" s="125"/>
+      <c r="B55" s="111"/>
+      <c r="C55" s="121"/>
       <c r="D55" s="9" t="s">
         <v>23</v>
       </c>
@@ -5350,9 +5351,9 @@
       <c r="U55" s="10"/>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A56" s="115"/>
-      <c r="B56" s="116"/>
-      <c r="C56" s="113"/>
+      <c r="A56" s="125"/>
+      <c r="B56" s="111"/>
+      <c r="C56" s="121"/>
       <c r="D56" s="48" t="s">
         <v>63</v>
       </c>
@@ -5384,9 +5385,9 @@
       <c r="U56" s="10"/>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A57" s="115"/>
-      <c r="B57" s="116"/>
-      <c r="C57" s="113"/>
+      <c r="A57" s="125"/>
+      <c r="B57" s="111"/>
+      <c r="C57" s="121"/>
       <c r="D57" s="9" t="s">
         <v>20</v>
       </c>
@@ -5412,9 +5413,9 @@
       <c r="U57" s="10"/>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A58" s="115"/>
-      <c r="B58" s="116"/>
-      <c r="C58" s="113"/>
+      <c r="A58" s="125"/>
+      <c r="B58" s="111"/>
+      <c r="C58" s="121"/>
       <c r="D58" s="9" t="s">
         <v>24</v>
       </c>
@@ -5440,9 +5441,9 @@
       <c r="U58" s="10"/>
     </row>
     <row r="59" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A59" s="115"/>
-      <c r="B59" s="116"/>
-      <c r="C59" s="113"/>
+      <c r="A59" s="125"/>
+      <c r="B59" s="111"/>
+      <c r="C59" s="121"/>
       <c r="D59" s="49" t="s">
         <v>64</v>
       </c>
@@ -5507,9 +5508,9 @@
       </c>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A60" s="115"/>
-      <c r="B60" s="116"/>
-      <c r="C60" s="113"/>
+      <c r="A60" s="125"/>
+      <c r="B60" s="111"/>
+      <c r="C60" s="121"/>
       <c r="D60" s="36" t="s">
         <v>66</v>
       </c>
@@ -5574,13 +5575,13 @@
       </c>
     </row>
     <row r="61" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="114" t="s">
+      <c r="A61" s="124" t="s">
         <v>69</v>
       </c>
-      <c r="B61" s="116" t="s">
+      <c r="B61" s="111" t="s">
         <v>72</v>
       </c>
-      <c r="C61" s="111" t="s">
+      <c r="C61" s="122" t="s">
         <v>73</v>
       </c>
       <c r="D61" s="10"/>
@@ -5603,9 +5604,9 @@
       <c r="U61" s="10"/>
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A62" s="115"/>
-      <c r="B62" s="116"/>
-      <c r="C62" s="112"/>
+      <c r="A62" s="125"/>
+      <c r="B62" s="111"/>
+      <c r="C62" s="123"/>
       <c r="D62" s="9" t="s">
         <v>25</v>
       </c>
@@ -5646,9 +5647,9 @@
       <c r="U62" s="10"/>
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A63" s="115"/>
-      <c r="B63" s="116"/>
-      <c r="C63" s="112"/>
+      <c r="A63" s="125"/>
+      <c r="B63" s="111"/>
+      <c r="C63" s="123"/>
       <c r="D63" s="9" t="s">
         <v>14</v>
       </c>
@@ -5689,9 +5690,9 @@
       <c r="U63" s="10"/>
     </row>
     <row r="64" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A64" s="115"/>
-      <c r="B64" s="116"/>
-      <c r="C64" s="112"/>
+      <c r="A64" s="125"/>
+      <c r="B64" s="111"/>
+      <c r="C64" s="123"/>
       <c r="D64" s="9" t="s">
         <v>36</v>
       </c>
@@ -5732,9 +5733,9 @@
       <c r="U64" s="10"/>
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A65" s="115"/>
-      <c r="B65" s="116"/>
-      <c r="C65" s="112"/>
+      <c r="A65" s="125"/>
+      <c r="B65" s="111"/>
+      <c r="C65" s="123"/>
       <c r="D65" s="9" t="s">
         <v>22</v>
       </c>
@@ -5775,9 +5776,9 @@
       <c r="U65" s="10"/>
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A66" s="115"/>
-      <c r="B66" s="116"/>
-      <c r="C66" s="112"/>
+      <c r="A66" s="125"/>
+      <c r="B66" s="111"/>
+      <c r="C66" s="123"/>
       <c r="D66" s="48" t="s">
         <v>61</v>
       </c>
@@ -5830,9 +5831,9 @@
       <c r="U66" s="10"/>
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A67" s="115"/>
-      <c r="B67" s="116"/>
-      <c r="C67" s="112"/>
+      <c r="A67" s="125"/>
+      <c r="B67" s="111"/>
+      <c r="C67" s="123"/>
       <c r="D67" s="9" t="s">
         <v>21</v>
       </c>
@@ -5873,9 +5874,9 @@
       <c r="U67" s="10"/>
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A68" s="115"/>
-      <c r="B68" s="116"/>
-      <c r="C68" s="112"/>
+      <c r="A68" s="125"/>
+      <c r="B68" s="111"/>
+      <c r="C68" s="123"/>
       <c r="D68" s="48" t="s">
         <v>62</v>
       </c>
@@ -5928,9 +5929,9 @@
       <c r="U68" s="10"/>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A69" s="115"/>
-      <c r="B69" s="116"/>
-      <c r="C69" s="112"/>
+      <c r="A69" s="125"/>
+      <c r="B69" s="111"/>
+      <c r="C69" s="123"/>
       <c r="D69" s="9" t="s">
         <v>23</v>
       </c>
@@ -5971,9 +5972,9 @@
       <c r="U69" s="10"/>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A70" s="115"/>
-      <c r="B70" s="116"/>
-      <c r="C70" s="112"/>
+      <c r="A70" s="125"/>
+      <c r="B70" s="111"/>
+      <c r="C70" s="123"/>
       <c r="D70" s="48" t="s">
         <v>63</v>
       </c>
@@ -6038,9 +6039,9 @@
       </c>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A71" s="115"/>
-      <c r="B71" s="116"/>
-      <c r="C71" s="112"/>
+      <c r="A71" s="125"/>
+      <c r="B71" s="111"/>
+      <c r="C71" s="123"/>
       <c r="D71" s="9" t="s">
         <v>20</v>
       </c>
@@ -6081,9 +6082,9 @@
       <c r="U71" s="10"/>
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A72" s="115"/>
-      <c r="B72" s="116"/>
-      <c r="C72" s="112"/>
+      <c r="A72" s="125"/>
+      <c r="B72" s="111"/>
+      <c r="C72" s="123"/>
       <c r="D72" s="9" t="s">
         <v>24</v>
       </c>
@@ -6109,9 +6110,9 @@
       </c>
     </row>
     <row r="73" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A73" s="115"/>
-      <c r="B73" s="116"/>
-      <c r="C73" s="112"/>
+      <c r="A73" s="125"/>
+      <c r="B73" s="111"/>
+      <c r="C73" s="123"/>
       <c r="D73" s="49" t="s">
         <v>64</v>
       </c>
@@ -6176,9 +6177,9 @@
       </c>
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A74" s="115"/>
-      <c r="B74" s="116"/>
-      <c r="C74" s="113" t="s">
+      <c r="A74" s="125"/>
+      <c r="B74" s="111"/>
+      <c r="C74" s="121" t="s">
         <v>74</v>
       </c>
       <c r="D74" s="10"/>
@@ -6194,16 +6195,16 @@
       <c r="N74" s="10"/>
       <c r="O74" s="10"/>
       <c r="P74" s="10"/>
-      <c r="Q74" s="10"/>
+      <c r="Q74" s="39"/>
       <c r="R74" s="10"/>
       <c r="S74" s="10"/>
       <c r="T74" s="10"/>
       <c r="U74" s="10"/>
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A75" s="115"/>
-      <c r="B75" s="116"/>
-      <c r="C75" s="113"/>
+      <c r="A75" s="125"/>
+      <c r="B75" s="111"/>
+      <c r="C75" s="121"/>
       <c r="D75" s="9" t="s">
         <v>25</v>
       </c>
@@ -6238,9 +6239,9 @@
       <c r="U75" s="10"/>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A76" s="115"/>
-      <c r="B76" s="116"/>
-      <c r="C76" s="113"/>
+      <c r="A76" s="125"/>
+      <c r="B76" s="111"/>
+      <c r="C76" s="121"/>
       <c r="D76" s="9" t="s">
         <v>14</v>
       </c>
@@ -6275,9 +6276,9 @@
       <c r="U76" s="10"/>
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A77" s="115"/>
-      <c r="B77" s="116"/>
-      <c r="C77" s="113"/>
+      <c r="A77" s="125"/>
+      <c r="B77" s="111"/>
+      <c r="C77" s="121"/>
       <c r="D77" s="9" t="s">
         <v>36</v>
       </c>
@@ -6312,9 +6313,9 @@
       <c r="U77" s="10"/>
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A78" s="115"/>
-      <c r="B78" s="116"/>
-      <c r="C78" s="113"/>
+      <c r="A78" s="125"/>
+      <c r="B78" s="111"/>
+      <c r="C78" s="121"/>
       <c r="D78" s="9" t="s">
         <v>22</v>
       </c>
@@ -6349,9 +6350,9 @@
       <c r="U78" s="10"/>
     </row>
     <row r="79" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A79" s="115"/>
-      <c r="B79" s="116"/>
-      <c r="C79" s="113"/>
+      <c r="A79" s="125"/>
+      <c r="B79" s="111"/>
+      <c r="C79" s="121"/>
       <c r="D79" s="48" t="s">
         <v>61</v>
       </c>
@@ -6404,9 +6405,9 @@
       <c r="U79" s="10"/>
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A80" s="115"/>
-      <c r="B80" s="116"/>
-      <c r="C80" s="113"/>
+      <c r="A80" s="125"/>
+      <c r="B80" s="111"/>
+      <c r="C80" s="121"/>
       <c r="D80" s="9" t="s">
         <v>21</v>
       </c>
@@ -6441,9 +6442,9 @@
       <c r="U80" s="10"/>
     </row>
     <row r="81" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A81" s="115"/>
-      <c r="B81" s="116"/>
-      <c r="C81" s="113"/>
+      <c r="A81" s="125"/>
+      <c r="B81" s="111"/>
+      <c r="C81" s="121"/>
       <c r="D81" s="48" t="s">
         <v>62</v>
       </c>
@@ -6496,9 +6497,9 @@
       <c r="U81" s="10"/>
     </row>
     <row r="82" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A82" s="115"/>
-      <c r="B82" s="116"/>
-      <c r="C82" s="113"/>
+      <c r="A82" s="125"/>
+      <c r="B82" s="111"/>
+      <c r="C82" s="121"/>
       <c r="D82" s="9" t="s">
         <v>23</v>
       </c>
@@ -6533,9 +6534,9 @@
       <c r="U82" s="10"/>
     </row>
     <row r="83" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A83" s="115"/>
-      <c r="B83" s="116"/>
-      <c r="C83" s="113"/>
+      <c r="A83" s="125"/>
+      <c r="B83" s="111"/>
+      <c r="C83" s="121"/>
       <c r="D83" s="48" t="s">
         <v>63</v>
       </c>
@@ -6600,9 +6601,9 @@
       </c>
     </row>
     <row r="84" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A84" s="115"/>
-      <c r="B84" s="116"/>
-      <c r="C84" s="113"/>
+      <c r="A84" s="125"/>
+      <c r="B84" s="111"/>
+      <c r="C84" s="121"/>
       <c r="D84" s="9" t="s">
         <v>20</v>
       </c>
@@ -6637,9 +6638,9 @@
       <c r="U84" s="10"/>
     </row>
     <row r="85" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A85" s="115"/>
-      <c r="B85" s="116"/>
-      <c r="C85" s="113"/>
+      <c r="A85" s="125"/>
+      <c r="B85" s="111"/>
+      <c r="C85" s="121"/>
       <c r="D85" s="9" t="s">
         <v>24</v>
       </c>
@@ -6665,9 +6666,9 @@
       </c>
     </row>
     <row r="86" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A86" s="115"/>
-      <c r="B86" s="116"/>
-      <c r="C86" s="113"/>
+      <c r="A86" s="125"/>
+      <c r="B86" s="111"/>
+      <c r="C86" s="121"/>
       <c r="D86" s="49" t="s">
         <v>64</v>
       </c>
@@ -6732,9 +6733,9 @@
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A87" s="115"/>
-      <c r="B87" s="116"/>
-      <c r="C87" s="113"/>
+      <c r="A87" s="125"/>
+      <c r="B87" s="111"/>
+      <c r="C87" s="121"/>
       <c r="D87" s="36" t="s">
         <v>68</v>
       </c>
@@ -6799,11 +6800,11 @@
       </c>
     </row>
     <row r="88" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="115"/>
-      <c r="B88" s="116" t="s">
+      <c r="A88" s="125"/>
+      <c r="B88" s="111" t="s">
         <v>75</v>
       </c>
-      <c r="C88" s="111" t="s">
+      <c r="C88" s="122" t="s">
         <v>76</v>
       </c>
       <c r="D88" s="10"/>
@@ -6826,9 +6827,9 @@
       <c r="U88" s="10"/>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A89" s="115"/>
-      <c r="B89" s="116"/>
-      <c r="C89" s="112"/>
+      <c r="A89" s="125"/>
+      <c r="B89" s="111"/>
+      <c r="C89" s="123"/>
       <c r="D89" s="9" t="s">
         <v>25</v>
       </c>
@@ -6881,9 +6882,9 @@
       <c r="U89" s="10"/>
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A90" s="115"/>
-      <c r="B90" s="116"/>
-      <c r="C90" s="112"/>
+      <c r="A90" s="125"/>
+      <c r="B90" s="111"/>
+      <c r="C90" s="123"/>
       <c r="D90" s="9" t="s">
         <v>14</v>
       </c>
@@ -6936,9 +6937,9 @@
       <c r="U90" s="10"/>
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A91" s="115"/>
-      <c r="B91" s="116"/>
-      <c r="C91" s="112"/>
+      <c r="A91" s="125"/>
+      <c r="B91" s="111"/>
+      <c r="C91" s="123"/>
       <c r="D91" s="9" t="s">
         <v>36</v>
       </c>
@@ -6987,9 +6988,9 @@
       <c r="S91" s="61"/>
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A92" s="115"/>
-      <c r="B92" s="116"/>
-      <c r="C92" s="112"/>
+      <c r="A92" s="125"/>
+      <c r="B92" s="111"/>
+      <c r="C92" s="123"/>
       <c r="D92" s="9" t="s">
         <v>22</v>
       </c>
@@ -7038,9 +7039,9 @@
       <c r="S92" s="61"/>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A93" s="115"/>
-      <c r="B93" s="116"/>
-      <c r="C93" s="112"/>
+      <c r="A93" s="125"/>
+      <c r="B93" s="111"/>
+      <c r="C93" s="123"/>
       <c r="D93" s="48" t="s">
         <v>61</v>
       </c>
@@ -7089,9 +7090,9 @@
       <c r="S93" s="10"/>
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A94" s="115"/>
-      <c r="B94" s="116"/>
-      <c r="C94" s="112"/>
+      <c r="A94" s="125"/>
+      <c r="B94" s="111"/>
+      <c r="C94" s="123"/>
       <c r="D94" s="9" t="s">
         <v>21</v>
       </c>
@@ -7140,9 +7141,9 @@
       <c r="S94" s="61"/>
     </row>
     <row r="95" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A95" s="115"/>
-      <c r="B95" s="116"/>
-      <c r="C95" s="112"/>
+      <c r="A95" s="125"/>
+      <c r="B95" s="111"/>
+      <c r="C95" s="123"/>
       <c r="D95" s="48" t="s">
         <v>62</v>
       </c>
@@ -7191,9 +7192,9 @@
       <c r="S95" s="10"/>
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A96" s="115"/>
-      <c r="B96" s="116"/>
-      <c r="C96" s="112"/>
+      <c r="A96" s="125"/>
+      <c r="B96" s="111"/>
+      <c r="C96" s="123"/>
       <c r="D96" s="9" t="s">
         <v>23</v>
       </c>
@@ -7242,9 +7243,9 @@
       <c r="S96" s="61"/>
     </row>
     <row r="97" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A97" s="115"/>
-      <c r="B97" s="116"/>
-      <c r="C97" s="112"/>
+      <c r="A97" s="125"/>
+      <c r="B97" s="111"/>
+      <c r="C97" s="123"/>
       <c r="D97" s="48" t="s">
         <v>63</v>
       </c>
@@ -7306,9 +7307,9 @@
       </c>
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A98" s="115"/>
-      <c r="B98" s="116"/>
-      <c r="C98" s="112"/>
+      <c r="A98" s="125"/>
+      <c r="B98" s="111"/>
+      <c r="C98" s="123"/>
       <c r="D98" s="9" t="s">
         <v>20</v>
       </c>
@@ -7357,9 +7358,9 @@
       <c r="S98" s="61"/>
     </row>
     <row r="99" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A99" s="115"/>
-      <c r="B99" s="116"/>
-      <c r="C99" s="112"/>
+      <c r="A99" s="125"/>
+      <c r="B99" s="111"/>
+      <c r="C99" s="123"/>
       <c r="D99" s="9" t="s">
         <v>24</v>
       </c>
@@ -7382,9 +7383,9 @@
       </c>
     </row>
     <row r="100" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A100" s="115"/>
-      <c r="B100" s="116"/>
-      <c r="C100" s="112"/>
+      <c r="A100" s="125"/>
+      <c r="B100" s="111"/>
+      <c r="C100" s="123"/>
       <c r="D100" s="49" t="s">
         <v>64</v>
       </c>
@@ -7449,9 +7450,9 @@
       </c>
     </row>
     <row r="101" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A101" s="115"/>
-      <c r="B101" s="116"/>
-      <c r="C101" s="111" t="s">
+      <c r="A101" s="125"/>
+      <c r="B101" s="111"/>
+      <c r="C101" s="122" t="s">
         <v>77</v>
       </c>
       <c r="I101" s="10"/>
@@ -7463,9 +7464,9 @@
       <c r="U101" s="10"/>
     </row>
     <row r="102" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A102" s="115"/>
-      <c r="B102" s="116"/>
-      <c r="C102" s="112"/>
+      <c r="A102" s="125"/>
+      <c r="B102" s="111"/>
+      <c r="C102" s="123"/>
       <c r="D102" s="9" t="s">
         <v>25</v>
       </c>
@@ -7518,9 +7519,9 @@
       <c r="U102" s="10"/>
     </row>
     <row r="103" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A103" s="115"/>
-      <c r="B103" s="116"/>
-      <c r="C103" s="112"/>
+      <c r="A103" s="125"/>
+      <c r="B103" s="111"/>
+      <c r="C103" s="123"/>
       <c r="D103" s="9" t="s">
         <v>14</v>
       </c>
@@ -7573,9 +7574,9 @@
       <c r="U103" s="10"/>
     </row>
     <row r="104" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A104" s="115"/>
-      <c r="B104" s="116"/>
-      <c r="C104" s="112"/>
+      <c r="A104" s="125"/>
+      <c r="B104" s="111"/>
+      <c r="C104" s="123"/>
       <c r="D104" s="9" t="s">
         <v>36</v>
       </c>
@@ -7624,9 +7625,9 @@
       <c r="S104" s="61"/>
     </row>
     <row r="105" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A105" s="115"/>
-      <c r="B105" s="116"/>
-      <c r="C105" s="112"/>
+      <c r="A105" s="125"/>
+      <c r="B105" s="111"/>
+      <c r="C105" s="123"/>
       <c r="D105" s="9" t="s">
         <v>22</v>
       </c>
@@ -7675,9 +7676,9 @@
       <c r="S105" s="61"/>
     </row>
     <row r="106" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A106" s="115"/>
-      <c r="B106" s="116"/>
-      <c r="C106" s="112"/>
+      <c r="A106" s="125"/>
+      <c r="B106" s="111"/>
+      <c r="C106" s="123"/>
       <c r="D106" s="48" t="s">
         <v>61</v>
       </c>
@@ -7726,9 +7727,9 @@
       <c r="S106" s="10"/>
     </row>
     <row r="107" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A107" s="115"/>
-      <c r="B107" s="116"/>
-      <c r="C107" s="112"/>
+      <c r="A107" s="125"/>
+      <c r="B107" s="111"/>
+      <c r="C107" s="123"/>
       <c r="D107" s="9" t="s">
         <v>21</v>
       </c>
@@ -7777,9 +7778,9 @@
       <c r="S107" s="61"/>
     </row>
     <row r="108" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A108" s="115"/>
-      <c r="B108" s="116"/>
-      <c r="C108" s="112"/>
+      <c r="A108" s="125"/>
+      <c r="B108" s="111"/>
+      <c r="C108" s="123"/>
       <c r="D108" s="48" t="s">
         <v>62</v>
       </c>
@@ -7828,9 +7829,9 @@
       <c r="S108" s="10"/>
     </row>
     <row r="109" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A109" s="115"/>
-      <c r="B109" s="116"/>
-      <c r="C109" s="112"/>
+      <c r="A109" s="125"/>
+      <c r="B109" s="111"/>
+      <c r="C109" s="123"/>
       <c r="D109" s="9" t="s">
         <v>23</v>
       </c>
@@ -7879,9 +7880,9 @@
       <c r="S109" s="61"/>
     </row>
     <row r="110" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A110" s="115"/>
-      <c r="B110" s="116"/>
-      <c r="C110" s="112"/>
+      <c r="A110" s="125"/>
+      <c r="B110" s="111"/>
+      <c r="C110" s="123"/>
       <c r="D110" s="48" t="s">
         <v>63</v>
       </c>
@@ -7943,9 +7944,9 @@
       </c>
     </row>
     <row r="111" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A111" s="115"/>
-      <c r="B111" s="116"/>
-      <c r="C111" s="112"/>
+      <c r="A111" s="125"/>
+      <c r="B111" s="111"/>
+      <c r="C111" s="123"/>
       <c r="D111" s="9" t="s">
         <v>20</v>
       </c>
@@ -7994,9 +7995,9 @@
       <c r="S111" s="61"/>
     </row>
     <row r="112" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A112" s="115"/>
-      <c r="B112" s="116"/>
-      <c r="C112" s="112"/>
+      <c r="A112" s="125"/>
+      <c r="B112" s="111"/>
+      <c r="C112" s="123"/>
       <c r="D112" s="9" t="s">
         <v>24</v>
       </c>
@@ -8019,9 +8020,9 @@
       </c>
     </row>
     <row r="113" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A113" s="115"/>
-      <c r="B113" s="116"/>
-      <c r="C113" s="112"/>
+      <c r="A113" s="125"/>
+      <c r="B113" s="111"/>
+      <c r="C113" s="123"/>
       <c r="D113" s="49" t="s">
         <v>64</v>
       </c>
@@ -8086,11 +8087,11 @@
       </c>
     </row>
     <row r="114" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="114" t="s">
+      <c r="A114" s="124" t="s">
         <v>69</v>
       </c>
-      <c r="B114" s="116"/>
-      <c r="C114" s="111" t="s">
+      <c r="B114" s="111"/>
+      <c r="C114" s="122" t="s">
         <v>78</v>
       </c>
       <c r="I114" s="10"/>
@@ -8102,9 +8103,9 @@
       <c r="U114" s="10"/>
     </row>
     <row r="115" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A115" s="115"/>
-      <c r="B115" s="116"/>
-      <c r="C115" s="112"/>
+      <c r="A115" s="125"/>
+      <c r="B115" s="111"/>
+      <c r="C115" s="123"/>
       <c r="D115" s="9" t="s">
         <v>25</v>
       </c>
@@ -8157,9 +8158,9 @@
       <c r="U115" s="10"/>
     </row>
     <row r="116" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A116" s="115"/>
-      <c r="B116" s="116"/>
-      <c r="C116" s="112"/>
+      <c r="A116" s="125"/>
+      <c r="B116" s="111"/>
+      <c r="C116" s="123"/>
       <c r="D116" s="9" t="s">
         <v>14</v>
       </c>
@@ -8212,9 +8213,9 @@
       <c r="U116" s="10"/>
     </row>
     <row r="117" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A117" s="115"/>
-      <c r="B117" s="116"/>
-      <c r="C117" s="112"/>
+      <c r="A117" s="125"/>
+      <c r="B117" s="111"/>
+      <c r="C117" s="123"/>
       <c r="D117" s="9" t="s">
         <v>36</v>
       </c>
@@ -8263,9 +8264,9 @@
       <c r="S117" s="61"/>
     </row>
     <row r="118" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A118" s="115"/>
-      <c r="B118" s="116"/>
-      <c r="C118" s="112"/>
+      <c r="A118" s="125"/>
+      <c r="B118" s="111"/>
+      <c r="C118" s="123"/>
       <c r="D118" s="9" t="s">
         <v>22</v>
       </c>
@@ -8314,9 +8315,9 @@
       <c r="S118" s="61"/>
     </row>
     <row r="119" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A119" s="115"/>
-      <c r="B119" s="116"/>
-      <c r="C119" s="112"/>
+      <c r="A119" s="125"/>
+      <c r="B119" s="111"/>
+      <c r="C119" s="123"/>
       <c r="D119" s="48" t="s">
         <v>61</v>
       </c>
@@ -8365,9 +8366,9 @@
       <c r="S119" s="10"/>
     </row>
     <row r="120" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A120" s="115"/>
-      <c r="B120" s="116"/>
-      <c r="C120" s="112"/>
+      <c r="A120" s="125"/>
+      <c r="B120" s="111"/>
+      <c r="C120" s="123"/>
       <c r="D120" s="9" t="s">
         <v>21</v>
       </c>
@@ -8416,9 +8417,9 @@
       <c r="S120" s="61"/>
     </row>
     <row r="121" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A121" s="115"/>
-      <c r="B121" s="116"/>
-      <c r="C121" s="112"/>
+      <c r="A121" s="125"/>
+      <c r="B121" s="111"/>
+      <c r="C121" s="123"/>
       <c r="D121" s="48" t="s">
         <v>62</v>
       </c>
@@ -8467,9 +8468,9 @@
       <c r="S121" s="10"/>
     </row>
     <row r="122" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A122" s="115"/>
-      <c r="B122" s="116"/>
-      <c r="C122" s="112"/>
+      <c r="A122" s="125"/>
+      <c r="B122" s="111"/>
+      <c r="C122" s="123"/>
       <c r="D122" s="9" t="s">
         <v>23</v>
       </c>
@@ -8518,9 +8519,9 @@
       <c r="S122" s="61"/>
     </row>
     <row r="123" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A123" s="115"/>
-      <c r="B123" s="116"/>
-      <c r="C123" s="112"/>
+      <c r="A123" s="125"/>
+      <c r="B123" s="111"/>
+      <c r="C123" s="123"/>
       <c r="D123" s="48" t="s">
         <v>63</v>
       </c>
@@ -8582,9 +8583,9 @@
       </c>
     </row>
     <row r="124" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A124" s="115"/>
-      <c r="B124" s="116"/>
-      <c r="C124" s="112"/>
+      <c r="A124" s="125"/>
+      <c r="B124" s="111"/>
+      <c r="C124" s="123"/>
       <c r="D124" s="9" t="s">
         <v>20</v>
       </c>
@@ -8633,9 +8634,9 @@
       <c r="S124" s="61"/>
     </row>
     <row r="125" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A125" s="115"/>
-      <c r="B125" s="116"/>
-      <c r="C125" s="112"/>
+      <c r="A125" s="125"/>
+      <c r="B125" s="111"/>
+      <c r="C125" s="123"/>
       <c r="D125" s="9" t="s">
         <v>24</v>
       </c>
@@ -8658,9 +8659,9 @@
       </c>
     </row>
     <row r="126" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A126" s="115"/>
-      <c r="B126" s="116"/>
-      <c r="C126" s="112"/>
+      <c r="A126" s="125"/>
+      <c r="B126" s="111"/>
+      <c r="C126" s="123"/>
       <c r="D126" s="49" t="s">
         <v>64</v>
       </c>
@@ -8725,9 +8726,9 @@
       </c>
     </row>
     <row r="127" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A127" s="115"/>
-      <c r="B127" s="116"/>
-      <c r="C127" s="111" t="s">
+      <c r="A127" s="125"/>
+      <c r="B127" s="111"/>
+      <c r="C127" s="122" t="s">
         <v>79</v>
       </c>
       <c r="I127" s="10"/>
@@ -8739,9 +8740,9 @@
       <c r="U127" s="10"/>
     </row>
     <row r="128" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A128" s="115"/>
-      <c r="B128" s="116"/>
-      <c r="C128" s="112"/>
+      <c r="A128" s="125"/>
+      <c r="B128" s="111"/>
+      <c r="C128" s="123"/>
       <c r="D128" s="9" t="s">
         <v>25</v>
       </c>
@@ -8794,9 +8795,9 @@
       <c r="U128" s="10"/>
     </row>
     <row r="129" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A129" s="115"/>
-      <c r="B129" s="116"/>
-      <c r="C129" s="112"/>
+      <c r="A129" s="125"/>
+      <c r="B129" s="111"/>
+      <c r="C129" s="123"/>
       <c r="D129" s="9" t="s">
         <v>14</v>
       </c>
@@ -8849,9 +8850,9 @@
       <c r="U129" s="10"/>
     </row>
     <row r="130" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A130" s="115"/>
-      <c r="B130" s="116"/>
-      <c r="C130" s="112"/>
+      <c r="A130" s="125"/>
+      <c r="B130" s="111"/>
+      <c r="C130" s="123"/>
       <c r="D130" s="9" t="s">
         <v>36</v>
       </c>
@@ -8900,9 +8901,9 @@
       <c r="S130" s="61"/>
     </row>
     <row r="131" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A131" s="115"/>
-      <c r="B131" s="116"/>
-      <c r="C131" s="112"/>
+      <c r="A131" s="125"/>
+      <c r="B131" s="111"/>
+      <c r="C131" s="123"/>
       <c r="D131" s="9" t="s">
         <v>22</v>
       </c>
@@ -8951,9 +8952,9 @@
       <c r="S131" s="61"/>
     </row>
     <row r="132" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A132" s="115"/>
-      <c r="B132" s="116"/>
-      <c r="C132" s="112"/>
+      <c r="A132" s="125"/>
+      <c r="B132" s="111"/>
+      <c r="C132" s="123"/>
       <c r="D132" s="48" t="s">
         <v>61</v>
       </c>
@@ -9002,9 +9003,9 @@
       <c r="S132" s="10"/>
     </row>
     <row r="133" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A133" s="115"/>
-      <c r="B133" s="116"/>
-      <c r="C133" s="112"/>
+      <c r="A133" s="125"/>
+      <c r="B133" s="111"/>
+      <c r="C133" s="123"/>
       <c r="D133" s="9" t="s">
         <v>21</v>
       </c>
@@ -9053,9 +9054,9 @@
       <c r="S133" s="61"/>
     </row>
     <row r="134" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A134" s="115"/>
-      <c r="B134" s="116"/>
-      <c r="C134" s="112"/>
+      <c r="A134" s="125"/>
+      <c r="B134" s="111"/>
+      <c r="C134" s="123"/>
       <c r="D134" s="48" t="s">
         <v>62</v>
       </c>
@@ -9104,9 +9105,9 @@
       <c r="S134" s="10"/>
     </row>
     <row r="135" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A135" s="115"/>
-      <c r="B135" s="116"/>
-      <c r="C135" s="112"/>
+      <c r="A135" s="125"/>
+      <c r="B135" s="111"/>
+      <c r="C135" s="123"/>
       <c r="D135" s="9" t="s">
         <v>23</v>
       </c>
@@ -9155,9 +9156,9 @@
       <c r="S135" s="61"/>
     </row>
     <row r="136" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A136" s="115"/>
-      <c r="B136" s="116"/>
-      <c r="C136" s="112"/>
+      <c r="A136" s="125"/>
+      <c r="B136" s="111"/>
+      <c r="C136" s="123"/>
       <c r="D136" s="48" t="s">
         <v>63</v>
       </c>
@@ -9219,9 +9220,9 @@
       </c>
     </row>
     <row r="137" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A137" s="115"/>
-      <c r="B137" s="116"/>
-      <c r="C137" s="112"/>
+      <c r="A137" s="125"/>
+      <c r="B137" s="111"/>
+      <c r="C137" s="123"/>
       <c r="D137" s="9" t="s">
         <v>20</v>
       </c>
@@ -9270,9 +9271,9 @@
       <c r="S137" s="61"/>
     </row>
     <row r="138" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A138" s="115"/>
-      <c r="B138" s="116"/>
-      <c r="C138" s="112"/>
+      <c r="A138" s="125"/>
+      <c r="B138" s="111"/>
+      <c r="C138" s="123"/>
       <c r="D138" s="9" t="s">
         <v>24</v>
       </c>
@@ -9295,9 +9296,9 @@
       </c>
     </row>
     <row r="139" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A139" s="115"/>
-      <c r="B139" s="116"/>
-      <c r="C139" s="112"/>
+      <c r="A139" s="125"/>
+      <c r="B139" s="111"/>
+      <c r="C139" s="123"/>
       <c r="D139" s="49" t="s">
         <v>64</v>
       </c>
@@ -9362,9 +9363,9 @@
       </c>
     </row>
     <row r="140" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A140" s="115"/>
-      <c r="B140" s="116"/>
-      <c r="C140" s="113" t="s">
+      <c r="A140" s="125"/>
+      <c r="B140" s="111"/>
+      <c r="C140" s="121" t="s">
         <v>80</v>
       </c>
       <c r="I140" s="10"/>
@@ -9376,9 +9377,9 @@
       <c r="U140" s="10"/>
     </row>
     <row r="141" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A141" s="115"/>
-      <c r="B141" s="116"/>
-      <c r="C141" s="113"/>
+      <c r="A141" s="125"/>
+      <c r="B141" s="111"/>
+      <c r="C141" s="121"/>
       <c r="D141" s="9" t="s">
         <v>25</v>
       </c>
@@ -9431,9 +9432,9 @@
       <c r="U141" s="10"/>
     </row>
     <row r="142" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A142" s="115"/>
-      <c r="B142" s="116"/>
-      <c r="C142" s="113"/>
+      <c r="A142" s="125"/>
+      <c r="B142" s="111"/>
+      <c r="C142" s="121"/>
       <c r="D142" s="9" t="s">
         <v>14</v>
       </c>
@@ -9486,9 +9487,9 @@
       <c r="U142" s="10"/>
     </row>
     <row r="143" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A143" s="115"/>
-      <c r="B143" s="116"/>
-      <c r="C143" s="113"/>
+      <c r="A143" s="125"/>
+      <c r="B143" s="111"/>
+      <c r="C143" s="121"/>
       <c r="D143" s="9" t="s">
         <v>36</v>
       </c>
@@ -9537,9 +9538,9 @@
       <c r="S143" s="61"/>
     </row>
     <row r="144" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A144" s="115"/>
-      <c r="B144" s="116"/>
-      <c r="C144" s="113"/>
+      <c r="A144" s="125"/>
+      <c r="B144" s="111"/>
+      <c r="C144" s="121"/>
       <c r="D144" s="9" t="s">
         <v>22</v>
       </c>
@@ -9588,9 +9589,9 @@
       <c r="S144" s="61"/>
     </row>
     <row r="145" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A145" s="115"/>
-      <c r="B145" s="116"/>
-      <c r="C145" s="113"/>
+      <c r="A145" s="125"/>
+      <c r="B145" s="111"/>
+      <c r="C145" s="121"/>
       <c r="D145" s="48" t="s">
         <v>61</v>
       </c>
@@ -9639,9 +9640,9 @@
       <c r="S145" s="10"/>
     </row>
     <row r="146" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A146" s="115"/>
-      <c r="B146" s="116"/>
-      <c r="C146" s="113"/>
+      <c r="A146" s="125"/>
+      <c r="B146" s="111"/>
+      <c r="C146" s="121"/>
       <c r="D146" s="9" t="s">
         <v>21</v>
       </c>
@@ -9690,9 +9691,9 @@
       <c r="S146" s="61"/>
     </row>
     <row r="147" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A147" s="115"/>
-      <c r="B147" s="116"/>
-      <c r="C147" s="113"/>
+      <c r="A147" s="125"/>
+      <c r="B147" s="111"/>
+      <c r="C147" s="121"/>
       <c r="D147" s="48" t="s">
         <v>62</v>
       </c>
@@ -9741,9 +9742,9 @@
       <c r="S147" s="10"/>
     </row>
     <row r="148" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A148" s="115"/>
-      <c r="B148" s="116"/>
-      <c r="C148" s="113"/>
+      <c r="A148" s="125"/>
+      <c r="B148" s="111"/>
+      <c r="C148" s="121"/>
       <c r="D148" s="9" t="s">
         <v>23</v>
       </c>
@@ -9792,9 +9793,9 @@
       <c r="S148" s="61"/>
     </row>
     <row r="149" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A149" s="115"/>
-      <c r="B149" s="116"/>
-      <c r="C149" s="113"/>
+      <c r="A149" s="125"/>
+      <c r="B149" s="111"/>
+      <c r="C149" s="121"/>
       <c r="D149" s="48" t="s">
         <v>63</v>
       </c>
@@ -9856,9 +9857,9 @@
       </c>
     </row>
     <row r="150" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A150" s="115"/>
-      <c r="B150" s="116"/>
-      <c r="C150" s="113"/>
+      <c r="A150" s="125"/>
+      <c r="B150" s="111"/>
+      <c r="C150" s="121"/>
       <c r="D150" s="9" t="s">
         <v>20</v>
       </c>
@@ -9907,9 +9908,9 @@
       <c r="S150" s="61"/>
     </row>
     <row r="151" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A151" s="115"/>
-      <c r="B151" s="116"/>
-      <c r="C151" s="113"/>
+      <c r="A151" s="125"/>
+      <c r="B151" s="111"/>
+      <c r="C151" s="121"/>
       <c r="D151" s="9" t="s">
         <v>24</v>
       </c>
@@ -9932,9 +9933,9 @@
       </c>
     </row>
     <row r="152" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A152" s="115"/>
-      <c r="B152" s="116"/>
-      <c r="C152" s="113"/>
+      <c r="A152" s="125"/>
+      <c r="B152" s="111"/>
+      <c r="C152" s="121"/>
       <c r="D152" s="49" t="s">
         <v>64</v>
       </c>
@@ -9999,9 +10000,9 @@
       </c>
     </row>
     <row r="153" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A153" s="115"/>
-      <c r="B153" s="116"/>
-      <c r="C153" s="113"/>
+      <c r="A153" s="125"/>
+      <c r="B153" s="111"/>
+      <c r="C153" s="121"/>
       <c r="D153" s="52" t="s">
         <v>67</v>
       </c>
@@ -10103,17 +10104,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A22:A31"/>
-    <mergeCell ref="A8:C11"/>
-    <mergeCell ref="B13:C15"/>
-    <mergeCell ref="B22:B27"/>
-    <mergeCell ref="A13:A19"/>
-    <mergeCell ref="B16:C19"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C30:C31"/>
     <mergeCell ref="C127:C139"/>
     <mergeCell ref="C140:C153"/>
     <mergeCell ref="A34:A60"/>
@@ -10130,6 +10120,17 @@
     <mergeCell ref="C34:C46"/>
     <mergeCell ref="B47:B60"/>
     <mergeCell ref="C47:C60"/>
+    <mergeCell ref="A22:A31"/>
+    <mergeCell ref="A8:C11"/>
+    <mergeCell ref="B13:C15"/>
+    <mergeCell ref="B22:B27"/>
+    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="B16:C19"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C30:C31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="58" fitToHeight="5" orientation="landscape" r:id="rId1"/>
@@ -10142,11 +10143,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y226"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:Y233"/>
   <sheetViews>
-    <sheetView topLeftCell="A112" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K104" sqref="K104"/>
+    <sheetView tabSelected="1" topLeftCell="A144" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A167" sqref="A167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14980,10 +14981,10 @@
         <v>1</v>
       </c>
       <c r="K147">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="L147">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M147">
         <v>1</v>
@@ -15004,7 +15005,7 @@
         <v>1</v>
       </c>
       <c r="U147" s="95">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="148" spans="1:21" x14ac:dyDescent="0.3">
@@ -15036,7 +15037,7 @@
         <v>2</v>
       </c>
       <c r="L148">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M148">
         <v>1</v>
@@ -15057,7 +15058,7 @@
         <v>2</v>
       </c>
       <c r="U148" s="95">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="149" spans="1:21" x14ac:dyDescent="0.3">
@@ -15089,7 +15090,7 @@
         <v>2</v>
       </c>
       <c r="L149">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M149">
         <v>1</v>
@@ -15110,7 +15111,7 @@
         <v>3</v>
       </c>
       <c r="U149" s="95">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="150" spans="1:21" x14ac:dyDescent="0.3">
@@ -15142,7 +15143,7 @@
         <v>2</v>
       </c>
       <c r="L150">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M150">
         <v>1</v>
@@ -15163,7 +15164,7 @@
         <v>4</v>
       </c>
       <c r="U150" s="95">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="151" spans="1:21" x14ac:dyDescent="0.3">
@@ -15195,7 +15196,7 @@
         <v>2</v>
       </c>
       <c r="L151">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M151">
         <v>1</v>
@@ -15216,7 +15217,7 @@
         <v>5</v>
       </c>
       <c r="U151" s="95">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="152" spans="1:21" x14ac:dyDescent="0.3">
@@ -15248,7 +15249,7 @@
         <v>2</v>
       </c>
       <c r="L152">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M152">
         <v>1</v>
@@ -15269,7 +15270,7 @@
         <v>6</v>
       </c>
       <c r="U152" s="95">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="153" spans="1:21" x14ac:dyDescent="0.3">
@@ -15301,7 +15302,7 @@
         <v>2</v>
       </c>
       <c r="L153" s="95">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M153" s="95">
         <v>1</v>
@@ -15322,7 +15323,7 @@
         <v>7</v>
       </c>
       <c r="U153" s="95">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="154" spans="1:21" x14ac:dyDescent="0.3">
@@ -15354,7 +15355,7 @@
         <v>2</v>
       </c>
       <c r="L154" s="95">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M154" s="95">
         <v>1</v>
@@ -15375,7 +15376,7 @@
         <v>8</v>
       </c>
       <c r="U154" s="95">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="155" spans="1:21" x14ac:dyDescent="0.3">
@@ -15428,7 +15429,7 @@
         <v>9</v>
       </c>
       <c r="U155" s="95">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="156" spans="1:21" x14ac:dyDescent="0.3">
@@ -15460,7 +15461,7 @@
         <v>10</v>
       </c>
       <c r="U156" s="95">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="157" spans="1:21" x14ac:dyDescent="0.3">
@@ -15473,17 +15474,17 @@
       <c r="C157">
         <v>1</v>
       </c>
-      <c r="E157">
-        <v>2</v>
-      </c>
-      <c r="F157">
+      <c r="E157" s="95">
+        <v>2</v>
+      </c>
+      <c r="F157" s="95">
         <v>1</v>
       </c>
       <c r="G157">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H157">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="158" spans="1:21" x14ac:dyDescent="0.3">
@@ -15496,17 +15497,17 @@
       <c r="C158">
         <v>1</v>
       </c>
-      <c r="E158">
-        <v>2</v>
-      </c>
-      <c r="F158">
+      <c r="E158" s="95">
+        <v>2</v>
+      </c>
+      <c r="F158" s="95">
         <v>1</v>
       </c>
       <c r="G158">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H158">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159" spans="1:21" x14ac:dyDescent="0.3">
@@ -15519,17 +15520,17 @@
       <c r="C159">
         <v>1</v>
       </c>
-      <c r="E159">
-        <v>2</v>
-      </c>
-      <c r="F159">
+      <c r="E159" s="95">
+        <v>2</v>
+      </c>
+      <c r="F159" s="95">
         <v>1</v>
       </c>
       <c r="G159">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="H159">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="160" spans="1:21" x14ac:dyDescent="0.3">
@@ -15542,20 +15543,20 @@
       <c r="C160">
         <v>1</v>
       </c>
-      <c r="E160">
-        <v>2</v>
-      </c>
-      <c r="F160">
+      <c r="E160" s="95">
+        <v>2</v>
+      </c>
+      <c r="F160" s="95">
         <v>1</v>
       </c>
       <c r="G160">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H160">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="161" spans="1:21" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A161" s="95">
         <v>5</v>
       </c>
@@ -15566,19 +15567,19 @@
         <v>1</v>
       </c>
       <c r="E161">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F161">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G161">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H161">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="162" spans="1:21" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A162" s="95">
         <v>6</v>
       </c>
@@ -15592,16 +15593,16 @@
         <v>2</v>
       </c>
       <c r="F162">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G162">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H162">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="163" spans="1:21" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A163" s="95">
         <v>7</v>
       </c>
@@ -15611,8 +15612,20 @@
       <c r="C163">
         <v>1</v>
       </c>
-    </row>
-    <row r="164" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="E163">
+        <v>2</v>
+      </c>
+      <c r="F163">
+        <v>1</v>
+      </c>
+      <c r="G163">
+        <v>7</v>
+      </c>
+      <c r="H163">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A164" s="95">
         <v>8</v>
       </c>
@@ -15622,8 +15635,20 @@
       <c r="C164">
         <v>1</v>
       </c>
-    </row>
-    <row r="165" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="E164">
+        <v>2</v>
+      </c>
+      <c r="F164">
+        <v>1</v>
+      </c>
+      <c r="G164">
+        <v>8</v>
+      </c>
+      <c r="H164">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A165" s="95">
         <v>9</v>
       </c>
@@ -15633,8 +15658,20 @@
       <c r="C165">
         <v>1</v>
       </c>
-    </row>
-    <row r="166" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="E165">
+        <v>2</v>
+      </c>
+      <c r="F165">
+        <v>1</v>
+      </c>
+      <c r="G165">
+        <v>9</v>
+      </c>
+      <c r="H165">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A166" s="95">
         <v>10</v>
       </c>
@@ -15644,479 +15681,154 @@
       <c r="C166">
         <v>1</v>
       </c>
-    </row>
-    <row r="168" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A168" s="1" t="s">
+      <c r="E166">
+        <v>2</v>
+      </c>
+      <c r="F166">
+        <v>1</v>
+      </c>
+      <c r="G166">
+        <v>10</v>
+      </c>
+      <c r="H166">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E167">
+        <v>1</v>
+      </c>
+      <c r="F167">
+        <v>2</v>
+      </c>
+      <c r="G167">
+        <v>1</v>
+      </c>
+      <c r="H167">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" s="95" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E168">
+        <v>2</v>
+      </c>
+      <c r="F168">
+        <v>2</v>
+      </c>
+      <c r="G168">
+        <v>1</v>
+      </c>
+      <c r="H168">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" s="95" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="170" spans="1:8" s="95" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="171" spans="1:8" s="95" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="172" spans="1:8" s="95" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="173" spans="1:8" s="95" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="174" spans="1:8" s="95" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="175" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A175" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="169" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="170" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A170" s="95" t="s">
+    <row r="176" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="177" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A177" s="95" t="s">
         <v>119</v>
       </c>
-      <c r="B170" s="95"/>
-      <c r="C170" s="95"/>
-      <c r="D170" s="95"/>
-      <c r="E170" s="95" t="s">
+      <c r="B177" s="95"/>
+      <c r="C177" s="95"/>
+      <c r="D177" s="95"/>
+      <c r="E177" s="95" t="s">
         <v>123</v>
       </c>
-      <c r="F170" s="95"/>
-      <c r="G170" s="95"/>
-      <c r="H170" s="95"/>
-      <c r="I170" s="95"/>
-      <c r="J170" s="95" t="s">
+      <c r="F177" s="95"/>
+      <c r="G177" s="95"/>
+      <c r="H177" s="95"/>
+      <c r="I177" s="95"/>
+      <c r="J177" s="95" t="s">
         <v>132</v>
       </c>
-      <c r="K170" s="95"/>
-      <c r="L170" s="95"/>
-      <c r="M170" s="95"/>
-      <c r="N170" s="95"/>
-      <c r="O170" s="95"/>
-      <c r="P170" s="95"/>
-      <c r="Q170" s="95"/>
-      <c r="S170" s="95" t="s">
+      <c r="K177" s="95"/>
+      <c r="L177" s="95"/>
+      <c r="M177" s="95"/>
+      <c r="N177" s="95"/>
+      <c r="O177" s="95"/>
+      <c r="P177" s="95"/>
+      <c r="Q177" s="95"/>
+      <c r="S177" s="95" t="s">
         <v>133</v>
       </c>
-      <c r="T170" s="95"/>
-      <c r="U170" s="95"/>
-    </row>
-    <row r="171" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A171" s="95" t="s">
+      <c r="T177" s="95"/>
+      <c r="U177" s="95"/>
+    </row>
+    <row r="178" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A178" s="95" t="s">
         <v>120</v>
       </c>
-      <c r="B171" s="95" t="s">
+      <c r="B178" s="95" t="s">
         <v>121</v>
       </c>
-      <c r="C171" s="95" t="s">
+      <c r="C178" s="95" t="s">
         <v>122</v>
       </c>
-      <c r="D171" s="95"/>
-      <c r="E171" s="95" t="s">
+      <c r="D178" s="95"/>
+      <c r="E178" s="95" t="s">
         <v>124</v>
       </c>
-      <c r="F171" s="95" t="s">
+      <c r="F178" s="95" t="s">
         <v>121</v>
       </c>
-      <c r="G171" s="95" t="s">
+      <c r="G178" s="95" t="s">
         <v>125</v>
       </c>
-      <c r="H171" s="95" t="s">
+      <c r="H178" s="95" t="s">
         <v>126</v>
       </c>
-      <c r="I171" s="95"/>
-      <c r="J171" s="95" t="s">
+      <c r="I178" s="95"/>
+      <c r="J178" s="95" t="s">
         <v>126</v>
       </c>
-      <c r="K171" s="95" t="s">
+      <c r="K178" s="95" t="s">
         <v>127</v>
       </c>
-      <c r="L171" s="95" t="s">
+      <c r="L178" s="95" t="s">
         <v>128</v>
       </c>
-      <c r="M171" s="95" t="s">
+      <c r="M178" s="95" t="s">
         <v>138</v>
       </c>
-      <c r="N171" s="95" t="s">
+      <c r="N178" s="95" t="s">
         <v>129</v>
       </c>
-      <c r="O171" s="95" t="s">
+      <c r="O178" s="95" t="s">
         <v>130</v>
       </c>
-      <c r="P171" s="95" t="s">
+      <c r="P178" s="95" t="s">
         <v>131</v>
       </c>
-      <c r="Q171" s="95"/>
-      <c r="S171" s="95" t="s">
+      <c r="Q178" s="95"/>
+      <c r="S178" s="95" t="s">
         <v>134</v>
       </c>
-      <c r="T171" s="95" t="s">
+      <c r="T178" s="95" t="s">
         <v>125</v>
       </c>
-      <c r="U171" s="95" t="s">
+      <c r="U178" s="95" t="s">
         <v>124</v>
-      </c>
-    </row>
-    <row r="172" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A172" s="95">
-        <v>1</v>
-      </c>
-      <c r="B172" s="95">
-        <v>1</v>
-      </c>
-      <c r="C172" s="95">
-        <v>1</v>
-      </c>
-      <c r="E172" s="95">
-        <v>1</v>
-      </c>
-      <c r="F172" s="95">
-        <v>1</v>
-      </c>
-      <c r="G172" s="95">
-        <v>1</v>
-      </c>
-      <c r="H172" s="95">
-        <v>1</v>
-      </c>
-      <c r="J172">
-        <v>1</v>
-      </c>
-      <c r="K172">
-        <v>2</v>
-      </c>
-      <c r="L172">
-        <v>0</v>
-      </c>
-      <c r="M172">
-        <v>1</v>
-      </c>
-      <c r="N172">
-        <v>1000000</v>
-      </c>
-      <c r="O172">
-        <v>1000000</v>
-      </c>
-      <c r="P172">
-        <v>0.5</v>
-      </c>
-      <c r="S172" s="95">
-        <v>1</v>
-      </c>
-      <c r="T172" s="95">
-        <v>1</v>
-      </c>
-      <c r="U172" s="95">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="173" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A173" s="95">
-        <v>2</v>
-      </c>
-      <c r="B173" s="95">
-        <v>1</v>
-      </c>
-      <c r="C173" s="95">
-        <v>2</v>
-      </c>
-      <c r="E173" s="95">
-        <v>1</v>
-      </c>
-      <c r="F173" s="95">
-        <v>1</v>
-      </c>
-      <c r="G173" s="95">
-        <v>2</v>
-      </c>
-      <c r="H173" s="95">
-        <v>1</v>
-      </c>
-      <c r="J173">
-        <v>2</v>
-      </c>
-      <c r="K173">
-        <v>2</v>
-      </c>
-      <c r="L173">
-        <v>0</v>
-      </c>
-      <c r="M173">
-        <v>1</v>
-      </c>
-      <c r="N173">
-        <v>2000000</v>
-      </c>
-      <c r="O173">
-        <v>3000000</v>
-      </c>
-      <c r="P173">
-        <v>0.9</v>
-      </c>
-      <c r="S173" s="95">
-        <v>2</v>
-      </c>
-      <c r="T173" s="95">
-        <v>2</v>
-      </c>
-      <c r="U173" s="95">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="174" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A174" s="95">
-        <v>3</v>
-      </c>
-      <c r="B174" s="95">
-        <v>1</v>
-      </c>
-      <c r="C174" s="95">
-        <v>3</v>
-      </c>
-      <c r="E174" s="95">
-        <v>1</v>
-      </c>
-      <c r="F174" s="95">
-        <v>1</v>
-      </c>
-      <c r="G174" s="95">
-        <v>3</v>
-      </c>
-      <c r="H174" s="95">
-        <v>1</v>
-      </c>
-      <c r="J174">
-        <v>3</v>
-      </c>
-      <c r="K174">
-        <v>2</v>
-      </c>
-      <c r="L174">
-        <v>0</v>
-      </c>
-      <c r="M174">
-        <v>1</v>
-      </c>
-      <c r="N174">
-        <v>5000000</v>
-      </c>
-      <c r="O174">
-        <v>5000000</v>
-      </c>
-      <c r="P174">
-        <v>1</v>
-      </c>
-      <c r="S174" s="95">
-        <v>3</v>
-      </c>
-      <c r="T174" s="95">
-        <v>3</v>
-      </c>
-      <c r="U174" s="95">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="175" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A175" s="95">
-        <v>4</v>
-      </c>
-      <c r="B175" s="95">
-        <v>1</v>
-      </c>
-      <c r="C175" s="95">
-        <v>4</v>
-      </c>
-      <c r="E175" s="95">
-        <v>1</v>
-      </c>
-      <c r="F175" s="95">
-        <v>1</v>
-      </c>
-      <c r="G175" s="95">
-        <v>4</v>
-      </c>
-      <c r="H175" s="95">
-        <v>1</v>
-      </c>
-      <c r="J175">
-        <v>4</v>
-      </c>
-      <c r="K175">
-        <v>2</v>
-      </c>
-      <c r="L175">
-        <v>0</v>
-      </c>
-      <c r="M175">
-        <v>1</v>
-      </c>
-      <c r="N175">
-        <v>10000000</v>
-      </c>
-      <c r="O175">
-        <v>10000000</v>
-      </c>
-      <c r="P175">
-        <v>1</v>
-      </c>
-      <c r="S175" s="95">
-        <v>4</v>
-      </c>
-      <c r="T175" s="95">
-        <v>4</v>
-      </c>
-      <c r="U175" s="95">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="176" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A176" s="95">
-        <v>5</v>
-      </c>
-      <c r="B176" s="95">
-        <v>1</v>
-      </c>
-      <c r="C176" s="95">
-        <v>5</v>
-      </c>
-      <c r="E176" s="95">
-        <v>1</v>
-      </c>
-      <c r="F176" s="95">
-        <v>1</v>
-      </c>
-      <c r="G176" s="95">
-        <v>5</v>
-      </c>
-      <c r="H176" s="95">
-        <v>1</v>
-      </c>
-      <c r="J176">
-        <v>5</v>
-      </c>
-      <c r="K176">
-        <v>2</v>
-      </c>
-      <c r="L176">
-        <v>0</v>
-      </c>
-      <c r="M176">
-        <v>1</v>
-      </c>
-      <c r="N176">
-        <v>20000000</v>
-      </c>
-      <c r="O176">
-        <v>10000000</v>
-      </c>
-      <c r="P176">
-        <v>1</v>
-      </c>
-      <c r="S176" s="95">
-        <v>5</v>
-      </c>
-      <c r="T176" s="95">
-        <v>5</v>
-      </c>
-      <c r="U176" s="95">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="177" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A177" s="95">
-        <v>6</v>
-      </c>
-      <c r="B177" s="95">
-        <v>1</v>
-      </c>
-      <c r="C177" s="95">
-        <v>6</v>
-      </c>
-      <c r="E177" s="95">
-        <v>1</v>
-      </c>
-      <c r="F177" s="95">
-        <v>1</v>
-      </c>
-      <c r="G177" s="95">
-        <v>6</v>
-      </c>
-      <c r="H177" s="95">
-        <v>1</v>
-      </c>
-      <c r="J177">
-        <v>6</v>
-      </c>
-      <c r="K177">
-        <v>14</v>
-      </c>
-      <c r="L177">
-        <v>2</v>
-      </c>
-      <c r="M177" s="95">
-        <v>1</v>
-      </c>
-      <c r="N177">
-        <v>0</v>
-      </c>
-      <c r="O177">
-        <v>3000000</v>
-      </c>
-      <c r="P177">
-        <v>0</v>
-      </c>
-      <c r="S177" s="95">
-        <v>6</v>
-      </c>
-      <c r="T177" s="95">
-        <v>6</v>
-      </c>
-      <c r="U177" s="95">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="178" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A178" s="95">
-        <v>7</v>
-      </c>
-      <c r="B178" s="95">
-        <v>1</v>
-      </c>
-      <c r="C178" s="95">
-        <v>7</v>
-      </c>
-      <c r="E178" s="95">
-        <v>1</v>
-      </c>
-      <c r="F178" s="95">
-        <v>1</v>
-      </c>
-      <c r="G178" s="95">
-        <v>7</v>
-      </c>
-      <c r="H178" s="95">
-        <v>1</v>
-      </c>
-      <c r="J178">
-        <v>7</v>
-      </c>
-      <c r="K178" s="95">
-        <v>14</v>
-      </c>
-      <c r="L178">
-        <v>2</v>
-      </c>
-      <c r="M178" s="95">
-        <v>1</v>
-      </c>
-      <c r="N178">
-        <v>0</v>
-      </c>
-      <c r="O178">
-        <v>9000000</v>
-      </c>
-      <c r="P178">
-        <v>0</v>
-      </c>
-      <c r="S178" s="95">
-        <v>7</v>
-      </c>
-      <c r="T178" s="95">
-        <v>7</v>
-      </c>
-      <c r="U178" s="95">
-        <v>1</v>
       </c>
     </row>
     <row r="179" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A179" s="95">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B179" s="95">
         <v>1</v>
       </c>
       <c r="C179" s="95">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E179" s="95">
         <v>1</v>
@@ -16125,37 +15837,37 @@
         <v>1</v>
       </c>
       <c r="G179" s="95">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H179" s="95">
         <v>1</v>
       </c>
       <c r="J179">
-        <v>8</v>
-      </c>
-      <c r="K179" s="95">
-        <v>14</v>
+        <v>1</v>
+      </c>
+      <c r="K179">
+        <v>2</v>
       </c>
       <c r="L179">
-        <v>2</v>
-      </c>
-      <c r="M179" s="95">
+        <v>0</v>
+      </c>
+      <c r="M179">
         <v>1</v>
       </c>
       <c r="N179">
-        <v>0</v>
+        <v>1000000</v>
       </c>
       <c r="O179">
-        <v>15000000</v>
+        <v>1000000</v>
       </c>
       <c r="P179">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S179" s="95">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="T179" s="95">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="U179" s="95">
         <v>1</v>
@@ -16163,13 +15875,13 @@
     </row>
     <row r="180" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A180" s="95">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B180" s="95">
         <v>1</v>
       </c>
       <c r="C180" s="95">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E180" s="95">
         <v>1</v>
@@ -16178,37 +15890,37 @@
         <v>1</v>
       </c>
       <c r="G180" s="95">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H180" s="95">
         <v>1</v>
       </c>
       <c r="J180">
-        <v>9</v>
-      </c>
-      <c r="K180" s="95">
-        <v>14</v>
+        <v>2</v>
+      </c>
+      <c r="K180">
+        <v>2</v>
       </c>
       <c r="L180">
-        <v>2</v>
-      </c>
-      <c r="M180" s="95">
+        <v>0</v>
+      </c>
+      <c r="M180">
         <v>1</v>
       </c>
       <c r="N180">
-        <v>0</v>
+        <v>2000000</v>
       </c>
       <c r="O180">
-        <v>20000000</v>
+        <v>3000000</v>
       </c>
       <c r="P180">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="S180" s="95">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="T180" s="95">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="U180" s="95">
         <v>1</v>
@@ -16216,13 +15928,13 @@
     </row>
     <row r="181" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A181" s="95">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B181" s="95">
         <v>1</v>
       </c>
       <c r="C181" s="95">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E181" s="95">
         <v>1</v>
@@ -16231,37 +15943,37 @@
         <v>1</v>
       </c>
       <c r="G181" s="95">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H181" s="95">
         <v>1</v>
       </c>
       <c r="J181">
-        <v>10</v>
-      </c>
-      <c r="K181" s="95">
-        <v>14</v>
+        <v>3</v>
+      </c>
+      <c r="K181">
+        <v>2</v>
       </c>
       <c r="L181">
-        <v>2</v>
-      </c>
-      <c r="M181" s="95">
+        <v>0</v>
+      </c>
+      <c r="M181">
         <v>1</v>
       </c>
       <c r="N181">
-        <v>0</v>
+        <v>5000000</v>
       </c>
       <c r="O181">
-        <v>10000000</v>
+        <v>5000000</v>
       </c>
       <c r="P181">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S181" s="95">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="T181" s="95">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="U181" s="95">
         <v>1</v>
@@ -16269,168 +15981,378 @@
     </row>
     <row r="182" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A182" s="95">
-        <v>1</v>
-      </c>
-      <c r="B182">
-        <v>2</v>
-      </c>
-      <c r="C182">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="B182" s="95">
+        <v>1</v>
+      </c>
+      <c r="C182" s="95">
+        <v>4</v>
       </c>
       <c r="E182" s="95">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F182" s="95">
         <v>1</v>
       </c>
       <c r="G182" s="95">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H182" s="95">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="J182">
+        <v>4</v>
+      </c>
+      <c r="K182">
+        <v>2</v>
+      </c>
+      <c r="L182">
+        <v>0</v>
+      </c>
+      <c r="M182">
+        <v>1</v>
+      </c>
+      <c r="N182">
+        <v>10000000</v>
+      </c>
+      <c r="O182">
+        <v>10000000</v>
+      </c>
+      <c r="P182">
+        <v>1</v>
+      </c>
+      <c r="S182" s="95">
+        <v>4</v>
+      </c>
+      <c r="T182" s="95">
+        <v>4</v>
+      </c>
+      <c r="U182" s="95">
+        <v>1</v>
       </c>
     </row>
     <row r="183" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A183" s="95">
-        <v>2</v>
-      </c>
-      <c r="B183">
-        <v>2</v>
-      </c>
-      <c r="C183">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="B183" s="95">
+        <v>1</v>
+      </c>
+      <c r="C183" s="95">
+        <v>5</v>
       </c>
       <c r="E183" s="95">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F183" s="95">
         <v>1</v>
       </c>
       <c r="G183" s="95">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H183" s="95">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="J183">
+        <v>5</v>
+      </c>
+      <c r="K183">
+        <v>2</v>
+      </c>
+      <c r="L183">
+        <v>0</v>
+      </c>
+      <c r="M183">
+        <v>1</v>
+      </c>
+      <c r="N183">
+        <v>20000000</v>
+      </c>
+      <c r="O183">
+        <v>10000000</v>
+      </c>
+      <c r="P183">
+        <v>1</v>
+      </c>
+      <c r="S183" s="95">
+        <v>5</v>
+      </c>
+      <c r="T183" s="95">
+        <v>5</v>
+      </c>
+      <c r="U183" s="95">
+        <v>1</v>
       </c>
     </row>
     <row r="184" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A184" s="95">
-        <v>3</v>
-      </c>
-      <c r="B184">
-        <v>2</v>
-      </c>
-      <c r="C184">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="B184" s="95">
+        <v>1</v>
+      </c>
+      <c r="C184" s="95">
+        <v>6</v>
       </c>
       <c r="E184" s="95">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F184" s="95">
         <v>1</v>
       </c>
       <c r="G184" s="95">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H184" s="95">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="J184">
+        <v>6</v>
+      </c>
+      <c r="K184">
+        <v>14</v>
+      </c>
+      <c r="L184">
+        <v>2</v>
+      </c>
+      <c r="M184" s="95">
+        <v>1</v>
+      </c>
+      <c r="N184">
+        <v>0</v>
+      </c>
+      <c r="O184">
+        <v>3000000</v>
+      </c>
+      <c r="P184">
+        <v>0</v>
+      </c>
+      <c r="S184" s="95">
+        <v>6</v>
+      </c>
+      <c r="T184" s="95">
+        <v>6</v>
+      </c>
+      <c r="U184" s="95">
+        <v>1</v>
       </c>
     </row>
     <row r="185" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A185" s="95">
-        <v>4</v>
-      </c>
-      <c r="B185">
-        <v>2</v>
-      </c>
-      <c r="C185">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="B185" s="95">
+        <v>1</v>
+      </c>
+      <c r="C185" s="95">
+        <v>7</v>
       </c>
       <c r="E185" s="95">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F185" s="95">
         <v>1</v>
       </c>
       <c r="G185" s="95">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H185" s="95">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="J185">
+        <v>7</v>
+      </c>
+      <c r="K185" s="95">
+        <v>14</v>
+      </c>
+      <c r="L185">
+        <v>2</v>
+      </c>
+      <c r="M185" s="95">
+        <v>1</v>
+      </c>
+      <c r="N185">
+        <v>0</v>
+      </c>
+      <c r="O185">
+        <v>9000000</v>
+      </c>
+      <c r="P185">
+        <v>0</v>
+      </c>
+      <c r="S185" s="95">
+        <v>7</v>
+      </c>
+      <c r="T185" s="95">
+        <v>7</v>
+      </c>
+      <c r="U185" s="95">
+        <v>1</v>
       </c>
     </row>
     <row r="186" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A186" s="95">
-        <v>5</v>
-      </c>
-      <c r="B186">
-        <v>2</v>
-      </c>
-      <c r="C186">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="B186" s="95">
+        <v>1</v>
+      </c>
+      <c r="C186" s="95">
+        <v>8</v>
       </c>
       <c r="E186" s="95">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F186" s="95">
         <v>1</v>
       </c>
       <c r="G186" s="95">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H186" s="95">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="J186">
+        <v>8</v>
+      </c>
+      <c r="K186" s="95">
+        <v>14</v>
+      </c>
+      <c r="L186">
+        <v>2</v>
+      </c>
+      <c r="M186" s="95">
+        <v>1</v>
+      </c>
+      <c r="N186">
+        <v>0</v>
+      </c>
+      <c r="O186">
+        <v>15000000</v>
+      </c>
+      <c r="P186">
+        <v>0</v>
+      </c>
+      <c r="S186" s="95">
+        <v>8</v>
+      </c>
+      <c r="T186" s="95">
+        <v>8</v>
+      </c>
+      <c r="U186" s="95">
+        <v>1</v>
       </c>
     </row>
     <row r="187" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A187" s="95">
-        <v>6</v>
-      </c>
-      <c r="B187">
-        <v>2</v>
-      </c>
-      <c r="C187">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="B187" s="95">
+        <v>1</v>
+      </c>
+      <c r="C187" s="95">
+        <v>9</v>
       </c>
       <c r="E187" s="95">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F187" s="95">
         <v>1</v>
       </c>
       <c r="G187" s="95">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H187" s="95">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="J187">
+        <v>9</v>
+      </c>
+      <c r="K187" s="95">
+        <v>14</v>
+      </c>
+      <c r="L187">
+        <v>2</v>
+      </c>
+      <c r="M187" s="95">
+        <v>1</v>
+      </c>
+      <c r="N187">
+        <v>0</v>
+      </c>
+      <c r="O187">
+        <v>20000000</v>
+      </c>
+      <c r="P187">
+        <v>0</v>
+      </c>
+      <c r="S187" s="95">
+        <v>9</v>
+      </c>
+      <c r="T187" s="95">
+        <v>9</v>
+      </c>
+      <c r="U187" s="95">
+        <v>1</v>
       </c>
     </row>
     <row r="188" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A188" s="95">
-        <v>7</v>
-      </c>
-      <c r="B188">
-        <v>2</v>
-      </c>
-      <c r="C188">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="B188" s="95">
+        <v>1</v>
+      </c>
+      <c r="C188" s="95">
+        <v>10</v>
       </c>
       <c r="E188" s="95">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F188" s="95">
         <v>1</v>
       </c>
       <c r="G188" s="95">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H188" s="95">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="J188">
+        <v>10</v>
+      </c>
+      <c r="K188" s="95">
+        <v>14</v>
+      </c>
+      <c r="L188">
+        <v>2</v>
+      </c>
+      <c r="M188" s="95">
+        <v>1</v>
+      </c>
+      <c r="N188">
+        <v>0</v>
+      </c>
+      <c r="O188">
+        <v>10000000</v>
+      </c>
+      <c r="P188">
+        <v>0</v>
+      </c>
+      <c r="S188" s="95">
+        <v>10</v>
+      </c>
+      <c r="T188" s="95">
+        <v>10</v>
+      </c>
+      <c r="U188" s="95">
+        <v>1</v>
       </c>
     </row>
     <row r="189" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A189" s="95">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B189">
         <v>2</v>
@@ -16445,7 +16367,7 @@
         <v>1</v>
       </c>
       <c r="G189" s="95">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H189" s="95">
         <v>2</v>
@@ -16453,7 +16375,7 @@
     </row>
     <row r="190" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A190" s="95">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B190">
         <v>2</v>
@@ -16468,7 +16390,7 @@
         <v>1</v>
       </c>
       <c r="G190" s="95">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H190" s="95">
         <v>2</v>
@@ -16476,126 +16398,189 @@
     </row>
     <row r="191" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A191" s="95">
+        <v>3</v>
+      </c>
+      <c r="B191">
+        <v>2</v>
+      </c>
+      <c r="C191">
+        <v>1</v>
+      </c>
+      <c r="E191" s="95">
+        <v>2</v>
+      </c>
+      <c r="F191" s="95">
+        <v>1</v>
+      </c>
+      <c r="G191" s="95">
+        <v>3</v>
+      </c>
+      <c r="H191" s="95">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="192" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A192" s="95">
+        <v>4</v>
+      </c>
+      <c r="B192">
+        <v>2</v>
+      </c>
+      <c r="C192">
+        <v>1</v>
+      </c>
+      <c r="E192" s="95">
+        <v>2</v>
+      </c>
+      <c r="F192" s="95">
+        <v>1</v>
+      </c>
+      <c r="G192" s="95">
+        <v>4</v>
+      </c>
+      <c r="H192" s="95">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A193" s="95">
+        <v>5</v>
+      </c>
+      <c r="B193">
+        <v>2</v>
+      </c>
+      <c r="C193">
+        <v>1</v>
+      </c>
+      <c r="E193" s="95">
+        <v>2</v>
+      </c>
+      <c r="F193" s="95">
+        <v>1</v>
+      </c>
+      <c r="G193" s="95">
+        <v>5</v>
+      </c>
+      <c r="H193" s="95">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A194" s="95">
+        <v>6</v>
+      </c>
+      <c r="B194">
+        <v>2</v>
+      </c>
+      <c r="C194">
+        <v>1</v>
+      </c>
+      <c r="E194" s="95">
+        <v>2</v>
+      </c>
+      <c r="F194" s="95">
+        <v>1</v>
+      </c>
+      <c r="G194" s="95">
+        <v>6</v>
+      </c>
+      <c r="H194" s="95">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A195" s="95">
+        <v>7</v>
+      </c>
+      <c r="B195">
+        <v>2</v>
+      </c>
+      <c r="C195">
+        <v>1</v>
+      </c>
+      <c r="E195" s="95">
+        <v>2</v>
+      </c>
+      <c r="F195" s="95">
+        <v>1</v>
+      </c>
+      <c r="G195" s="95">
+        <v>7</v>
+      </c>
+      <c r="H195" s="95">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A196" s="95">
+        <v>8</v>
+      </c>
+      <c r="B196">
+        <v>2</v>
+      </c>
+      <c r="C196">
+        <v>1</v>
+      </c>
+      <c r="E196" s="95">
+        <v>2</v>
+      </c>
+      <c r="F196" s="95">
+        <v>1</v>
+      </c>
+      <c r="G196" s="95">
+        <v>8</v>
+      </c>
+      <c r="H196" s="95">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A197" s="95">
+        <v>9</v>
+      </c>
+      <c r="B197">
+        <v>2</v>
+      </c>
+      <c r="C197">
+        <v>1</v>
+      </c>
+      <c r="E197" s="95">
+        <v>2</v>
+      </c>
+      <c r="F197" s="95">
+        <v>1</v>
+      </c>
+      <c r="G197" s="95">
+        <v>9</v>
+      </c>
+      <c r="H197" s="95">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A198" s="95">
         <v>10</v>
       </c>
-      <c r="B191">
-        <v>2</v>
-      </c>
-      <c r="C191">
-        <v>1</v>
-      </c>
-      <c r="E191" s="95">
-        <v>2</v>
-      </c>
-      <c r="F191" s="95">
-        <v>1</v>
-      </c>
-      <c r="G191" s="95">
+      <c r="B198">
+        <v>2</v>
+      </c>
+      <c r="C198">
+        <v>1</v>
+      </c>
+      <c r="E198" s="95">
+        <v>2</v>
+      </c>
+      <c r="F198" s="95">
+        <v>1</v>
+      </c>
+      <c r="G198" s="95">
         <v>10</v>
       </c>
-      <c r="H191" s="95">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="192" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="E192" s="95">
-        <v>3</v>
-      </c>
-      <c r="F192" s="95">
-        <v>1</v>
-      </c>
-      <c r="G192" s="95">
-        <v>1</v>
-      </c>
-      <c r="H192" s="95">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="193" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E193" s="95">
-        <v>3</v>
-      </c>
-      <c r="F193" s="95">
-        <v>1</v>
-      </c>
-      <c r="G193" s="95">
-        <v>2</v>
-      </c>
-      <c r="H193" s="95">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="194" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E194" s="95">
-        <v>3</v>
-      </c>
-      <c r="F194" s="95">
-        <v>1</v>
-      </c>
-      <c r="G194" s="95">
-        <v>3</v>
-      </c>
-      <c r="H194" s="95">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="195" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E195" s="95">
-        <v>3</v>
-      </c>
-      <c r="F195" s="95">
-        <v>1</v>
-      </c>
-      <c r="G195" s="95">
-        <v>4</v>
-      </c>
-      <c r="H195" s="95">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="196" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E196" s="95">
-        <v>3</v>
-      </c>
-      <c r="F196" s="95">
-        <v>1</v>
-      </c>
-      <c r="G196" s="95">
-        <v>5</v>
-      </c>
-      <c r="H196" s="95">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="197" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E197" s="95">
-        <v>3</v>
-      </c>
-      <c r="F197" s="95">
-        <v>1</v>
-      </c>
-      <c r="G197" s="95">
-        <v>6</v>
-      </c>
-      <c r="H197" s="95">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="198" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E198" s="95">
-        <v>3</v>
-      </c>
-      <c r="F198" s="95">
-        <v>1</v>
-      </c>
-      <c r="G198" s="95">
-        <v>7</v>
-      </c>
       <c r="H198" s="95">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="199" spans="5:8" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E199" s="95">
         <v>3</v>
       </c>
@@ -16603,13 +16588,13 @@
         <v>1</v>
       </c>
       <c r="G199" s="95">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H199" s="95">
         <v>3</v>
       </c>
     </row>
-    <row r="200" spans="5:8" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E200" s="95">
         <v>3</v>
       </c>
@@ -16617,13 +16602,13 @@
         <v>1</v>
       </c>
       <c r="G200" s="95">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H200" s="95">
         <v>3</v>
       </c>
     </row>
-    <row r="201" spans="5:8" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E201" s="95">
         <v>3</v>
       </c>
@@ -16631,108 +16616,108 @@
         <v>1</v>
       </c>
       <c r="G201" s="95">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H201" s="95">
         <v>3</v>
       </c>
     </row>
-    <row r="202" spans="5:8" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E202" s="95">
+        <v>3</v>
+      </c>
+      <c r="F202" s="95">
+        <v>1</v>
+      </c>
+      <c r="G202" s="95">
         <v>4</v>
       </c>
-      <c r="F202" s="95">
-        <v>1</v>
-      </c>
-      <c r="G202" s="95">
-        <v>1</v>
-      </c>
       <c r="H202" s="95">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="203" spans="5:8" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E203" s="95">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F203" s="95">
         <v>1</v>
       </c>
       <c r="G203" s="95">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H203" s="95">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="204" spans="5:8" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E204" s="95">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F204" s="95">
         <v>1</v>
       </c>
       <c r="G204" s="95">
+        <v>6</v>
+      </c>
+      <c r="H204" s="95">
         <v>3</v>
       </c>
-      <c r="H204" s="95">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="205" spans="5:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="205" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E205" s="95">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F205" s="95">
         <v>1</v>
       </c>
       <c r="G205" s="95">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H205" s="95">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="206" spans="5:8" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E206" s="95">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F206" s="95">
         <v>1</v>
       </c>
       <c r="G206" s="95">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H206" s="95">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="207" spans="5:8" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E207" s="95">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F207" s="95">
         <v>1</v>
       </c>
       <c r="G207" s="95">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H207" s="95">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="208" spans="5:8" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E208" s="95">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F208" s="95">
         <v>1</v>
       </c>
       <c r="G208" s="95">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H208" s="95">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="209" spans="5:8" x14ac:dyDescent="0.3">
@@ -16743,7 +16728,7 @@
         <v>1</v>
       </c>
       <c r="G209" s="95">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H209" s="95">
         <v>4</v>
@@ -16757,7 +16742,7 @@
         <v>1</v>
       </c>
       <c r="G210" s="95">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H210" s="95">
         <v>4</v>
@@ -16771,7 +16756,7 @@
         <v>1</v>
       </c>
       <c r="G211" s="95">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H211" s="95">
         <v>4</v>
@@ -16779,100 +16764,100 @@
     </row>
     <row r="212" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E212" s="95">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F212" s="95">
         <v>1</v>
       </c>
       <c r="G212" s="95">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H212" s="95">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="213" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E213" s="95">
+        <v>4</v>
+      </c>
+      <c r="F213" s="95">
+        <v>1</v>
+      </c>
+      <c r="G213" s="95">
         <v>5</v>
       </c>
-      <c r="F213" s="95">
-        <v>1</v>
-      </c>
-      <c r="G213" s="95">
-        <v>2</v>
-      </c>
       <c r="H213" s="95">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="214" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E214" s="95">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F214" s="95">
         <v>1</v>
       </c>
       <c r="G214" s="95">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H214" s="95">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="215" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E215" s="95">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F215" s="95">
         <v>1</v>
       </c>
       <c r="G215" s="95">
+        <v>7</v>
+      </c>
+      <c r="H215" s="95">
         <v>4</v>
-      </c>
-      <c r="H215" s="95">
-        <v>5</v>
       </c>
     </row>
     <row r="216" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E216" s="95">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F216" s="95">
         <v>1</v>
       </c>
       <c r="G216" s="95">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H216" s="95">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="217" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E217" s="95">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F217" s="95">
         <v>1</v>
       </c>
       <c r="G217" s="95">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H217" s="95">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="218" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E218" s="95">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F218" s="95">
         <v>1</v>
       </c>
       <c r="G218" s="95">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H218" s="95">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="219" spans="5:8" x14ac:dyDescent="0.3">
@@ -16883,7 +16868,7 @@
         <v>1</v>
       </c>
       <c r="G219" s="95">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H219" s="95">
         <v>5</v>
@@ -16897,7 +16882,7 @@
         <v>1</v>
       </c>
       <c r="G220" s="95">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H220" s="95">
         <v>5</v>
@@ -16911,79 +16896,177 @@
         <v>1</v>
       </c>
       <c r="G221" s="95">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H221" s="95">
         <v>5</v>
       </c>
     </row>
     <row r="222" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E222">
-        <v>1</v>
-      </c>
-      <c r="F222">
-        <v>2</v>
-      </c>
-      <c r="G222">
-        <v>1</v>
-      </c>
-      <c r="H222">
+      <c r="E222" s="95">
+        <v>5</v>
+      </c>
+      <c r="F222" s="95">
+        <v>1</v>
+      </c>
+      <c r="G222" s="95">
+        <v>4</v>
+      </c>
+      <c r="H222" s="95">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="223" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E223" s="95">
+        <v>5</v>
+      </c>
+      <c r="F223" s="95">
+        <v>1</v>
+      </c>
+      <c r="G223" s="95">
+        <v>5</v>
+      </c>
+      <c r="H223" s="95">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="224" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E224" s="95">
+        <v>5</v>
+      </c>
+      <c r="F224" s="95">
+        <v>1</v>
+      </c>
+      <c r="G224" s="95">
         <v>6</v>
       </c>
-    </row>
-    <row r="223" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E223">
-        <v>2</v>
-      </c>
-      <c r="F223">
-        <v>2</v>
-      </c>
-      <c r="G223">
-        <v>1</v>
-      </c>
-      <c r="H223">
+      <c r="H224" s="95">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="225" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E225" s="95">
+        <v>5</v>
+      </c>
+      <c r="F225" s="95">
+        <v>1</v>
+      </c>
+      <c r="G225" s="95">
         <v>7</v>
       </c>
-    </row>
-    <row r="224" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E224">
+      <c r="H225" s="95">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="226" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E226" s="95">
+        <v>5</v>
+      </c>
+      <c r="F226" s="95">
+        <v>1</v>
+      </c>
+      <c r="G226" s="95">
+        <v>8</v>
+      </c>
+      <c r="H226" s="95">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="227" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E227" s="95">
+        <v>5</v>
+      </c>
+      <c r="F227" s="95">
+        <v>1</v>
+      </c>
+      <c r="G227" s="95">
+        <v>9</v>
+      </c>
+      <c r="H227" s="95">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="228" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E228" s="95">
+        <v>5</v>
+      </c>
+      <c r="F228" s="95">
+        <v>1</v>
+      </c>
+      <c r="G228" s="95">
+        <v>10</v>
+      </c>
+      <c r="H228" s="95">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="229" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E229">
+        <v>1</v>
+      </c>
+      <c r="F229">
+        <v>2</v>
+      </c>
+      <c r="G229">
+        <v>1</v>
+      </c>
+      <c r="H229">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="230" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E230">
+        <v>2</v>
+      </c>
+      <c r="F230">
+        <v>2</v>
+      </c>
+      <c r="G230">
+        <v>1</v>
+      </c>
+      <c r="H230">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="231" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E231">
         <v>3</v>
       </c>
-      <c r="F224">
-        <v>2</v>
-      </c>
-      <c r="G224">
-        <v>1</v>
-      </c>
-      <c r="H224">
+      <c r="F231">
+        <v>2</v>
+      </c>
+      <c r="G231">
+        <v>1</v>
+      </c>
+      <c r="H231">
         <v>8</v>
       </c>
     </row>
-    <row r="225" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E225">
+    <row r="232" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E232">
         <v>4</v>
       </c>
-      <c r="F225">
-        <v>2</v>
-      </c>
-      <c r="G225">
-        <v>1</v>
-      </c>
-      <c r="H225">
+      <c r="F232">
+        <v>2</v>
+      </c>
+      <c r="G232">
+        <v>1</v>
+      </c>
+      <c r="H232">
         <v>9</v>
       </c>
     </row>
-    <row r="226" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E226">
+    <row r="233" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E233">
         <v>5</v>
       </c>
-      <c r="F226">
-        <v>2</v>
-      </c>
-      <c r="G226">
-        <v>1</v>
-      </c>
-      <c r="H226">
+      <c r="F233">
+        <v>2</v>
+      </c>
+      <c r="G233">
+        <v>1</v>
+      </c>
+      <c r="H233">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added two iteration version of fm26
</commit_message>
<xml_diff>
--- a/ftest/data/fm24/Worked_Example_Calculation_Net_Loss_Pre_Cat_Simple_Complex_Test_Case_working.xlsx
+++ b/ftest/data/fm24/Worked_Example_Calculation_Net_Loss_Pre_Cat_Simple_Complex_Test_Case_working.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\git\ktest\ftest\data\fm24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{4163ED01-A627-4BC4-9485-9F3F4B5C4221}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{9A0EF08B-7DC8-4AC7-A508-43985020D89A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="-12" windowWidth="18972" windowHeight="5916" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-12" yWindow="-12" windowWidth="18972" windowHeight="5916" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="9" r:id="rId1"/>
@@ -1088,21 +1088,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1131,6 +1116,21 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2926,11 +2926,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U166"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <pane xSplit="4" ySplit="7" topLeftCell="F59" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
+      <pane xSplit="4" ySplit="7" topLeftCell="F65" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="H103" sqref="H103"/>
+      <selection pane="bottomRight" activeCell="K73" sqref="K73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3086,11 +3086,11 @@
       <c r="U7" s="10"/>
     </row>
     <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="117" t="s">
+      <c r="A8" s="112" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="118"/>
-      <c r="C8" s="119"/>
+      <c r="B8" s="113"/>
+      <c r="C8" s="114"/>
       <c r="D8" s="33" t="s">
         <v>38</v>
       </c>
@@ -3155,9 +3155,9 @@
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A9" s="120"/>
-      <c r="B9" s="121"/>
-      <c r="C9" s="122"/>
+      <c r="A9" s="115"/>
+      <c r="B9" s="116"/>
+      <c r="C9" s="117"/>
       <c r="D9" s="33" t="s">
         <v>39</v>
       </c>
@@ -3222,9 +3222,9 @@
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A10" s="120"/>
-      <c r="B10" s="121"/>
-      <c r="C10" s="122"/>
+      <c r="A10" s="115"/>
+      <c r="B10" s="116"/>
+      <c r="C10" s="117"/>
       <c r="D10" s="33" t="s">
         <v>40</v>
       </c>
@@ -3289,9 +3289,9 @@
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A11" s="123"/>
-      <c r="B11" s="124"/>
-      <c r="C11" s="125"/>
+      <c r="A11" s="118"/>
+      <c r="B11" s="119"/>
+      <c r="C11" s="120"/>
       <c r="D11" s="9" t="s">
         <v>37</v>
       </c>
@@ -3376,13 +3376,13 @@
       <c r="U12" s="10"/>
     </row>
     <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="116" t="s">
+      <c r="A13" s="111" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="116" t="s">
+      <c r="B13" s="111" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="116"/>
+      <c r="C13" s="111"/>
       <c r="D13" s="34" t="s">
         <v>49</v>
       </c>
@@ -3425,9 +3425,9 @@
       </c>
     </row>
     <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="116"/>
-      <c r="B14" s="116"/>
-      <c r="C14" s="116"/>
+      <c r="A14" s="111"/>
+      <c r="B14" s="111"/>
+      <c r="C14" s="111"/>
       <c r="D14" s="34" t="s">
         <v>50</v>
       </c>
@@ -3480,9 +3480,9 @@
       <c r="U14" s="40"/>
     </row>
     <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="116"/>
-      <c r="B15" s="116"/>
-      <c r="C15" s="116"/>
+      <c r="A15" s="111"/>
+      <c r="B15" s="111"/>
+      <c r="C15" s="111"/>
       <c r="D15" s="34" t="s">
         <v>51</v>
       </c>
@@ -3535,11 +3535,11 @@
       <c r="U15" s="40"/>
     </row>
     <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="116"/>
-      <c r="B16" s="117" t="s">
+      <c r="A16" s="111"/>
+      <c r="B16" s="112" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="119"/>
+      <c r="C16" s="114"/>
       <c r="D16" s="33" t="s">
         <v>38</v>
       </c>
@@ -3604,9 +3604,9 @@
       </c>
     </row>
     <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="116"/>
-      <c r="B17" s="120"/>
-      <c r="C17" s="122"/>
+      <c r="A17" s="111"/>
+      <c r="B17" s="115"/>
+      <c r="C17" s="117"/>
       <c r="D17" s="33" t="s">
         <v>39</v>
       </c>
@@ -3671,9 +3671,9 @@
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A18" s="116"/>
-      <c r="B18" s="120"/>
-      <c r="C18" s="122"/>
+      <c r="A18" s="111"/>
+      <c r="B18" s="115"/>
+      <c r="C18" s="117"/>
       <c r="D18" s="33" t="s">
         <v>40</v>
       </c>
@@ -3738,9 +3738,9 @@
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A19" s="116"/>
-      <c r="B19" s="123"/>
-      <c r="C19" s="125"/>
+      <c r="A19" s="111"/>
+      <c r="B19" s="118"/>
+      <c r="C19" s="120"/>
       <c r="D19" s="35" t="s">
         <v>47</v>
       </c>
@@ -3845,13 +3845,13 @@
       <c r="U21" s="10"/>
     </row>
     <row r="22" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="116" t="s">
+      <c r="A22" s="111" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="116" t="s">
+      <c r="B22" s="111" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="113" t="s">
+      <c r="C22" s="121" t="s">
         <v>56</v>
       </c>
       <c r="D22" s="9" t="s">
@@ -3906,9 +3906,9 @@
       <c r="U22" s="10"/>
     </row>
     <row r="23" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="116"/>
-      <c r="B23" s="116"/>
-      <c r="C23" s="113"/>
+      <c r="A23" s="111"/>
+      <c r="B23" s="111"/>
+      <c r="C23" s="121"/>
       <c r="D23" s="9" t="s">
         <v>32</v>
       </c>
@@ -3961,9 +3961,9 @@
       <c r="U23" s="10"/>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A24" s="116"/>
-      <c r="B24" s="116"/>
-      <c r="C24" s="113"/>
+      <c r="A24" s="111"/>
+      <c r="B24" s="111"/>
+      <c r="C24" s="121"/>
       <c r="D24" s="9" t="s">
         <v>30</v>
       </c>
@@ -4016,9 +4016,9 @@
       <c r="U24" s="10"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A25" s="116"/>
-      <c r="B25" s="116"/>
-      <c r="C25" s="113"/>
+      <c r="A25" s="111"/>
+      <c r="B25" s="111"/>
+      <c r="C25" s="121"/>
       <c r="D25" s="36" t="s">
         <v>53</v>
       </c>
@@ -4071,9 +4071,9 @@
       <c r="U25" s="10"/>
     </row>
     <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="116"/>
-      <c r="B26" s="116"/>
-      <c r="C26" s="113" t="s">
+      <c r="A26" s="111"/>
+      <c r="B26" s="111"/>
+      <c r="C26" s="121" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="9" t="s">
@@ -4128,9 +4128,9 @@
       <c r="U26" s="10"/>
     </row>
     <row r="27" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="116"/>
-      <c r="B27" s="116"/>
-      <c r="C27" s="113"/>
+      <c r="A27" s="111"/>
+      <c r="B27" s="111"/>
+      <c r="C27" s="121"/>
       <c r="D27" s="36" t="s">
         <v>58</v>
       </c>
@@ -4192,11 +4192,11 @@
       <c r="U27" s="42"/>
     </row>
     <row r="28" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="116"/>
-      <c r="B28" s="116" t="s">
+      <c r="A28" s="111"/>
+      <c r="B28" s="111" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="113" t="s">
+      <c r="C28" s="121" t="s">
         <v>21</v>
       </c>
       <c r="D28" s="9" t="s">
@@ -4230,9 +4230,9 @@
       <c r="U28" s="10"/>
     </row>
     <row r="29" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="116"/>
-      <c r="B29" s="116"/>
-      <c r="C29" s="113"/>
+      <c r="A29" s="111"/>
+      <c r="B29" s="111"/>
+      <c r="C29" s="121"/>
       <c r="D29" s="36" t="s">
         <v>59</v>
       </c>
@@ -4294,9 +4294,9 @@
       <c r="U29" s="10"/>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A30" s="116"/>
-      <c r="B30" s="116"/>
-      <c r="C30" s="113" t="s">
+      <c r="A30" s="111"/>
+      <c r="B30" s="111"/>
+      <c r="C30" s="121" t="s">
         <v>57</v>
       </c>
       <c r="D30" s="9" t="s">
@@ -4330,9 +4330,9 @@
       <c r="U30" s="10"/>
     </row>
     <row r="31" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="116"/>
-      <c r="B31" s="116"/>
-      <c r="C31" s="113"/>
+      <c r="A31" s="111"/>
+      <c r="B31" s="111"/>
+      <c r="C31" s="121"/>
       <c r="D31" s="35" t="s">
         <v>60</v>
       </c>
@@ -4439,13 +4439,13 @@
       <c r="U33" s="10"/>
     </row>
     <row r="34" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="114" t="s">
+      <c r="A34" s="124" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="116" t="s">
+      <c r="B34" s="111" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="113" t="s">
+      <c r="C34" s="121" t="s">
         <v>16</v>
       </c>
       <c r="D34" s="9" t="s">
@@ -4488,9 +4488,9 @@
       <c r="U34" s="10"/>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A35" s="115"/>
-      <c r="B35" s="116"/>
-      <c r="C35" s="113"/>
+      <c r="A35" s="125"/>
+      <c r="B35" s="111"/>
+      <c r="C35" s="121"/>
       <c r="D35" s="9" t="s">
         <v>14</v>
       </c>
@@ -4531,9 +4531,9 @@
       <c r="U35" s="10"/>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A36" s="115"/>
-      <c r="B36" s="116"/>
-      <c r="C36" s="113"/>
+      <c r="A36" s="125"/>
+      <c r="B36" s="111"/>
+      <c r="C36" s="121"/>
       <c r="D36" s="9" t="s">
         <v>36</v>
       </c>
@@ -4574,9 +4574,9 @@
       <c r="U36" s="10"/>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A37" s="115"/>
-      <c r="B37" s="116"/>
-      <c r="C37" s="113"/>
+      <c r="A37" s="125"/>
+      <c r="B37" s="111"/>
+      <c r="C37" s="121"/>
       <c r="D37" s="9" t="s">
         <v>22</v>
       </c>
@@ -4617,9 +4617,9 @@
       <c r="U37" s="10"/>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A38" s="115"/>
-      <c r="B38" s="116"/>
-      <c r="C38" s="113"/>
+      <c r="A38" s="125"/>
+      <c r="B38" s="111"/>
+      <c r="C38" s="121"/>
       <c r="D38" s="48" t="s">
         <v>61</v>
       </c>
@@ -4672,9 +4672,9 @@
       <c r="U38" s="10"/>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A39" s="115"/>
-      <c r="B39" s="116"/>
-      <c r="C39" s="113"/>
+      <c r="A39" s="125"/>
+      <c r="B39" s="111"/>
+      <c r="C39" s="121"/>
       <c r="D39" s="9" t="s">
         <v>21</v>
       </c>
@@ -4715,9 +4715,9 @@
       <c r="U39" s="10"/>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A40" s="115"/>
-      <c r="B40" s="116"/>
-      <c r="C40" s="113"/>
+      <c r="A40" s="125"/>
+      <c r="B40" s="111"/>
+      <c r="C40" s="121"/>
       <c r="D40" s="48" t="s">
         <v>62</v>
       </c>
@@ -4770,9 +4770,9 @@
       <c r="U40" s="10"/>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A41" s="115"/>
-      <c r="B41" s="116"/>
-      <c r="C41" s="113"/>
+      <c r="A41" s="125"/>
+      <c r="B41" s="111"/>
+      <c r="C41" s="121"/>
       <c r="D41" s="9" t="s">
         <v>23</v>
       </c>
@@ -4813,9 +4813,9 @@
       <c r="U41" s="10"/>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A42" s="115"/>
-      <c r="B42" s="116"/>
-      <c r="C42" s="113"/>
+      <c r="A42" s="125"/>
+      <c r="B42" s="111"/>
+      <c r="C42" s="121"/>
       <c r="D42" s="48" t="s">
         <v>63</v>
       </c>
@@ -4868,9 +4868,9 @@
       <c r="U42" s="10"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A43" s="115"/>
-      <c r="B43" s="116"/>
-      <c r="C43" s="113"/>
+      <c r="A43" s="125"/>
+      <c r="B43" s="111"/>
+      <c r="C43" s="121"/>
       <c r="D43" s="9" t="s">
         <v>20</v>
       </c>
@@ -4911,9 +4911,9 @@
       <c r="U43" s="10"/>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A44" s="115"/>
-      <c r="B44" s="116"/>
-      <c r="C44" s="113"/>
+      <c r="A44" s="125"/>
+      <c r="B44" s="111"/>
+      <c r="C44" s="121"/>
       <c r="D44" s="9" t="s">
         <v>24</v>
       </c>
@@ -4954,9 +4954,9 @@
       <c r="U44" s="10"/>
     </row>
     <row r="45" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A45" s="115"/>
-      <c r="B45" s="116"/>
-      <c r="C45" s="113"/>
+      <c r="A45" s="125"/>
+      <c r="B45" s="111"/>
+      <c r="C45" s="121"/>
       <c r="D45" s="49" t="s">
         <v>64</v>
       </c>
@@ -5021,9 +5021,9 @@
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A46" s="115"/>
-      <c r="B46" s="116"/>
-      <c r="C46" s="113"/>
+      <c r="A46" s="125"/>
+      <c r="B46" s="111"/>
+      <c r="C46" s="121"/>
       <c r="D46" s="36" t="s">
         <v>65</v>
       </c>
@@ -5088,11 +5088,11 @@
       </c>
     </row>
     <row r="47" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="115"/>
-      <c r="B47" s="116" t="s">
+      <c r="A47" s="125"/>
+      <c r="B47" s="111" t="s">
         <v>71</v>
       </c>
-      <c r="C47" s="113" t="s">
+      <c r="C47" s="121" t="s">
         <v>15</v>
       </c>
       <c r="D47" s="10"/>
@@ -5115,9 +5115,9 @@
       <c r="U47" s="10"/>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A48" s="115"/>
-      <c r="B48" s="116"/>
-      <c r="C48" s="113"/>
+      <c r="A48" s="125"/>
+      <c r="B48" s="111"/>
+      <c r="C48" s="121"/>
       <c r="D48" s="9" t="s">
         <v>25</v>
       </c>
@@ -5143,9 +5143,9 @@
       <c r="U48" s="10"/>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A49" s="115"/>
-      <c r="B49" s="116"/>
-      <c r="C49" s="113"/>
+      <c r="A49" s="125"/>
+      <c r="B49" s="111"/>
+      <c r="C49" s="121"/>
       <c r="D49" s="9" t="s">
         <v>14</v>
       </c>
@@ -5171,9 +5171,9 @@
       <c r="U49" s="10"/>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A50" s="115"/>
-      <c r="B50" s="116"/>
-      <c r="C50" s="113"/>
+      <c r="A50" s="125"/>
+      <c r="B50" s="111"/>
+      <c r="C50" s="121"/>
       <c r="D50" s="9" t="s">
         <v>36</v>
       </c>
@@ -5199,9 +5199,9 @@
       <c r="U50" s="10"/>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A51" s="115"/>
-      <c r="B51" s="116"/>
-      <c r="C51" s="113"/>
+      <c r="A51" s="125"/>
+      <c r="B51" s="111"/>
+      <c r="C51" s="121"/>
       <c r="D51" s="9" t="s">
         <v>22</v>
       </c>
@@ -5227,9 +5227,9 @@
       <c r="U51" s="10"/>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A52" s="115"/>
-      <c r="B52" s="116"/>
-      <c r="C52" s="113"/>
+      <c r="A52" s="125"/>
+      <c r="B52" s="111"/>
+      <c r="C52" s="121"/>
       <c r="D52" s="48" t="s">
         <v>61</v>
       </c>
@@ -5261,9 +5261,9 @@
       <c r="U52" s="10"/>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A53" s="115"/>
-      <c r="B53" s="116"/>
-      <c r="C53" s="113"/>
+      <c r="A53" s="125"/>
+      <c r="B53" s="111"/>
+      <c r="C53" s="121"/>
       <c r="D53" s="9" t="s">
         <v>21</v>
       </c>
@@ -5289,9 +5289,9 @@
       <c r="U53" s="10"/>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A54" s="115"/>
-      <c r="B54" s="116"/>
-      <c r="C54" s="113"/>
+      <c r="A54" s="125"/>
+      <c r="B54" s="111"/>
+      <c r="C54" s="121"/>
       <c r="D54" s="48" t="s">
         <v>62</v>
       </c>
@@ -5323,9 +5323,9 @@
       <c r="U54" s="10"/>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A55" s="115"/>
-      <c r="B55" s="116"/>
-      <c r="C55" s="113"/>
+      <c r="A55" s="125"/>
+      <c r="B55" s="111"/>
+      <c r="C55" s="121"/>
       <c r="D55" s="9" t="s">
         <v>23</v>
       </c>
@@ -5351,9 +5351,9 @@
       <c r="U55" s="10"/>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A56" s="115"/>
-      <c r="B56" s="116"/>
-      <c r="C56" s="113"/>
+      <c r="A56" s="125"/>
+      <c r="B56" s="111"/>
+      <c r="C56" s="121"/>
       <c r="D56" s="48" t="s">
         <v>63</v>
       </c>
@@ -5385,9 +5385,9 @@
       <c r="U56" s="10"/>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A57" s="115"/>
-      <c r="B57" s="116"/>
-      <c r="C57" s="113"/>
+      <c r="A57" s="125"/>
+      <c r="B57" s="111"/>
+      <c r="C57" s="121"/>
       <c r="D57" s="9" t="s">
         <v>20</v>
       </c>
@@ -5413,9 +5413,9 @@
       <c r="U57" s="10"/>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A58" s="115"/>
-      <c r="B58" s="116"/>
-      <c r="C58" s="113"/>
+      <c r="A58" s="125"/>
+      <c r="B58" s="111"/>
+      <c r="C58" s="121"/>
       <c r="D58" s="9" t="s">
         <v>24</v>
       </c>
@@ -5441,9 +5441,9 @@
       <c r="U58" s="10"/>
     </row>
     <row r="59" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A59" s="115"/>
-      <c r="B59" s="116"/>
-      <c r="C59" s="113"/>
+      <c r="A59" s="125"/>
+      <c r="B59" s="111"/>
+      <c r="C59" s="121"/>
       <c r="D59" s="49" t="s">
         <v>64</v>
       </c>
@@ -5508,9 +5508,9 @@
       </c>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A60" s="115"/>
-      <c r="B60" s="116"/>
-      <c r="C60" s="113"/>
+      <c r="A60" s="125"/>
+      <c r="B60" s="111"/>
+      <c r="C60" s="121"/>
       <c r="D60" s="36" t="s">
         <v>66</v>
       </c>
@@ -5575,13 +5575,13 @@
       </c>
     </row>
     <row r="61" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="114" t="s">
+      <c r="A61" s="124" t="s">
         <v>69</v>
       </c>
-      <c r="B61" s="116" t="s">
+      <c r="B61" s="111" t="s">
         <v>72</v>
       </c>
-      <c r="C61" s="111" t="s">
+      <c r="C61" s="122" t="s">
         <v>73</v>
       </c>
       <c r="D61" s="10"/>
@@ -5604,9 +5604,9 @@
       <c r="U61" s="10"/>
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A62" s="115"/>
-      <c r="B62" s="116"/>
-      <c r="C62" s="112"/>
+      <c r="A62" s="125"/>
+      <c r="B62" s="111"/>
+      <c r="C62" s="123"/>
       <c r="D62" s="9" t="s">
         <v>25</v>
       </c>
@@ -5647,9 +5647,9 @@
       <c r="U62" s="10"/>
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A63" s="115"/>
-      <c r="B63" s="116"/>
-      <c r="C63" s="112"/>
+      <c r="A63" s="125"/>
+      <c r="B63" s="111"/>
+      <c r="C63" s="123"/>
       <c r="D63" s="9" t="s">
         <v>14</v>
       </c>
@@ -5690,9 +5690,9 @@
       <c r="U63" s="10"/>
     </row>
     <row r="64" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A64" s="115"/>
-      <c r="B64" s="116"/>
-      <c r="C64" s="112"/>
+      <c r="A64" s="125"/>
+      <c r="B64" s="111"/>
+      <c r="C64" s="123"/>
       <c r="D64" s="9" t="s">
         <v>36</v>
       </c>
@@ -5733,9 +5733,9 @@
       <c r="U64" s="10"/>
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A65" s="115"/>
-      <c r="B65" s="116"/>
-      <c r="C65" s="112"/>
+      <c r="A65" s="125"/>
+      <c r="B65" s="111"/>
+      <c r="C65" s="123"/>
       <c r="D65" s="9" t="s">
         <v>22</v>
       </c>
@@ -5776,9 +5776,9 @@
       <c r="U65" s="10"/>
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A66" s="115"/>
-      <c r="B66" s="116"/>
-      <c r="C66" s="112"/>
+      <c r="A66" s="125"/>
+      <c r="B66" s="111"/>
+      <c r="C66" s="123"/>
       <c r="D66" s="48" t="s">
         <v>61</v>
       </c>
@@ -5831,9 +5831,9 @@
       <c r="U66" s="10"/>
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A67" s="115"/>
-      <c r="B67" s="116"/>
-      <c r="C67" s="112"/>
+      <c r="A67" s="125"/>
+      <c r="B67" s="111"/>
+      <c r="C67" s="123"/>
       <c r="D67" s="9" t="s">
         <v>21</v>
       </c>
@@ -5874,9 +5874,9 @@
       <c r="U67" s="10"/>
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A68" s="115"/>
-      <c r="B68" s="116"/>
-      <c r="C68" s="112"/>
+      <c r="A68" s="125"/>
+      <c r="B68" s="111"/>
+      <c r="C68" s="123"/>
       <c r="D68" s="48" t="s">
         <v>62</v>
       </c>
@@ -5929,9 +5929,9 @@
       <c r="U68" s="10"/>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A69" s="115"/>
-      <c r="B69" s="116"/>
-      <c r="C69" s="112"/>
+      <c r="A69" s="125"/>
+      <c r="B69" s="111"/>
+      <c r="C69" s="123"/>
       <c r="D69" s="9" t="s">
         <v>23</v>
       </c>
@@ -5972,9 +5972,9 @@
       <c r="U69" s="10"/>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A70" s="115"/>
-      <c r="B70" s="116"/>
-      <c r="C70" s="112"/>
+      <c r="A70" s="125"/>
+      <c r="B70" s="111"/>
+      <c r="C70" s="123"/>
       <c r="D70" s="48" t="s">
         <v>63</v>
       </c>
@@ -6039,9 +6039,9 @@
       </c>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A71" s="115"/>
-      <c r="B71" s="116"/>
-      <c r="C71" s="112"/>
+      <c r="A71" s="125"/>
+      <c r="B71" s="111"/>
+      <c r="C71" s="123"/>
       <c r="D71" s="9" t="s">
         <v>20</v>
       </c>
@@ -6082,9 +6082,9 @@
       <c r="U71" s="10"/>
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A72" s="115"/>
-      <c r="B72" s="116"/>
-      <c r="C72" s="112"/>
+      <c r="A72" s="125"/>
+      <c r="B72" s="111"/>
+      <c r="C72" s="123"/>
       <c r="D72" s="9" t="s">
         <v>24</v>
       </c>
@@ -6110,9 +6110,9 @@
       </c>
     </row>
     <row r="73" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A73" s="115"/>
-      <c r="B73" s="116"/>
-      <c r="C73" s="112"/>
+      <c r="A73" s="125"/>
+      <c r="B73" s="111"/>
+      <c r="C73" s="123"/>
       <c r="D73" s="49" t="s">
         <v>64</v>
       </c>
@@ -6177,9 +6177,9 @@
       </c>
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A74" s="115"/>
-      <c r="B74" s="116"/>
-      <c r="C74" s="113" t="s">
+      <c r="A74" s="125"/>
+      <c r="B74" s="111"/>
+      <c r="C74" s="121" t="s">
         <v>74</v>
       </c>
       <c r="D74" s="10"/>
@@ -6202,9 +6202,9 @@
       <c r="U74" s="10"/>
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A75" s="115"/>
-      <c r="B75" s="116"/>
-      <c r="C75" s="113"/>
+      <c r="A75" s="125"/>
+      <c r="B75" s="111"/>
+      <c r="C75" s="121"/>
       <c r="D75" s="9" t="s">
         <v>25</v>
       </c>
@@ -6239,9 +6239,9 @@
       <c r="U75" s="10"/>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A76" s="115"/>
-      <c r="B76" s="116"/>
-      <c r="C76" s="113"/>
+      <c r="A76" s="125"/>
+      <c r="B76" s="111"/>
+      <c r="C76" s="121"/>
       <c r="D76" s="9" t="s">
         <v>14</v>
       </c>
@@ -6276,9 +6276,9 @@
       <c r="U76" s="10"/>
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A77" s="115"/>
-      <c r="B77" s="116"/>
-      <c r="C77" s="113"/>
+      <c r="A77" s="125"/>
+      <c r="B77" s="111"/>
+      <c r="C77" s="121"/>
       <c r="D77" s="9" t="s">
         <v>36</v>
       </c>
@@ -6313,9 +6313,9 @@
       <c r="U77" s="10"/>
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A78" s="115"/>
-      <c r="B78" s="116"/>
-      <c r="C78" s="113"/>
+      <c r="A78" s="125"/>
+      <c r="B78" s="111"/>
+      <c r="C78" s="121"/>
       <c r="D78" s="9" t="s">
         <v>22</v>
       </c>
@@ -6350,9 +6350,9 @@
       <c r="U78" s="10"/>
     </row>
     <row r="79" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A79" s="115"/>
-      <c r="B79" s="116"/>
-      <c r="C79" s="113"/>
+      <c r="A79" s="125"/>
+      <c r="B79" s="111"/>
+      <c r="C79" s="121"/>
       <c r="D79" s="48" t="s">
         <v>61</v>
       </c>
@@ -6405,9 +6405,9 @@
       <c r="U79" s="10"/>
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A80" s="115"/>
-      <c r="B80" s="116"/>
-      <c r="C80" s="113"/>
+      <c r="A80" s="125"/>
+      <c r="B80" s="111"/>
+      <c r="C80" s="121"/>
       <c r="D80" s="9" t="s">
         <v>21</v>
       </c>
@@ -6442,9 +6442,9 @@
       <c r="U80" s="10"/>
     </row>
     <row r="81" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A81" s="115"/>
-      <c r="B81" s="116"/>
-      <c r="C81" s="113"/>
+      <c r="A81" s="125"/>
+      <c r="B81" s="111"/>
+      <c r="C81" s="121"/>
       <c r="D81" s="48" t="s">
         <v>62</v>
       </c>
@@ -6497,9 +6497,9 @@
       <c r="U81" s="10"/>
     </row>
     <row r="82" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A82" s="115"/>
-      <c r="B82" s="116"/>
-      <c r="C82" s="113"/>
+      <c r="A82" s="125"/>
+      <c r="B82" s="111"/>
+      <c r="C82" s="121"/>
       <c r="D82" s="9" t="s">
         <v>23</v>
       </c>
@@ -6534,9 +6534,9 @@
       <c r="U82" s="10"/>
     </row>
     <row r="83" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A83" s="115"/>
-      <c r="B83" s="116"/>
-      <c r="C83" s="113"/>
+      <c r="A83" s="125"/>
+      <c r="B83" s="111"/>
+      <c r="C83" s="121"/>
       <c r="D83" s="48" t="s">
         <v>63</v>
       </c>
@@ -6601,9 +6601,9 @@
       </c>
     </row>
     <row r="84" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A84" s="115"/>
-      <c r="B84" s="116"/>
-      <c r="C84" s="113"/>
+      <c r="A84" s="125"/>
+      <c r="B84" s="111"/>
+      <c r="C84" s="121"/>
       <c r="D84" s="9" t="s">
         <v>20</v>
       </c>
@@ -6638,9 +6638,9 @@
       <c r="U84" s="10"/>
     </row>
     <row r="85" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A85" s="115"/>
-      <c r="B85" s="116"/>
-      <c r="C85" s="113"/>
+      <c r="A85" s="125"/>
+      <c r="B85" s="111"/>
+      <c r="C85" s="121"/>
       <c r="D85" s="9" t="s">
         <v>24</v>
       </c>
@@ -6666,9 +6666,9 @@
       </c>
     </row>
     <row r="86" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A86" s="115"/>
-      <c r="B86" s="116"/>
-      <c r="C86" s="113"/>
+      <c r="A86" s="125"/>
+      <c r="B86" s="111"/>
+      <c r="C86" s="121"/>
       <c r="D86" s="49" t="s">
         <v>64</v>
       </c>
@@ -6733,9 +6733,9 @@
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A87" s="115"/>
-      <c r="B87" s="116"/>
-      <c r="C87" s="113"/>
+      <c r="A87" s="125"/>
+      <c r="B87" s="111"/>
+      <c r="C87" s="121"/>
       <c r="D87" s="36" t="s">
         <v>68</v>
       </c>
@@ -6800,11 +6800,11 @@
       </c>
     </row>
     <row r="88" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="115"/>
-      <c r="B88" s="116" t="s">
+      <c r="A88" s="125"/>
+      <c r="B88" s="111" t="s">
         <v>75</v>
       </c>
-      <c r="C88" s="111" t="s">
+      <c r="C88" s="122" t="s">
         <v>76</v>
       </c>
       <c r="D88" s="10"/>
@@ -6827,9 +6827,9 @@
       <c r="U88" s="10"/>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A89" s="115"/>
-      <c r="B89" s="116"/>
-      <c r="C89" s="112"/>
+      <c r="A89" s="125"/>
+      <c r="B89" s="111"/>
+      <c r="C89" s="123"/>
       <c r="D89" s="9" t="s">
         <v>25</v>
       </c>
@@ -6882,9 +6882,9 @@
       <c r="U89" s="10"/>
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A90" s="115"/>
-      <c r="B90" s="116"/>
-      <c r="C90" s="112"/>
+      <c r="A90" s="125"/>
+      <c r="B90" s="111"/>
+      <c r="C90" s="123"/>
       <c r="D90" s="9" t="s">
         <v>14</v>
       </c>
@@ -6937,9 +6937,9 @@
       <c r="U90" s="10"/>
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A91" s="115"/>
-      <c r="B91" s="116"/>
-      <c r="C91" s="112"/>
+      <c r="A91" s="125"/>
+      <c r="B91" s="111"/>
+      <c r="C91" s="123"/>
       <c r="D91" s="9" t="s">
         <v>36</v>
       </c>
@@ -6988,9 +6988,9 @@
       <c r="S91" s="61"/>
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A92" s="115"/>
-      <c r="B92" s="116"/>
-      <c r="C92" s="112"/>
+      <c r="A92" s="125"/>
+      <c r="B92" s="111"/>
+      <c r="C92" s="123"/>
       <c r="D92" s="9" t="s">
         <v>22</v>
       </c>
@@ -7039,9 +7039,9 @@
       <c r="S92" s="61"/>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A93" s="115"/>
-      <c r="B93" s="116"/>
-      <c r="C93" s="112"/>
+      <c r="A93" s="125"/>
+      <c r="B93" s="111"/>
+      <c r="C93" s="123"/>
       <c r="D93" s="48" t="s">
         <v>61</v>
       </c>
@@ -7090,9 +7090,9 @@
       <c r="S93" s="10"/>
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A94" s="115"/>
-      <c r="B94" s="116"/>
-      <c r="C94" s="112"/>
+      <c r="A94" s="125"/>
+      <c r="B94" s="111"/>
+      <c r="C94" s="123"/>
       <c r="D94" s="9" t="s">
         <v>21</v>
       </c>
@@ -7141,9 +7141,9 @@
       <c r="S94" s="61"/>
     </row>
     <row r="95" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A95" s="115"/>
-      <c r="B95" s="116"/>
-      <c r="C95" s="112"/>
+      <c r="A95" s="125"/>
+      <c r="B95" s="111"/>
+      <c r="C95" s="123"/>
       <c r="D95" s="48" t="s">
         <v>62</v>
       </c>
@@ -7192,9 +7192,9 @@
       <c r="S95" s="10"/>
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A96" s="115"/>
-      <c r="B96" s="116"/>
-      <c r="C96" s="112"/>
+      <c r="A96" s="125"/>
+      <c r="B96" s="111"/>
+      <c r="C96" s="123"/>
       <c r="D96" s="9" t="s">
         <v>23</v>
       </c>
@@ -7243,9 +7243,9 @@
       <c r="S96" s="61"/>
     </row>
     <row r="97" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A97" s="115"/>
-      <c r="B97" s="116"/>
-      <c r="C97" s="112"/>
+      <c r="A97" s="125"/>
+      <c r="B97" s="111"/>
+      <c r="C97" s="123"/>
       <c r="D97" s="48" t="s">
         <v>63</v>
       </c>
@@ -7307,9 +7307,9 @@
       </c>
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A98" s="115"/>
-      <c r="B98" s="116"/>
-      <c r="C98" s="112"/>
+      <c r="A98" s="125"/>
+      <c r="B98" s="111"/>
+      <c r="C98" s="123"/>
       <c r="D98" s="9" t="s">
         <v>20</v>
       </c>
@@ -7358,9 +7358,9 @@
       <c r="S98" s="61"/>
     </row>
     <row r="99" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A99" s="115"/>
-      <c r="B99" s="116"/>
-      <c r="C99" s="112"/>
+      <c r="A99" s="125"/>
+      <c r="B99" s="111"/>
+      <c r="C99" s="123"/>
       <c r="D99" s="9" t="s">
         <v>24</v>
       </c>
@@ -7383,9 +7383,9 @@
       </c>
     </row>
     <row r="100" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A100" s="115"/>
-      <c r="B100" s="116"/>
-      <c r="C100" s="112"/>
+      <c r="A100" s="125"/>
+      <c r="B100" s="111"/>
+      <c r="C100" s="123"/>
       <c r="D100" s="49" t="s">
         <v>64</v>
       </c>
@@ -7450,9 +7450,9 @@
       </c>
     </row>
     <row r="101" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A101" s="115"/>
-      <c r="B101" s="116"/>
-      <c r="C101" s="111" t="s">
+      <c r="A101" s="125"/>
+      <c r="B101" s="111"/>
+      <c r="C101" s="122" t="s">
         <v>77</v>
       </c>
       <c r="I101" s="10"/>
@@ -7464,9 +7464,9 @@
       <c r="U101" s="10"/>
     </row>
     <row r="102" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A102" s="115"/>
-      <c r="B102" s="116"/>
-      <c r="C102" s="112"/>
+      <c r="A102" s="125"/>
+      <c r="B102" s="111"/>
+      <c r="C102" s="123"/>
       <c r="D102" s="9" t="s">
         <v>25</v>
       </c>
@@ -7519,9 +7519,9 @@
       <c r="U102" s="10"/>
     </row>
     <row r="103" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A103" s="115"/>
-      <c r="B103" s="116"/>
-      <c r="C103" s="112"/>
+      <c r="A103" s="125"/>
+      <c r="B103" s="111"/>
+      <c r="C103" s="123"/>
       <c r="D103" s="9" t="s">
         <v>14</v>
       </c>
@@ -7574,9 +7574,9 @@
       <c r="U103" s="10"/>
     </row>
     <row r="104" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A104" s="115"/>
-      <c r="B104" s="116"/>
-      <c r="C104" s="112"/>
+      <c r="A104" s="125"/>
+      <c r="B104" s="111"/>
+      <c r="C104" s="123"/>
       <c r="D104" s="9" t="s">
         <v>36</v>
       </c>
@@ -7625,9 +7625,9 @@
       <c r="S104" s="61"/>
     </row>
     <row r="105" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A105" s="115"/>
-      <c r="B105" s="116"/>
-      <c r="C105" s="112"/>
+      <c r="A105" s="125"/>
+      <c r="B105" s="111"/>
+      <c r="C105" s="123"/>
       <c r="D105" s="9" t="s">
         <v>22</v>
       </c>
@@ -7676,9 +7676,9 @@
       <c r="S105" s="61"/>
     </row>
     <row r="106" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A106" s="115"/>
-      <c r="B106" s="116"/>
-      <c r="C106" s="112"/>
+      <c r="A106" s="125"/>
+      <c r="B106" s="111"/>
+      <c r="C106" s="123"/>
       <c r="D106" s="48" t="s">
         <v>61</v>
       </c>
@@ -7727,9 +7727,9 @@
       <c r="S106" s="10"/>
     </row>
     <row r="107" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A107" s="115"/>
-      <c r="B107" s="116"/>
-      <c r="C107" s="112"/>
+      <c r="A107" s="125"/>
+      <c r="B107" s="111"/>
+      <c r="C107" s="123"/>
       <c r="D107" s="9" t="s">
         <v>21</v>
       </c>
@@ -7778,9 +7778,9 @@
       <c r="S107" s="61"/>
     </row>
     <row r="108" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A108" s="115"/>
-      <c r="B108" s="116"/>
-      <c r="C108" s="112"/>
+      <c r="A108" s="125"/>
+      <c r="B108" s="111"/>
+      <c r="C108" s="123"/>
       <c r="D108" s="48" t="s">
         <v>62</v>
       </c>
@@ -7829,9 +7829,9 @@
       <c r="S108" s="10"/>
     </row>
     <row r="109" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A109" s="115"/>
-      <c r="B109" s="116"/>
-      <c r="C109" s="112"/>
+      <c r="A109" s="125"/>
+      <c r="B109" s="111"/>
+      <c r="C109" s="123"/>
       <c r="D109" s="9" t="s">
         <v>23</v>
       </c>
@@ -7880,9 +7880,9 @@
       <c r="S109" s="61"/>
     </row>
     <row r="110" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A110" s="115"/>
-      <c r="B110" s="116"/>
-      <c r="C110" s="112"/>
+      <c r="A110" s="125"/>
+      <c r="B110" s="111"/>
+      <c r="C110" s="123"/>
       <c r="D110" s="48" t="s">
         <v>63</v>
       </c>
@@ -7944,9 +7944,9 @@
       </c>
     </row>
     <row r="111" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A111" s="115"/>
-      <c r="B111" s="116"/>
-      <c r="C111" s="112"/>
+      <c r="A111" s="125"/>
+      <c r="B111" s="111"/>
+      <c r="C111" s="123"/>
       <c r="D111" s="9" t="s">
         <v>20</v>
       </c>
@@ -7995,9 +7995,9 @@
       <c r="S111" s="61"/>
     </row>
     <row r="112" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A112" s="115"/>
-      <c r="B112" s="116"/>
-      <c r="C112" s="112"/>
+      <c r="A112" s="125"/>
+      <c r="B112" s="111"/>
+      <c r="C112" s="123"/>
       <c r="D112" s="9" t="s">
         <v>24</v>
       </c>
@@ -8020,9 +8020,9 @@
       </c>
     </row>
     <row r="113" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A113" s="115"/>
-      <c r="B113" s="116"/>
-      <c r="C113" s="112"/>
+      <c r="A113" s="125"/>
+      <c r="B113" s="111"/>
+      <c r="C113" s="123"/>
       <c r="D113" s="49" t="s">
         <v>64</v>
       </c>
@@ -8087,11 +8087,11 @@
       </c>
     </row>
     <row r="114" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="114" t="s">
+      <c r="A114" s="124" t="s">
         <v>69</v>
       </c>
-      <c r="B114" s="116"/>
-      <c r="C114" s="111" t="s">
+      <c r="B114" s="111"/>
+      <c r="C114" s="122" t="s">
         <v>78</v>
       </c>
       <c r="I114" s="10"/>
@@ -8103,9 +8103,9 @@
       <c r="U114" s="10"/>
     </row>
     <row r="115" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A115" s="115"/>
-      <c r="B115" s="116"/>
-      <c r="C115" s="112"/>
+      <c r="A115" s="125"/>
+      <c r="B115" s="111"/>
+      <c r="C115" s="123"/>
       <c r="D115" s="9" t="s">
         <v>25</v>
       </c>
@@ -8158,9 +8158,9 @@
       <c r="U115" s="10"/>
     </row>
     <row r="116" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A116" s="115"/>
-      <c r="B116" s="116"/>
-      <c r="C116" s="112"/>
+      <c r="A116" s="125"/>
+      <c r="B116" s="111"/>
+      <c r="C116" s="123"/>
       <c r="D116" s="9" t="s">
         <v>14</v>
       </c>
@@ -8213,9 +8213,9 @@
       <c r="U116" s="10"/>
     </row>
     <row r="117" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A117" s="115"/>
-      <c r="B117" s="116"/>
-      <c r="C117" s="112"/>
+      <c r="A117" s="125"/>
+      <c r="B117" s="111"/>
+      <c r="C117" s="123"/>
       <c r="D117" s="9" t="s">
         <v>36</v>
       </c>
@@ -8264,9 +8264,9 @@
       <c r="S117" s="61"/>
     </row>
     <row r="118" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A118" s="115"/>
-      <c r="B118" s="116"/>
-      <c r="C118" s="112"/>
+      <c r="A118" s="125"/>
+      <c r="B118" s="111"/>
+      <c r="C118" s="123"/>
       <c r="D118" s="9" t="s">
         <v>22</v>
       </c>
@@ -8315,9 +8315,9 @@
       <c r="S118" s="61"/>
     </row>
     <row r="119" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A119" s="115"/>
-      <c r="B119" s="116"/>
-      <c r="C119" s="112"/>
+      <c r="A119" s="125"/>
+      <c r="B119" s="111"/>
+      <c r="C119" s="123"/>
       <c r="D119" s="48" t="s">
         <v>61</v>
       </c>
@@ -8366,9 +8366,9 @@
       <c r="S119" s="10"/>
     </row>
     <row r="120" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A120" s="115"/>
-      <c r="B120" s="116"/>
-      <c r="C120" s="112"/>
+      <c r="A120" s="125"/>
+      <c r="B120" s="111"/>
+      <c r="C120" s="123"/>
       <c r="D120" s="9" t="s">
         <v>21</v>
       </c>
@@ -8417,9 +8417,9 @@
       <c r="S120" s="61"/>
     </row>
     <row r="121" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A121" s="115"/>
-      <c r="B121" s="116"/>
-      <c r="C121" s="112"/>
+      <c r="A121" s="125"/>
+      <c r="B121" s="111"/>
+      <c r="C121" s="123"/>
       <c r="D121" s="48" t="s">
         <v>62</v>
       </c>
@@ -8468,9 +8468,9 @@
       <c r="S121" s="10"/>
     </row>
     <row r="122" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A122" s="115"/>
-      <c r="B122" s="116"/>
-      <c r="C122" s="112"/>
+      <c r="A122" s="125"/>
+      <c r="B122" s="111"/>
+      <c r="C122" s="123"/>
       <c r="D122" s="9" t="s">
         <v>23</v>
       </c>
@@ -8519,9 +8519,9 @@
       <c r="S122" s="61"/>
     </row>
     <row r="123" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A123" s="115"/>
-      <c r="B123" s="116"/>
-      <c r="C123" s="112"/>
+      <c r="A123" s="125"/>
+      <c r="B123" s="111"/>
+      <c r="C123" s="123"/>
       <c r="D123" s="48" t="s">
         <v>63</v>
       </c>
@@ -8583,9 +8583,9 @@
       </c>
     </row>
     <row r="124" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A124" s="115"/>
-      <c r="B124" s="116"/>
-      <c r="C124" s="112"/>
+      <c r="A124" s="125"/>
+      <c r="B124" s="111"/>
+      <c r="C124" s="123"/>
       <c r="D124" s="9" t="s">
         <v>20</v>
       </c>
@@ -8634,9 +8634,9 @@
       <c r="S124" s="61"/>
     </row>
     <row r="125" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A125" s="115"/>
-      <c r="B125" s="116"/>
-      <c r="C125" s="112"/>
+      <c r="A125" s="125"/>
+      <c r="B125" s="111"/>
+      <c r="C125" s="123"/>
       <c r="D125" s="9" t="s">
         <v>24</v>
       </c>
@@ -8659,9 +8659,9 @@
       </c>
     </row>
     <row r="126" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A126" s="115"/>
-      <c r="B126" s="116"/>
-      <c r="C126" s="112"/>
+      <c r="A126" s="125"/>
+      <c r="B126" s="111"/>
+      <c r="C126" s="123"/>
       <c r="D126" s="49" t="s">
         <v>64</v>
       </c>
@@ -8726,9 +8726,9 @@
       </c>
     </row>
     <row r="127" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A127" s="115"/>
-      <c r="B127" s="116"/>
-      <c r="C127" s="111" t="s">
+      <c r="A127" s="125"/>
+      <c r="B127" s="111"/>
+      <c r="C127" s="122" t="s">
         <v>79</v>
       </c>
       <c r="I127" s="10"/>
@@ -8740,9 +8740,9 @@
       <c r="U127" s="10"/>
     </row>
     <row r="128" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A128" s="115"/>
-      <c r="B128" s="116"/>
-      <c r="C128" s="112"/>
+      <c r="A128" s="125"/>
+      <c r="B128" s="111"/>
+      <c r="C128" s="123"/>
       <c r="D128" s="9" t="s">
         <v>25</v>
       </c>
@@ -8795,9 +8795,9 @@
       <c r="U128" s="10"/>
     </row>
     <row r="129" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A129" s="115"/>
-      <c r="B129" s="116"/>
-      <c r="C129" s="112"/>
+      <c r="A129" s="125"/>
+      <c r="B129" s="111"/>
+      <c r="C129" s="123"/>
       <c r="D129" s="9" t="s">
         <v>14</v>
       </c>
@@ -8850,9 +8850,9 @@
       <c r="U129" s="10"/>
     </row>
     <row r="130" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A130" s="115"/>
-      <c r="B130" s="116"/>
-      <c r="C130" s="112"/>
+      <c r="A130" s="125"/>
+      <c r="B130" s="111"/>
+      <c r="C130" s="123"/>
       <c r="D130" s="9" t="s">
         <v>36</v>
       </c>
@@ -8901,9 +8901,9 @@
       <c r="S130" s="61"/>
     </row>
     <row r="131" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A131" s="115"/>
-      <c r="B131" s="116"/>
-      <c r="C131" s="112"/>
+      <c r="A131" s="125"/>
+      <c r="B131" s="111"/>
+      <c r="C131" s="123"/>
       <c r="D131" s="9" t="s">
         <v>22</v>
       </c>
@@ -8952,9 +8952,9 @@
       <c r="S131" s="61"/>
     </row>
     <row r="132" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A132" s="115"/>
-      <c r="B132" s="116"/>
-      <c r="C132" s="112"/>
+      <c r="A132" s="125"/>
+      <c r="B132" s="111"/>
+      <c r="C132" s="123"/>
       <c r="D132" s="48" t="s">
         <v>61</v>
       </c>
@@ -9003,9 +9003,9 @@
       <c r="S132" s="10"/>
     </row>
     <row r="133" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A133" s="115"/>
-      <c r="B133" s="116"/>
-      <c r="C133" s="112"/>
+      <c r="A133" s="125"/>
+      <c r="B133" s="111"/>
+      <c r="C133" s="123"/>
       <c r="D133" s="9" t="s">
         <v>21</v>
       </c>
@@ -9054,9 +9054,9 @@
       <c r="S133" s="61"/>
     </row>
     <row r="134" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A134" s="115"/>
-      <c r="B134" s="116"/>
-      <c r="C134" s="112"/>
+      <c r="A134" s="125"/>
+      <c r="B134" s="111"/>
+      <c r="C134" s="123"/>
       <c r="D134" s="48" t="s">
         <v>62</v>
       </c>
@@ -9105,9 +9105,9 @@
       <c r="S134" s="10"/>
     </row>
     <row r="135" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A135" s="115"/>
-      <c r="B135" s="116"/>
-      <c r="C135" s="112"/>
+      <c r="A135" s="125"/>
+      <c r="B135" s="111"/>
+      <c r="C135" s="123"/>
       <c r="D135" s="9" t="s">
         <v>23</v>
       </c>
@@ -9156,9 +9156,9 @@
       <c r="S135" s="61"/>
     </row>
     <row r="136" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A136" s="115"/>
-      <c r="B136" s="116"/>
-      <c r="C136" s="112"/>
+      <c r="A136" s="125"/>
+      <c r="B136" s="111"/>
+      <c r="C136" s="123"/>
       <c r="D136" s="48" t="s">
         <v>63</v>
       </c>
@@ -9220,9 +9220,9 @@
       </c>
     </row>
     <row r="137" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A137" s="115"/>
-      <c r="B137" s="116"/>
-      <c r="C137" s="112"/>
+      <c r="A137" s="125"/>
+      <c r="B137" s="111"/>
+      <c r="C137" s="123"/>
       <c r="D137" s="9" t="s">
         <v>20</v>
       </c>
@@ -9271,9 +9271,9 @@
       <c r="S137" s="61"/>
     </row>
     <row r="138" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A138" s="115"/>
-      <c r="B138" s="116"/>
-      <c r="C138" s="112"/>
+      <c r="A138" s="125"/>
+      <c r="B138" s="111"/>
+      <c r="C138" s="123"/>
       <c r="D138" s="9" t="s">
         <v>24</v>
       </c>
@@ -9296,9 +9296,9 @@
       </c>
     </row>
     <row r="139" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A139" s="115"/>
-      <c r="B139" s="116"/>
-      <c r="C139" s="112"/>
+      <c r="A139" s="125"/>
+      <c r="B139" s="111"/>
+      <c r="C139" s="123"/>
       <c r="D139" s="49" t="s">
         <v>64</v>
       </c>
@@ -9363,9 +9363,9 @@
       </c>
     </row>
     <row r="140" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A140" s="115"/>
-      <c r="B140" s="116"/>
-      <c r="C140" s="113" t="s">
+      <c r="A140" s="125"/>
+      <c r="B140" s="111"/>
+      <c r="C140" s="121" t="s">
         <v>80</v>
       </c>
       <c r="I140" s="10"/>
@@ -9377,9 +9377,9 @@
       <c r="U140" s="10"/>
     </row>
     <row r="141" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A141" s="115"/>
-      <c r="B141" s="116"/>
-      <c r="C141" s="113"/>
+      <c r="A141" s="125"/>
+      <c r="B141" s="111"/>
+      <c r="C141" s="121"/>
       <c r="D141" s="9" t="s">
         <v>25</v>
       </c>
@@ -9432,9 +9432,9 @@
       <c r="U141" s="10"/>
     </row>
     <row r="142" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A142" s="115"/>
-      <c r="B142" s="116"/>
-      <c r="C142" s="113"/>
+      <c r="A142" s="125"/>
+      <c r="B142" s="111"/>
+      <c r="C142" s="121"/>
       <c r="D142" s="9" t="s">
         <v>14</v>
       </c>
@@ -9487,9 +9487,9 @@
       <c r="U142" s="10"/>
     </row>
     <row r="143" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A143" s="115"/>
-      <c r="B143" s="116"/>
-      <c r="C143" s="113"/>
+      <c r="A143" s="125"/>
+      <c r="B143" s="111"/>
+      <c r="C143" s="121"/>
       <c r="D143" s="9" t="s">
         <v>36</v>
       </c>
@@ -9538,9 +9538,9 @@
       <c r="S143" s="61"/>
     </row>
     <row r="144" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A144" s="115"/>
-      <c r="B144" s="116"/>
-      <c r="C144" s="113"/>
+      <c r="A144" s="125"/>
+      <c r="B144" s="111"/>
+      <c r="C144" s="121"/>
       <c r="D144" s="9" t="s">
         <v>22</v>
       </c>
@@ -9589,9 +9589,9 @@
       <c r="S144" s="61"/>
     </row>
     <row r="145" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A145" s="115"/>
-      <c r="B145" s="116"/>
-      <c r="C145" s="113"/>
+      <c r="A145" s="125"/>
+      <c r="B145" s="111"/>
+      <c r="C145" s="121"/>
       <c r="D145" s="48" t="s">
         <v>61</v>
       </c>
@@ -9640,9 +9640,9 @@
       <c r="S145" s="10"/>
     </row>
     <row r="146" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A146" s="115"/>
-      <c r="B146" s="116"/>
-      <c r="C146" s="113"/>
+      <c r="A146" s="125"/>
+      <c r="B146" s="111"/>
+      <c r="C146" s="121"/>
       <c r="D146" s="9" t="s">
         <v>21</v>
       </c>
@@ -9691,9 +9691,9 @@
       <c r="S146" s="61"/>
     </row>
     <row r="147" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A147" s="115"/>
-      <c r="B147" s="116"/>
-      <c r="C147" s="113"/>
+      <c r="A147" s="125"/>
+      <c r="B147" s="111"/>
+      <c r="C147" s="121"/>
       <c r="D147" s="48" t="s">
         <v>62</v>
       </c>
@@ -9742,9 +9742,9 @@
       <c r="S147" s="10"/>
     </row>
     <row r="148" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A148" s="115"/>
-      <c r="B148" s="116"/>
-      <c r="C148" s="113"/>
+      <c r="A148" s="125"/>
+      <c r="B148" s="111"/>
+      <c r="C148" s="121"/>
       <c r="D148" s="9" t="s">
         <v>23</v>
       </c>
@@ -9793,9 +9793,9 @@
       <c r="S148" s="61"/>
     </row>
     <row r="149" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A149" s="115"/>
-      <c r="B149" s="116"/>
-      <c r="C149" s="113"/>
+      <c r="A149" s="125"/>
+      <c r="B149" s="111"/>
+      <c r="C149" s="121"/>
       <c r="D149" s="48" t="s">
         <v>63</v>
       </c>
@@ -9857,9 +9857,9 @@
       </c>
     </row>
     <row r="150" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A150" s="115"/>
-      <c r="B150" s="116"/>
-      <c r="C150" s="113"/>
+      <c r="A150" s="125"/>
+      <c r="B150" s="111"/>
+      <c r="C150" s="121"/>
       <c r="D150" s="9" t="s">
         <v>20</v>
       </c>
@@ -9908,9 +9908,9 @@
       <c r="S150" s="61"/>
     </row>
     <row r="151" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A151" s="115"/>
-      <c r="B151" s="116"/>
-      <c r="C151" s="113"/>
+      <c r="A151" s="125"/>
+      <c r="B151" s="111"/>
+      <c r="C151" s="121"/>
       <c r="D151" s="9" t="s">
         <v>24</v>
       </c>
@@ -9933,9 +9933,9 @@
       </c>
     </row>
     <row r="152" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A152" s="115"/>
-      <c r="B152" s="116"/>
-      <c r="C152" s="113"/>
+      <c r="A152" s="125"/>
+      <c r="B152" s="111"/>
+      <c r="C152" s="121"/>
       <c r="D152" s="49" t="s">
         <v>64</v>
       </c>
@@ -10000,9 +10000,9 @@
       </c>
     </row>
     <row r="153" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A153" s="115"/>
-      <c r="B153" s="116"/>
-      <c r="C153" s="113"/>
+      <c r="A153" s="125"/>
+      <c r="B153" s="111"/>
+      <c r="C153" s="121"/>
       <c r="D153" s="52" t="s">
         <v>67</v>
       </c>
@@ -10104,17 +10104,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A22:A31"/>
-    <mergeCell ref="A8:C11"/>
-    <mergeCell ref="B13:C15"/>
-    <mergeCell ref="B22:B27"/>
-    <mergeCell ref="A13:A19"/>
-    <mergeCell ref="B16:C19"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C30:C31"/>
     <mergeCell ref="C127:C139"/>
     <mergeCell ref="C140:C153"/>
     <mergeCell ref="A34:A60"/>
@@ -10131,6 +10120,17 @@
     <mergeCell ref="C34:C46"/>
     <mergeCell ref="B47:B60"/>
     <mergeCell ref="C47:C60"/>
+    <mergeCell ref="A22:A31"/>
+    <mergeCell ref="A8:C11"/>
+    <mergeCell ref="B13:C15"/>
+    <mergeCell ref="B22:B27"/>
+    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="B16:C19"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C30:C31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="58" fitToHeight="5" orientation="landscape" r:id="rId1"/>
@@ -10146,8 +10146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Y233"/>
   <sheetViews>
-    <sheetView topLeftCell="A167" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q190" sqref="Q190"/>
+    <sheetView tabSelected="1" topLeftCell="A140" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L147" sqref="L147:L154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14984,7 +14984,7 @@
         <v>14</v>
       </c>
       <c r="L147">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M147">
         <v>1</v>
@@ -15036,8 +15036,8 @@
       <c r="K148">
         <v>2</v>
       </c>
-      <c r="L148">
-        <v>2</v>
+      <c r="L148" s="95">
+        <v>0</v>
       </c>
       <c r="M148">
         <v>1</v>
@@ -15089,8 +15089,8 @@
       <c r="K149">
         <v>2</v>
       </c>
-      <c r="L149">
-        <v>2</v>
+      <c r="L149" s="95">
+        <v>0</v>
       </c>
       <c r="M149">
         <v>1</v>
@@ -15142,8 +15142,8 @@
       <c r="K150">
         <v>2</v>
       </c>
-      <c r="L150">
-        <v>2</v>
+      <c r="L150" s="95">
+        <v>0</v>
       </c>
       <c r="M150">
         <v>1</v>
@@ -15195,8 +15195,8 @@
       <c r="K151">
         <v>2</v>
       </c>
-      <c r="L151">
-        <v>2</v>
+      <c r="L151" s="95">
+        <v>0</v>
       </c>
       <c r="M151">
         <v>1</v>
@@ -15248,8 +15248,8 @@
       <c r="K152">
         <v>2</v>
       </c>
-      <c r="L152">
-        <v>2</v>
+      <c r="L152" s="95">
+        <v>0</v>
       </c>
       <c r="M152">
         <v>1</v>
@@ -15302,7 +15302,7 @@
         <v>2</v>
       </c>
       <c r="L153" s="95">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M153" s="95">
         <v>1</v>
@@ -15355,7 +15355,7 @@
         <v>2</v>
       </c>
       <c r="L154" s="95">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M154" s="95">
         <v>1</v>

</xml_diff>

<commit_message>
new reinsurance test case
</commit_message>
<xml_diff>
--- a/ftest/data/fm24/Worked_Example_Calculation_Net_Loss_Pre_Cat_Simple_Complex_Test_Case_working.xlsx
+++ b/ftest/data/fm24/Worked_Example_Calculation_Net_Loss_Pre_Cat_Simple_Complex_Test_Case_working.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\git\ktest2\ftest\data\fm24\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\git\ktest\ftest\data\fm24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D4BA14A3-7D9F-4B55-AFC0-97D1F8A2248E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7DA8A3C9-5850-45AB-AFB1-3AB13F0387EC}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="-12" windowWidth="18972" windowHeight="5916" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-12" yWindow="-12" windowWidth="18972" windowHeight="5916" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="9" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="146">
   <si>
     <t>Policy Limit</t>
   </si>
@@ -1097,21 +1097,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1140,6 +1125,21 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2935,7 +2935,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U166"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
+    <sheetView zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
       <pane xSplit="4" ySplit="7" topLeftCell="E11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
@@ -3095,11 +3095,11 @@
       <c r="U7" s="10"/>
     </row>
     <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="117" t="s">
+      <c r="A8" s="112" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="118"/>
-      <c r="C8" s="119"/>
+      <c r="B8" s="113"/>
+      <c r="C8" s="114"/>
       <c r="D8" s="33" t="s">
         <v>38</v>
       </c>
@@ -3164,9 +3164,9 @@
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A9" s="120"/>
-      <c r="B9" s="121"/>
-      <c r="C9" s="122"/>
+      <c r="A9" s="115"/>
+      <c r="B9" s="116"/>
+      <c r="C9" s="117"/>
       <c r="D9" s="33" t="s">
         <v>39</v>
       </c>
@@ -3231,9 +3231,9 @@
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A10" s="120"/>
-      <c r="B10" s="121"/>
-      <c r="C10" s="122"/>
+      <c r="A10" s="115"/>
+      <c r="B10" s="116"/>
+      <c r="C10" s="117"/>
       <c r="D10" s="33" t="s">
         <v>40</v>
       </c>
@@ -3298,9 +3298,9 @@
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A11" s="123"/>
-      <c r="B11" s="124"/>
-      <c r="C11" s="125"/>
+      <c r="A11" s="118"/>
+      <c r="B11" s="119"/>
+      <c r="C11" s="120"/>
       <c r="D11" s="9" t="s">
         <v>37</v>
       </c>
@@ -3385,13 +3385,13 @@
       <c r="U12" s="10"/>
     </row>
     <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="116" t="s">
+      <c r="A13" s="111" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="116" t="s">
+      <c r="B13" s="111" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="116"/>
+      <c r="C13" s="111"/>
       <c r="D13" s="34" t="s">
         <v>49</v>
       </c>
@@ -3434,9 +3434,9 @@
       </c>
     </row>
     <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="116"/>
-      <c r="B14" s="116"/>
-      <c r="C14" s="116"/>
+      <c r="A14" s="111"/>
+      <c r="B14" s="111"/>
+      <c r="C14" s="111"/>
       <c r="D14" s="34" t="s">
         <v>50</v>
       </c>
@@ -3489,9 +3489,9 @@
       <c r="U14" s="40"/>
     </row>
     <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="116"/>
-      <c r="B15" s="116"/>
-      <c r="C15" s="116"/>
+      <c r="A15" s="111"/>
+      <c r="B15" s="111"/>
+      <c r="C15" s="111"/>
       <c r="D15" s="34" t="s">
         <v>51</v>
       </c>
@@ -3544,11 +3544,11 @@
       <c r="U15" s="40"/>
     </row>
     <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="116"/>
-      <c r="B16" s="117" t="s">
+      <c r="A16" s="111"/>
+      <c r="B16" s="112" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="119"/>
+      <c r="C16" s="114"/>
       <c r="D16" s="33" t="s">
         <v>38</v>
       </c>
@@ -3613,9 +3613,9 @@
       </c>
     </row>
     <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="116"/>
-      <c r="B17" s="120"/>
-      <c r="C17" s="122"/>
+      <c r="A17" s="111"/>
+      <c r="B17" s="115"/>
+      <c r="C17" s="117"/>
       <c r="D17" s="33" t="s">
         <v>39</v>
       </c>
@@ -3680,9 +3680,9 @@
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A18" s="116"/>
-      <c r="B18" s="120"/>
-      <c r="C18" s="122"/>
+      <c r="A18" s="111"/>
+      <c r="B18" s="115"/>
+      <c r="C18" s="117"/>
       <c r="D18" s="33" t="s">
         <v>40</v>
       </c>
@@ -3747,9 +3747,9 @@
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A19" s="116"/>
-      <c r="B19" s="123"/>
-      <c r="C19" s="125"/>
+      <c r="A19" s="111"/>
+      <c r="B19" s="118"/>
+      <c r="C19" s="120"/>
       <c r="D19" s="35" t="s">
         <v>47</v>
       </c>
@@ -3854,13 +3854,13 @@
       <c r="U21" s="10"/>
     </row>
     <row r="22" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="116" t="s">
+      <c r="A22" s="111" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="116" t="s">
+      <c r="B22" s="111" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="113" t="s">
+      <c r="C22" s="121" t="s">
         <v>56</v>
       </c>
       <c r="D22" s="9" t="s">
@@ -3915,9 +3915,9 @@
       <c r="U22" s="10"/>
     </row>
     <row r="23" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="116"/>
-      <c r="B23" s="116"/>
-      <c r="C23" s="113"/>
+      <c r="A23" s="111"/>
+      <c r="B23" s="111"/>
+      <c r="C23" s="121"/>
       <c r="D23" s="9" t="s">
         <v>32</v>
       </c>
@@ -3970,9 +3970,9 @@
       <c r="U23" s="10"/>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A24" s="116"/>
-      <c r="B24" s="116"/>
-      <c r="C24" s="113"/>
+      <c r="A24" s="111"/>
+      <c r="B24" s="111"/>
+      <c r="C24" s="121"/>
       <c r="D24" s="9" t="s">
         <v>30</v>
       </c>
@@ -4025,9 +4025,9 @@
       <c r="U24" s="10"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A25" s="116"/>
-      <c r="B25" s="116"/>
-      <c r="C25" s="113"/>
+      <c r="A25" s="111"/>
+      <c r="B25" s="111"/>
+      <c r="C25" s="121"/>
       <c r="D25" s="36" t="s">
         <v>53</v>
       </c>
@@ -4080,9 +4080,9 @@
       <c r="U25" s="10"/>
     </row>
     <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="116"/>
-      <c r="B26" s="116"/>
-      <c r="C26" s="113" t="s">
+      <c r="A26" s="111"/>
+      <c r="B26" s="111"/>
+      <c r="C26" s="121" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="9" t="s">
@@ -4137,9 +4137,9 @@
       <c r="U26" s="10"/>
     </row>
     <row r="27" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="116"/>
-      <c r="B27" s="116"/>
-      <c r="C27" s="113"/>
+      <c r="A27" s="111"/>
+      <c r="B27" s="111"/>
+      <c r="C27" s="121"/>
       <c r="D27" s="36" t="s">
         <v>58</v>
       </c>
@@ -4201,11 +4201,11 @@
       <c r="U27" s="42"/>
     </row>
     <row r="28" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="116"/>
-      <c r="B28" s="116" t="s">
+      <c r="A28" s="111"/>
+      <c r="B28" s="111" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="113" t="s">
+      <c r="C28" s="121" t="s">
         <v>21</v>
       </c>
       <c r="D28" s="9" t="s">
@@ -4239,9 +4239,9 @@
       <c r="U28" s="10"/>
     </row>
     <row r="29" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="116"/>
-      <c r="B29" s="116"/>
-      <c r="C29" s="113"/>
+      <c r="A29" s="111"/>
+      <c r="B29" s="111"/>
+      <c r="C29" s="121"/>
       <c r="D29" s="36" t="s">
         <v>59</v>
       </c>
@@ -4303,9 +4303,9 @@
       <c r="U29" s="10"/>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A30" s="116"/>
-      <c r="B30" s="116"/>
-      <c r="C30" s="113" t="s">
+      <c r="A30" s="111"/>
+      <c r="B30" s="111"/>
+      <c r="C30" s="121" t="s">
         <v>57</v>
       </c>
       <c r="D30" s="9" t="s">
@@ -4339,9 +4339,9 @@
       <c r="U30" s="10"/>
     </row>
     <row r="31" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="116"/>
-      <c r="B31" s="116"/>
-      <c r="C31" s="113"/>
+      <c r="A31" s="111"/>
+      <c r="B31" s="111"/>
+      <c r="C31" s="121"/>
       <c r="D31" s="35" t="s">
         <v>60</v>
       </c>
@@ -4448,13 +4448,13 @@
       <c r="U33" s="10"/>
     </row>
     <row r="34" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="114" t="s">
+      <c r="A34" s="124" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="116" t="s">
+      <c r="B34" s="111" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="113" t="s">
+      <c r="C34" s="121" t="s">
         <v>16</v>
       </c>
       <c r="D34" s="9" t="s">
@@ -4497,9 +4497,9 @@
       <c r="U34" s="10"/>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A35" s="115"/>
-      <c r="B35" s="116"/>
-      <c r="C35" s="113"/>
+      <c r="A35" s="125"/>
+      <c r="B35" s="111"/>
+      <c r="C35" s="121"/>
       <c r="D35" s="9" t="s">
         <v>14</v>
       </c>
@@ -4540,9 +4540,9 @@
       <c r="U35" s="10"/>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A36" s="115"/>
-      <c r="B36" s="116"/>
-      <c r="C36" s="113"/>
+      <c r="A36" s="125"/>
+      <c r="B36" s="111"/>
+      <c r="C36" s="121"/>
       <c r="D36" s="9" t="s">
         <v>36</v>
       </c>
@@ -4583,9 +4583,9 @@
       <c r="U36" s="10"/>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A37" s="115"/>
-      <c r="B37" s="116"/>
-      <c r="C37" s="113"/>
+      <c r="A37" s="125"/>
+      <c r="B37" s="111"/>
+      <c r="C37" s="121"/>
       <c r="D37" s="9" t="s">
         <v>22</v>
       </c>
@@ -4626,9 +4626,9 @@
       <c r="U37" s="10"/>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A38" s="115"/>
-      <c r="B38" s="116"/>
-      <c r="C38" s="113"/>
+      <c r="A38" s="125"/>
+      <c r="B38" s="111"/>
+      <c r="C38" s="121"/>
       <c r="D38" s="48" t="s">
         <v>61</v>
       </c>
@@ -4681,9 +4681,9 @@
       <c r="U38" s="10"/>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A39" s="115"/>
-      <c r="B39" s="116"/>
-      <c r="C39" s="113"/>
+      <c r="A39" s="125"/>
+      <c r="B39" s="111"/>
+      <c r="C39" s="121"/>
       <c r="D39" s="9" t="s">
         <v>21</v>
       </c>
@@ -4724,9 +4724,9 @@
       <c r="U39" s="10"/>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A40" s="115"/>
-      <c r="B40" s="116"/>
-      <c r="C40" s="113"/>
+      <c r="A40" s="125"/>
+      <c r="B40" s="111"/>
+      <c r="C40" s="121"/>
       <c r="D40" s="48" t="s">
         <v>62</v>
       </c>
@@ -4779,9 +4779,9 @@
       <c r="U40" s="10"/>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A41" s="115"/>
-      <c r="B41" s="116"/>
-      <c r="C41" s="113"/>
+      <c r="A41" s="125"/>
+      <c r="B41" s="111"/>
+      <c r="C41" s="121"/>
       <c r="D41" s="9" t="s">
         <v>23</v>
       </c>
@@ -4822,9 +4822,9 @@
       <c r="U41" s="10"/>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A42" s="115"/>
-      <c r="B42" s="116"/>
-      <c r="C42" s="113"/>
+      <c r="A42" s="125"/>
+      <c r="B42" s="111"/>
+      <c r="C42" s="121"/>
       <c r="D42" s="48" t="s">
         <v>63</v>
       </c>
@@ -4877,9 +4877,9 @@
       <c r="U42" s="10"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A43" s="115"/>
-      <c r="B43" s="116"/>
-      <c r="C43" s="113"/>
+      <c r="A43" s="125"/>
+      <c r="B43" s="111"/>
+      <c r="C43" s="121"/>
       <c r="D43" s="9" t="s">
         <v>20</v>
       </c>
@@ -4920,9 +4920,9 @@
       <c r="U43" s="10"/>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A44" s="115"/>
-      <c r="B44" s="116"/>
-      <c r="C44" s="113"/>
+      <c r="A44" s="125"/>
+      <c r="B44" s="111"/>
+      <c r="C44" s="121"/>
       <c r="D44" s="9" t="s">
         <v>24</v>
       </c>
@@ -4963,9 +4963,9 @@
       <c r="U44" s="10"/>
     </row>
     <row r="45" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A45" s="115"/>
-      <c r="B45" s="116"/>
-      <c r="C45" s="113"/>
+      <c r="A45" s="125"/>
+      <c r="B45" s="111"/>
+      <c r="C45" s="121"/>
       <c r="D45" s="49" t="s">
         <v>64</v>
       </c>
@@ -5030,9 +5030,9 @@
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A46" s="115"/>
-      <c r="B46" s="116"/>
-      <c r="C46" s="113"/>
+      <c r="A46" s="125"/>
+      <c r="B46" s="111"/>
+      <c r="C46" s="121"/>
       <c r="D46" s="36" t="s">
         <v>65</v>
       </c>
@@ -5097,11 +5097,11 @@
       </c>
     </row>
     <row r="47" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="115"/>
-      <c r="B47" s="116" t="s">
+      <c r="A47" s="125"/>
+      <c r="B47" s="111" t="s">
         <v>71</v>
       </c>
-      <c r="C47" s="113" t="s">
+      <c r="C47" s="121" t="s">
         <v>15</v>
       </c>
       <c r="D47" s="10"/>
@@ -5124,9 +5124,9 @@
       <c r="U47" s="10"/>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A48" s="115"/>
-      <c r="B48" s="116"/>
-      <c r="C48" s="113"/>
+      <c r="A48" s="125"/>
+      <c r="B48" s="111"/>
+      <c r="C48" s="121"/>
       <c r="D48" s="9" t="s">
         <v>25</v>
       </c>
@@ -5152,9 +5152,9 @@
       <c r="U48" s="10"/>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A49" s="115"/>
-      <c r="B49" s="116"/>
-      <c r="C49" s="113"/>
+      <c r="A49" s="125"/>
+      <c r="B49" s="111"/>
+      <c r="C49" s="121"/>
       <c r="D49" s="9" t="s">
         <v>14</v>
       </c>
@@ -5180,9 +5180,9 @@
       <c r="U49" s="10"/>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A50" s="115"/>
-      <c r="B50" s="116"/>
-      <c r="C50" s="113"/>
+      <c r="A50" s="125"/>
+      <c r="B50" s="111"/>
+      <c r="C50" s="121"/>
       <c r="D50" s="9" t="s">
         <v>36</v>
       </c>
@@ -5208,9 +5208,9 @@
       <c r="U50" s="10"/>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A51" s="115"/>
-      <c r="B51" s="116"/>
-      <c r="C51" s="113"/>
+      <c r="A51" s="125"/>
+      <c r="B51" s="111"/>
+      <c r="C51" s="121"/>
       <c r="D51" s="9" t="s">
         <v>22</v>
       </c>
@@ -5236,9 +5236,9 @@
       <c r="U51" s="10"/>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A52" s="115"/>
-      <c r="B52" s="116"/>
-      <c r="C52" s="113"/>
+      <c r="A52" s="125"/>
+      <c r="B52" s="111"/>
+      <c r="C52" s="121"/>
       <c r="D52" s="48" t="s">
         <v>61</v>
       </c>
@@ -5270,9 +5270,9 @@
       <c r="U52" s="10"/>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A53" s="115"/>
-      <c r="B53" s="116"/>
-      <c r="C53" s="113"/>
+      <c r="A53" s="125"/>
+      <c r="B53" s="111"/>
+      <c r="C53" s="121"/>
       <c r="D53" s="9" t="s">
         <v>21</v>
       </c>
@@ -5298,9 +5298,9 @@
       <c r="U53" s="10"/>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A54" s="115"/>
-      <c r="B54" s="116"/>
-      <c r="C54" s="113"/>
+      <c r="A54" s="125"/>
+      <c r="B54" s="111"/>
+      <c r="C54" s="121"/>
       <c r="D54" s="48" t="s">
         <v>62</v>
       </c>
@@ -5332,9 +5332,9 @@
       <c r="U54" s="10"/>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A55" s="115"/>
-      <c r="B55" s="116"/>
-      <c r="C55" s="113"/>
+      <c r="A55" s="125"/>
+      <c r="B55" s="111"/>
+      <c r="C55" s="121"/>
       <c r="D55" s="9" t="s">
         <v>23</v>
       </c>
@@ -5360,9 +5360,9 @@
       <c r="U55" s="10"/>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A56" s="115"/>
-      <c r="B56" s="116"/>
-      <c r="C56" s="113"/>
+      <c r="A56" s="125"/>
+      <c r="B56" s="111"/>
+      <c r="C56" s="121"/>
       <c r="D56" s="48" t="s">
         <v>63</v>
       </c>
@@ -5394,9 +5394,9 @@
       <c r="U56" s="10"/>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A57" s="115"/>
-      <c r="B57" s="116"/>
-      <c r="C57" s="113"/>
+      <c r="A57" s="125"/>
+      <c r="B57" s="111"/>
+      <c r="C57" s="121"/>
       <c r="D57" s="9" t="s">
         <v>20</v>
       </c>
@@ -5422,9 +5422,9 @@
       <c r="U57" s="10"/>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A58" s="115"/>
-      <c r="B58" s="116"/>
-      <c r="C58" s="113"/>
+      <c r="A58" s="125"/>
+      <c r="B58" s="111"/>
+      <c r="C58" s="121"/>
       <c r="D58" s="9" t="s">
         <v>24</v>
       </c>
@@ -5450,9 +5450,9 @@
       <c r="U58" s="10"/>
     </row>
     <row r="59" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A59" s="115"/>
-      <c r="B59" s="116"/>
-      <c r="C59" s="113"/>
+      <c r="A59" s="125"/>
+      <c r="B59" s="111"/>
+      <c r="C59" s="121"/>
       <c r="D59" s="49" t="s">
         <v>64</v>
       </c>
@@ -5517,9 +5517,9 @@
       </c>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A60" s="115"/>
-      <c r="B60" s="116"/>
-      <c r="C60" s="113"/>
+      <c r="A60" s="125"/>
+      <c r="B60" s="111"/>
+      <c r="C60" s="121"/>
       <c r="D60" s="36" t="s">
         <v>66</v>
       </c>
@@ -5584,13 +5584,13 @@
       </c>
     </row>
     <row r="61" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="114" t="s">
+      <c r="A61" s="124" t="s">
         <v>69</v>
       </c>
-      <c r="B61" s="116" t="s">
+      <c r="B61" s="111" t="s">
         <v>72</v>
       </c>
-      <c r="C61" s="111" t="s">
+      <c r="C61" s="122" t="s">
         <v>73</v>
       </c>
       <c r="D61" s="10"/>
@@ -5613,9 +5613,9 @@
       <c r="U61" s="10"/>
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A62" s="115"/>
-      <c r="B62" s="116"/>
-      <c r="C62" s="112"/>
+      <c r="A62" s="125"/>
+      <c r="B62" s="111"/>
+      <c r="C62" s="123"/>
       <c r="D62" s="9" t="s">
         <v>25</v>
       </c>
@@ -5656,9 +5656,9 @@
       <c r="U62" s="10"/>
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A63" s="115"/>
-      <c r="B63" s="116"/>
-      <c r="C63" s="112"/>
+      <c r="A63" s="125"/>
+      <c r="B63" s="111"/>
+      <c r="C63" s="123"/>
       <c r="D63" s="9" t="s">
         <v>14</v>
       </c>
@@ -5699,9 +5699,9 @@
       <c r="U63" s="10"/>
     </row>
     <row r="64" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A64" s="115"/>
-      <c r="B64" s="116"/>
-      <c r="C64" s="112"/>
+      <c r="A64" s="125"/>
+      <c r="B64" s="111"/>
+      <c r="C64" s="123"/>
       <c r="D64" s="9" t="s">
         <v>36</v>
       </c>
@@ -5742,9 +5742,9 @@
       <c r="U64" s="10"/>
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A65" s="115"/>
-      <c r="B65" s="116"/>
-      <c r="C65" s="112"/>
+      <c r="A65" s="125"/>
+      <c r="B65" s="111"/>
+      <c r="C65" s="123"/>
       <c r="D65" s="9" t="s">
         <v>22</v>
       </c>
@@ -5785,9 +5785,9 @@
       <c r="U65" s="10"/>
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A66" s="115"/>
-      <c r="B66" s="116"/>
-      <c r="C66" s="112"/>
+      <c r="A66" s="125"/>
+      <c r="B66" s="111"/>
+      <c r="C66" s="123"/>
       <c r="D66" s="48" t="s">
         <v>61</v>
       </c>
@@ -5840,9 +5840,9 @@
       <c r="U66" s="10"/>
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A67" s="115"/>
-      <c r="B67" s="116"/>
-      <c r="C67" s="112"/>
+      <c r="A67" s="125"/>
+      <c r="B67" s="111"/>
+      <c r="C67" s="123"/>
       <c r="D67" s="9" t="s">
         <v>21</v>
       </c>
@@ -5883,9 +5883,9 @@
       <c r="U67" s="10"/>
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A68" s="115"/>
-      <c r="B68" s="116"/>
-      <c r="C68" s="112"/>
+      <c r="A68" s="125"/>
+      <c r="B68" s="111"/>
+      <c r="C68" s="123"/>
       <c r="D68" s="48" t="s">
         <v>62</v>
       </c>
@@ -5938,9 +5938,9 @@
       <c r="U68" s="10"/>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A69" s="115"/>
-      <c r="B69" s="116"/>
-      <c r="C69" s="112"/>
+      <c r="A69" s="125"/>
+      <c r="B69" s="111"/>
+      <c r="C69" s="123"/>
       <c r="D69" s="9" t="s">
         <v>23</v>
       </c>
@@ -5981,9 +5981,9 @@
       <c r="U69" s="10"/>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A70" s="115"/>
-      <c r="B70" s="116"/>
-      <c r="C70" s="112"/>
+      <c r="A70" s="125"/>
+      <c r="B70" s="111"/>
+      <c r="C70" s="123"/>
       <c r="D70" s="48" t="s">
         <v>63</v>
       </c>
@@ -6048,9 +6048,9 @@
       </c>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A71" s="115"/>
-      <c r="B71" s="116"/>
-      <c r="C71" s="112"/>
+      <c r="A71" s="125"/>
+      <c r="B71" s="111"/>
+      <c r="C71" s="123"/>
       <c r="D71" s="9" t="s">
         <v>20</v>
       </c>
@@ -6091,9 +6091,9 @@
       <c r="U71" s="10"/>
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A72" s="115"/>
-      <c r="B72" s="116"/>
-      <c r="C72" s="112"/>
+      <c r="A72" s="125"/>
+      <c r="B72" s="111"/>
+      <c r="C72" s="123"/>
       <c r="D72" s="9" t="s">
         <v>24</v>
       </c>
@@ -6119,9 +6119,9 @@
       </c>
     </row>
     <row r="73" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A73" s="115"/>
-      <c r="B73" s="116"/>
-      <c r="C73" s="112"/>
+      <c r="A73" s="125"/>
+      <c r="B73" s="111"/>
+      <c r="C73" s="123"/>
       <c r="D73" s="49" t="s">
         <v>64</v>
       </c>
@@ -6186,9 +6186,9 @@
       </c>
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A74" s="115"/>
-      <c r="B74" s="116"/>
-      <c r="C74" s="113" t="s">
+      <c r="A74" s="125"/>
+      <c r="B74" s="111"/>
+      <c r="C74" s="121" t="s">
         <v>74</v>
       </c>
       <c r="D74" s="10"/>
@@ -6211,9 +6211,9 @@
       <c r="U74" s="10"/>
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A75" s="115"/>
-      <c r="B75" s="116"/>
-      <c r="C75" s="113"/>
+      <c r="A75" s="125"/>
+      <c r="B75" s="111"/>
+      <c r="C75" s="121"/>
       <c r="D75" s="9" t="s">
         <v>25</v>
       </c>
@@ -6248,9 +6248,9 @@
       <c r="U75" s="10"/>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A76" s="115"/>
-      <c r="B76" s="116"/>
-      <c r="C76" s="113"/>
+      <c r="A76" s="125"/>
+      <c r="B76" s="111"/>
+      <c r="C76" s="121"/>
       <c r="D76" s="9" t="s">
         <v>14</v>
       </c>
@@ -6285,9 +6285,9 @@
       <c r="U76" s="10"/>
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A77" s="115"/>
-      <c r="B77" s="116"/>
-      <c r="C77" s="113"/>
+      <c r="A77" s="125"/>
+      <c r="B77" s="111"/>
+      <c r="C77" s="121"/>
       <c r="D77" s="9" t="s">
         <v>36</v>
       </c>
@@ -6322,9 +6322,9 @@
       <c r="U77" s="10"/>
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A78" s="115"/>
-      <c r="B78" s="116"/>
-      <c r="C78" s="113"/>
+      <c r="A78" s="125"/>
+      <c r="B78" s="111"/>
+      <c r="C78" s="121"/>
       <c r="D78" s="9" t="s">
         <v>22</v>
       </c>
@@ -6359,9 +6359,9 @@
       <c r="U78" s="10"/>
     </row>
     <row r="79" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A79" s="115"/>
-      <c r="B79" s="116"/>
-      <c r="C79" s="113"/>
+      <c r="A79" s="125"/>
+      <c r="B79" s="111"/>
+      <c r="C79" s="121"/>
       <c r="D79" s="48" t="s">
         <v>61</v>
       </c>
@@ -6414,9 +6414,9 @@
       <c r="U79" s="10"/>
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A80" s="115"/>
-      <c r="B80" s="116"/>
-      <c r="C80" s="113"/>
+      <c r="A80" s="125"/>
+      <c r="B80" s="111"/>
+      <c r="C80" s="121"/>
       <c r="D80" s="9" t="s">
         <v>21</v>
       </c>
@@ -6451,9 +6451,9 @@
       <c r="U80" s="10"/>
     </row>
     <row r="81" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A81" s="115"/>
-      <c r="B81" s="116"/>
-      <c r="C81" s="113"/>
+      <c r="A81" s="125"/>
+      <c r="B81" s="111"/>
+      <c r="C81" s="121"/>
       <c r="D81" s="48" t="s">
         <v>62</v>
       </c>
@@ -6506,9 +6506,9 @@
       <c r="U81" s="10"/>
     </row>
     <row r="82" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A82" s="115"/>
-      <c r="B82" s="116"/>
-      <c r="C82" s="113"/>
+      <c r="A82" s="125"/>
+      <c r="B82" s="111"/>
+      <c r="C82" s="121"/>
       <c r="D82" s="9" t="s">
         <v>23</v>
       </c>
@@ -6543,9 +6543,9 @@
       <c r="U82" s="10"/>
     </row>
     <row r="83" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A83" s="115"/>
-      <c r="B83" s="116"/>
-      <c r="C83" s="113"/>
+      <c r="A83" s="125"/>
+      <c r="B83" s="111"/>
+      <c r="C83" s="121"/>
       <c r="D83" s="48" t="s">
         <v>63</v>
       </c>
@@ -6610,9 +6610,9 @@
       </c>
     </row>
     <row r="84" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A84" s="115"/>
-      <c r="B84" s="116"/>
-      <c r="C84" s="113"/>
+      <c r="A84" s="125"/>
+      <c r="B84" s="111"/>
+      <c r="C84" s="121"/>
       <c r="D84" s="9" t="s">
         <v>20</v>
       </c>
@@ -6647,9 +6647,9 @@
       <c r="U84" s="10"/>
     </row>
     <row r="85" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A85" s="115"/>
-      <c r="B85" s="116"/>
-      <c r="C85" s="113"/>
+      <c r="A85" s="125"/>
+      <c r="B85" s="111"/>
+      <c r="C85" s="121"/>
       <c r="D85" s="9" t="s">
         <v>24</v>
       </c>
@@ -6675,9 +6675,9 @@
       </c>
     </row>
     <row r="86" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A86" s="115"/>
-      <c r="B86" s="116"/>
-      <c r="C86" s="113"/>
+      <c r="A86" s="125"/>
+      <c r="B86" s="111"/>
+      <c r="C86" s="121"/>
       <c r="D86" s="49" t="s">
         <v>64</v>
       </c>
@@ -6742,9 +6742,9 @@
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A87" s="115"/>
-      <c r="B87" s="116"/>
-      <c r="C87" s="113"/>
+      <c r="A87" s="125"/>
+      <c r="B87" s="111"/>
+      <c r="C87" s="121"/>
       <c r="D87" s="36" t="s">
         <v>68</v>
       </c>
@@ -6809,11 +6809,11 @@
       </c>
     </row>
     <row r="88" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="115"/>
-      <c r="B88" s="116" t="s">
+      <c r="A88" s="125"/>
+      <c r="B88" s="111" t="s">
         <v>75</v>
       </c>
-      <c r="C88" s="111" t="s">
+      <c r="C88" s="122" t="s">
         <v>76</v>
       </c>
       <c r="D88" s="10"/>
@@ -6836,9 +6836,9 @@
       <c r="U88" s="10"/>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A89" s="115"/>
-      <c r="B89" s="116"/>
-      <c r="C89" s="112"/>
+      <c r="A89" s="125"/>
+      <c r="B89" s="111"/>
+      <c r="C89" s="123"/>
       <c r="D89" s="9" t="s">
         <v>25</v>
       </c>
@@ -6891,9 +6891,9 @@
       <c r="U89" s="10"/>
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A90" s="115"/>
-      <c r="B90" s="116"/>
-      <c r="C90" s="112"/>
+      <c r="A90" s="125"/>
+      <c r="B90" s="111"/>
+      <c r="C90" s="123"/>
       <c r="D90" s="9" t="s">
         <v>14</v>
       </c>
@@ -6946,9 +6946,9 @@
       <c r="U90" s="10"/>
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A91" s="115"/>
-      <c r="B91" s="116"/>
-      <c r="C91" s="112"/>
+      <c r="A91" s="125"/>
+      <c r="B91" s="111"/>
+      <c r="C91" s="123"/>
       <c r="D91" s="9" t="s">
         <v>36</v>
       </c>
@@ -6997,9 +6997,9 @@
       <c r="S91" s="61"/>
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A92" s="115"/>
-      <c r="B92" s="116"/>
-      <c r="C92" s="112"/>
+      <c r="A92" s="125"/>
+      <c r="B92" s="111"/>
+      <c r="C92" s="123"/>
       <c r="D92" s="9" t="s">
         <v>22</v>
       </c>
@@ -7048,9 +7048,9 @@
       <c r="S92" s="61"/>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A93" s="115"/>
-      <c r="B93" s="116"/>
-      <c r="C93" s="112"/>
+      <c r="A93" s="125"/>
+      <c r="B93" s="111"/>
+      <c r="C93" s="123"/>
       <c r="D93" s="48" t="s">
         <v>61</v>
       </c>
@@ -7099,9 +7099,9 @@
       <c r="S93" s="10"/>
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A94" s="115"/>
-      <c r="B94" s="116"/>
-      <c r="C94" s="112"/>
+      <c r="A94" s="125"/>
+      <c r="B94" s="111"/>
+      <c r="C94" s="123"/>
       <c r="D94" s="9" t="s">
         <v>21</v>
       </c>
@@ -7150,9 +7150,9 @@
       <c r="S94" s="61"/>
     </row>
     <row r="95" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A95" s="115"/>
-      <c r="B95" s="116"/>
-      <c r="C95" s="112"/>
+      <c r="A95" s="125"/>
+      <c r="B95" s="111"/>
+      <c r="C95" s="123"/>
       <c r="D95" s="48" t="s">
         <v>62</v>
       </c>
@@ -7201,9 +7201,9 @@
       <c r="S95" s="10"/>
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A96" s="115"/>
-      <c r="B96" s="116"/>
-      <c r="C96" s="112"/>
+      <c r="A96" s="125"/>
+      <c r="B96" s="111"/>
+      <c r="C96" s="123"/>
       <c r="D96" s="9" t="s">
         <v>23</v>
       </c>
@@ -7252,9 +7252,9 @@
       <c r="S96" s="61"/>
     </row>
     <row r="97" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A97" s="115"/>
-      <c r="B97" s="116"/>
-      <c r="C97" s="112"/>
+      <c r="A97" s="125"/>
+      <c r="B97" s="111"/>
+      <c r="C97" s="123"/>
       <c r="D97" s="48" t="s">
         <v>63</v>
       </c>
@@ -7316,9 +7316,9 @@
       </c>
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A98" s="115"/>
-      <c r="B98" s="116"/>
-      <c r="C98" s="112"/>
+      <c r="A98" s="125"/>
+      <c r="B98" s="111"/>
+      <c r="C98" s="123"/>
       <c r="D98" s="9" t="s">
         <v>20</v>
       </c>
@@ -7367,9 +7367,9 @@
       <c r="S98" s="61"/>
     </row>
     <row r="99" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A99" s="115"/>
-      <c r="B99" s="116"/>
-      <c r="C99" s="112"/>
+      <c r="A99" s="125"/>
+      <c r="B99" s="111"/>
+      <c r="C99" s="123"/>
       <c r="D99" s="9" t="s">
         <v>24</v>
       </c>
@@ -7392,9 +7392,9 @@
       </c>
     </row>
     <row r="100" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A100" s="115"/>
-      <c r="B100" s="116"/>
-      <c r="C100" s="112"/>
+      <c r="A100" s="125"/>
+      <c r="B100" s="111"/>
+      <c r="C100" s="123"/>
       <c r="D100" s="49" t="s">
         <v>64</v>
       </c>
@@ -7459,9 +7459,9 @@
       </c>
     </row>
     <row r="101" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A101" s="115"/>
-      <c r="B101" s="116"/>
-      <c r="C101" s="111" t="s">
+      <c r="A101" s="125"/>
+      <c r="B101" s="111"/>
+      <c r="C101" s="122" t="s">
         <v>77</v>
       </c>
       <c r="I101" s="10"/>
@@ -7473,9 +7473,9 @@
       <c r="U101" s="10"/>
     </row>
     <row r="102" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A102" s="115"/>
-      <c r="B102" s="116"/>
-      <c r="C102" s="112"/>
+      <c r="A102" s="125"/>
+      <c r="B102" s="111"/>
+      <c r="C102" s="123"/>
       <c r="D102" s="9" t="s">
         <v>25</v>
       </c>
@@ -7528,9 +7528,9 @@
       <c r="U102" s="10"/>
     </row>
     <row r="103" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A103" s="115"/>
-      <c r="B103" s="116"/>
-      <c r="C103" s="112"/>
+      <c r="A103" s="125"/>
+      <c r="B103" s="111"/>
+      <c r="C103" s="123"/>
       <c r="D103" s="9" t="s">
         <v>14</v>
       </c>
@@ -7583,9 +7583,9 @@
       <c r="U103" s="10"/>
     </row>
     <row r="104" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A104" s="115"/>
-      <c r="B104" s="116"/>
-      <c r="C104" s="112"/>
+      <c r="A104" s="125"/>
+      <c r="B104" s="111"/>
+      <c r="C104" s="123"/>
       <c r="D104" s="9" t="s">
         <v>36</v>
       </c>
@@ -7634,9 +7634,9 @@
       <c r="S104" s="61"/>
     </row>
     <row r="105" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A105" s="115"/>
-      <c r="B105" s="116"/>
-      <c r="C105" s="112"/>
+      <c r="A105" s="125"/>
+      <c r="B105" s="111"/>
+      <c r="C105" s="123"/>
       <c r="D105" s="9" t="s">
         <v>22</v>
       </c>
@@ -7685,9 +7685,9 @@
       <c r="S105" s="61"/>
     </row>
     <row r="106" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A106" s="115"/>
-      <c r="B106" s="116"/>
-      <c r="C106" s="112"/>
+      <c r="A106" s="125"/>
+      <c r="B106" s="111"/>
+      <c r="C106" s="123"/>
       <c r="D106" s="48" t="s">
         <v>61</v>
       </c>
@@ -7736,9 +7736,9 @@
       <c r="S106" s="10"/>
     </row>
     <row r="107" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A107" s="115"/>
-      <c r="B107" s="116"/>
-      <c r="C107" s="112"/>
+      <c r="A107" s="125"/>
+      <c r="B107" s="111"/>
+      <c r="C107" s="123"/>
       <c r="D107" s="9" t="s">
         <v>21</v>
       </c>
@@ -7787,9 +7787,9 @@
       <c r="S107" s="61"/>
     </row>
     <row r="108" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A108" s="115"/>
-      <c r="B108" s="116"/>
-      <c r="C108" s="112"/>
+      <c r="A108" s="125"/>
+      <c r="B108" s="111"/>
+      <c r="C108" s="123"/>
       <c r="D108" s="48" t="s">
         <v>62</v>
       </c>
@@ -7838,9 +7838,9 @@
       <c r="S108" s="10"/>
     </row>
     <row r="109" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A109" s="115"/>
-      <c r="B109" s="116"/>
-      <c r="C109" s="112"/>
+      <c r="A109" s="125"/>
+      <c r="B109" s="111"/>
+      <c r="C109" s="123"/>
       <c r="D109" s="9" t="s">
         <v>23</v>
       </c>
@@ -7889,9 +7889,9 @@
       <c r="S109" s="61"/>
     </row>
     <row r="110" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A110" s="115"/>
-      <c r="B110" s="116"/>
-      <c r="C110" s="112"/>
+      <c r="A110" s="125"/>
+      <c r="B110" s="111"/>
+      <c r="C110" s="123"/>
       <c r="D110" s="48" t="s">
         <v>63</v>
       </c>
@@ -7953,9 +7953,9 @@
       </c>
     </row>
     <row r="111" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A111" s="115"/>
-      <c r="B111" s="116"/>
-      <c r="C111" s="112"/>
+      <c r="A111" s="125"/>
+      <c r="B111" s="111"/>
+      <c r="C111" s="123"/>
       <c r="D111" s="9" t="s">
         <v>20</v>
       </c>
@@ -8004,9 +8004,9 @@
       <c r="S111" s="61"/>
     </row>
     <row r="112" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A112" s="115"/>
-      <c r="B112" s="116"/>
-      <c r="C112" s="112"/>
+      <c r="A112" s="125"/>
+      <c r="B112" s="111"/>
+      <c r="C112" s="123"/>
       <c r="D112" s="9" t="s">
         <v>24</v>
       </c>
@@ -8029,9 +8029,9 @@
       </c>
     </row>
     <row r="113" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A113" s="115"/>
-      <c r="B113" s="116"/>
-      <c r="C113" s="112"/>
+      <c r="A113" s="125"/>
+      <c r="B113" s="111"/>
+      <c r="C113" s="123"/>
       <c r="D113" s="49" t="s">
         <v>64</v>
       </c>
@@ -8096,11 +8096,11 @@
       </c>
     </row>
     <row r="114" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="114" t="s">
+      <c r="A114" s="124" t="s">
         <v>69</v>
       </c>
-      <c r="B114" s="116"/>
-      <c r="C114" s="111" t="s">
+      <c r="B114" s="111"/>
+      <c r="C114" s="122" t="s">
         <v>78</v>
       </c>
       <c r="I114" s="10"/>
@@ -8112,9 +8112,9 @@
       <c r="U114" s="10"/>
     </row>
     <row r="115" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A115" s="115"/>
-      <c r="B115" s="116"/>
-      <c r="C115" s="112"/>
+      <c r="A115" s="125"/>
+      <c r="B115" s="111"/>
+      <c r="C115" s="123"/>
       <c r="D115" s="9" t="s">
         <v>25</v>
       </c>
@@ -8167,9 +8167,9 @@
       <c r="U115" s="10"/>
     </row>
     <row r="116" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A116" s="115"/>
-      <c r="B116" s="116"/>
-      <c r="C116" s="112"/>
+      <c r="A116" s="125"/>
+      <c r="B116" s="111"/>
+      <c r="C116" s="123"/>
       <c r="D116" s="9" t="s">
         <v>14</v>
       </c>
@@ -8222,9 +8222,9 @@
       <c r="U116" s="10"/>
     </row>
     <row r="117" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A117" s="115"/>
-      <c r="B117" s="116"/>
-      <c r="C117" s="112"/>
+      <c r="A117" s="125"/>
+      <c r="B117" s="111"/>
+      <c r="C117" s="123"/>
       <c r="D117" s="9" t="s">
         <v>36</v>
       </c>
@@ -8273,9 +8273,9 @@
       <c r="S117" s="61"/>
     </row>
     <row r="118" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A118" s="115"/>
-      <c r="B118" s="116"/>
-      <c r="C118" s="112"/>
+      <c r="A118" s="125"/>
+      <c r="B118" s="111"/>
+      <c r="C118" s="123"/>
       <c r="D118" s="9" t="s">
         <v>22</v>
       </c>
@@ -8324,9 +8324,9 @@
       <c r="S118" s="61"/>
     </row>
     <row r="119" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A119" s="115"/>
-      <c r="B119" s="116"/>
-      <c r="C119" s="112"/>
+      <c r="A119" s="125"/>
+      <c r="B119" s="111"/>
+      <c r="C119" s="123"/>
       <c r="D119" s="48" t="s">
         <v>61</v>
       </c>
@@ -8375,9 +8375,9 @@
       <c r="S119" s="10"/>
     </row>
     <row r="120" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A120" s="115"/>
-      <c r="B120" s="116"/>
-      <c r="C120" s="112"/>
+      <c r="A120" s="125"/>
+      <c r="B120" s="111"/>
+      <c r="C120" s="123"/>
       <c r="D120" s="9" t="s">
         <v>21</v>
       </c>
@@ -8426,9 +8426,9 @@
       <c r="S120" s="61"/>
     </row>
     <row r="121" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A121" s="115"/>
-      <c r="B121" s="116"/>
-      <c r="C121" s="112"/>
+      <c r="A121" s="125"/>
+      <c r="B121" s="111"/>
+      <c r="C121" s="123"/>
       <c r="D121" s="48" t="s">
         <v>62</v>
       </c>
@@ -8477,9 +8477,9 @@
       <c r="S121" s="10"/>
     </row>
     <row r="122" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A122" s="115"/>
-      <c r="B122" s="116"/>
-      <c r="C122" s="112"/>
+      <c r="A122" s="125"/>
+      <c r="B122" s="111"/>
+      <c r="C122" s="123"/>
       <c r="D122" s="9" t="s">
         <v>23</v>
       </c>
@@ -8528,9 +8528,9 @@
       <c r="S122" s="61"/>
     </row>
     <row r="123" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A123" s="115"/>
-      <c r="B123" s="116"/>
-      <c r="C123" s="112"/>
+      <c r="A123" s="125"/>
+      <c r="B123" s="111"/>
+      <c r="C123" s="123"/>
       <c r="D123" s="48" t="s">
         <v>63</v>
       </c>
@@ -8592,9 +8592,9 @@
       </c>
     </row>
     <row r="124" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A124" s="115"/>
-      <c r="B124" s="116"/>
-      <c r="C124" s="112"/>
+      <c r="A124" s="125"/>
+      <c r="B124" s="111"/>
+      <c r="C124" s="123"/>
       <c r="D124" s="9" t="s">
         <v>20</v>
       </c>
@@ -8643,9 +8643,9 @@
       <c r="S124" s="61"/>
     </row>
     <row r="125" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A125" s="115"/>
-      <c r="B125" s="116"/>
-      <c r="C125" s="112"/>
+      <c r="A125" s="125"/>
+      <c r="B125" s="111"/>
+      <c r="C125" s="123"/>
       <c r="D125" s="9" t="s">
         <v>24</v>
       </c>
@@ -8668,9 +8668,9 @@
       </c>
     </row>
     <row r="126" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A126" s="115"/>
-      <c r="B126" s="116"/>
-      <c r="C126" s="112"/>
+      <c r="A126" s="125"/>
+      <c r="B126" s="111"/>
+      <c r="C126" s="123"/>
       <c r="D126" s="49" t="s">
         <v>64</v>
       </c>
@@ -8735,9 +8735,9 @@
       </c>
     </row>
     <row r="127" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A127" s="115"/>
-      <c r="B127" s="116"/>
-      <c r="C127" s="111" t="s">
+      <c r="A127" s="125"/>
+      <c r="B127" s="111"/>
+      <c r="C127" s="122" t="s">
         <v>79</v>
       </c>
       <c r="I127" s="10"/>
@@ -8749,9 +8749,9 @@
       <c r="U127" s="10"/>
     </row>
     <row r="128" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A128" s="115"/>
-      <c r="B128" s="116"/>
-      <c r="C128" s="112"/>
+      <c r="A128" s="125"/>
+      <c r="B128" s="111"/>
+      <c r="C128" s="123"/>
       <c r="D128" s="9" t="s">
         <v>25</v>
       </c>
@@ -8804,9 +8804,9 @@
       <c r="U128" s="10"/>
     </row>
     <row r="129" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A129" s="115"/>
-      <c r="B129" s="116"/>
-      <c r="C129" s="112"/>
+      <c r="A129" s="125"/>
+      <c r="B129" s="111"/>
+      <c r="C129" s="123"/>
       <c r="D129" s="9" t="s">
         <v>14</v>
       </c>
@@ -8859,9 +8859,9 @@
       <c r="U129" s="10"/>
     </row>
     <row r="130" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A130" s="115"/>
-      <c r="B130" s="116"/>
-      <c r="C130" s="112"/>
+      <c r="A130" s="125"/>
+      <c r="B130" s="111"/>
+      <c r="C130" s="123"/>
       <c r="D130" s="9" t="s">
         <v>36</v>
       </c>
@@ -8910,9 +8910,9 @@
       <c r="S130" s="61"/>
     </row>
     <row r="131" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A131" s="115"/>
-      <c r="B131" s="116"/>
-      <c r="C131" s="112"/>
+      <c r="A131" s="125"/>
+      <c r="B131" s="111"/>
+      <c r="C131" s="123"/>
       <c r="D131" s="9" t="s">
         <v>22</v>
       </c>
@@ -8961,9 +8961,9 @@
       <c r="S131" s="61"/>
     </row>
     <row r="132" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A132" s="115"/>
-      <c r="B132" s="116"/>
-      <c r="C132" s="112"/>
+      <c r="A132" s="125"/>
+      <c r="B132" s="111"/>
+      <c r="C132" s="123"/>
       <c r="D132" s="48" t="s">
         <v>61</v>
       </c>
@@ -9012,9 +9012,9 @@
       <c r="S132" s="10"/>
     </row>
     <row r="133" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A133" s="115"/>
-      <c r="B133" s="116"/>
-      <c r="C133" s="112"/>
+      <c r="A133" s="125"/>
+      <c r="B133" s="111"/>
+      <c r="C133" s="123"/>
       <c r="D133" s="9" t="s">
         <v>21</v>
       </c>
@@ -9063,9 +9063,9 @@
       <c r="S133" s="61"/>
     </row>
     <row r="134" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A134" s="115"/>
-      <c r="B134" s="116"/>
-      <c r="C134" s="112"/>
+      <c r="A134" s="125"/>
+      <c r="B134" s="111"/>
+      <c r="C134" s="123"/>
       <c r="D134" s="48" t="s">
         <v>62</v>
       </c>
@@ -9114,9 +9114,9 @@
       <c r="S134" s="10"/>
     </row>
     <row r="135" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A135" s="115"/>
-      <c r="B135" s="116"/>
-      <c r="C135" s="112"/>
+      <c r="A135" s="125"/>
+      <c r="B135" s="111"/>
+      <c r="C135" s="123"/>
       <c r="D135" s="9" t="s">
         <v>23</v>
       </c>
@@ -9165,9 +9165,9 @@
       <c r="S135" s="61"/>
     </row>
     <row r="136" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A136" s="115"/>
-      <c r="B136" s="116"/>
-      <c r="C136" s="112"/>
+      <c r="A136" s="125"/>
+      <c r="B136" s="111"/>
+      <c r="C136" s="123"/>
       <c r="D136" s="48" t="s">
         <v>63</v>
       </c>
@@ -9229,9 +9229,9 @@
       </c>
     </row>
     <row r="137" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A137" s="115"/>
-      <c r="B137" s="116"/>
-      <c r="C137" s="112"/>
+      <c r="A137" s="125"/>
+      <c r="B137" s="111"/>
+      <c r="C137" s="123"/>
       <c r="D137" s="9" t="s">
         <v>20</v>
       </c>
@@ -9280,9 +9280,9 @@
       <c r="S137" s="61"/>
     </row>
     <row r="138" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A138" s="115"/>
-      <c r="B138" s="116"/>
-      <c r="C138" s="112"/>
+      <c r="A138" s="125"/>
+      <c r="B138" s="111"/>
+      <c r="C138" s="123"/>
       <c r="D138" s="9" t="s">
         <v>24</v>
       </c>
@@ -9305,9 +9305,9 @@
       </c>
     </row>
     <row r="139" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A139" s="115"/>
-      <c r="B139" s="116"/>
-      <c r="C139" s="112"/>
+      <c r="A139" s="125"/>
+      <c r="B139" s="111"/>
+      <c r="C139" s="123"/>
       <c r="D139" s="49" t="s">
         <v>64</v>
       </c>
@@ -9372,9 +9372,9 @@
       </c>
     </row>
     <row r="140" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A140" s="115"/>
-      <c r="B140" s="116"/>
-      <c r="C140" s="113" t="s">
+      <c r="A140" s="125"/>
+      <c r="B140" s="111"/>
+      <c r="C140" s="121" t="s">
         <v>80</v>
       </c>
       <c r="I140" s="10"/>
@@ -9386,9 +9386,9 @@
       <c r="U140" s="10"/>
     </row>
     <row r="141" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A141" s="115"/>
-      <c r="B141" s="116"/>
-      <c r="C141" s="113"/>
+      <c r="A141" s="125"/>
+      <c r="B141" s="111"/>
+      <c r="C141" s="121"/>
       <c r="D141" s="9" t="s">
         <v>25</v>
       </c>
@@ -9441,9 +9441,9 @@
       <c r="U141" s="10"/>
     </row>
     <row r="142" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A142" s="115"/>
-      <c r="B142" s="116"/>
-      <c r="C142" s="113"/>
+      <c r="A142" s="125"/>
+      <c r="B142" s="111"/>
+      <c r="C142" s="121"/>
       <c r="D142" s="9" t="s">
         <v>14</v>
       </c>
@@ -9496,9 +9496,9 @@
       <c r="U142" s="10"/>
     </row>
     <row r="143" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A143" s="115"/>
-      <c r="B143" s="116"/>
-      <c r="C143" s="113"/>
+      <c r="A143" s="125"/>
+      <c r="B143" s="111"/>
+      <c r="C143" s="121"/>
       <c r="D143" s="9" t="s">
         <v>36</v>
       </c>
@@ -9547,9 +9547,9 @@
       <c r="S143" s="61"/>
     </row>
     <row r="144" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A144" s="115"/>
-      <c r="B144" s="116"/>
-      <c r="C144" s="113"/>
+      <c r="A144" s="125"/>
+      <c r="B144" s="111"/>
+      <c r="C144" s="121"/>
       <c r="D144" s="9" t="s">
         <v>22</v>
       </c>
@@ -9598,9 +9598,9 @@
       <c r="S144" s="61"/>
     </row>
     <row r="145" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A145" s="115"/>
-      <c r="B145" s="116"/>
-      <c r="C145" s="113"/>
+      <c r="A145" s="125"/>
+      <c r="B145" s="111"/>
+      <c r="C145" s="121"/>
       <c r="D145" s="48" t="s">
         <v>61</v>
       </c>
@@ -9649,9 +9649,9 @@
       <c r="S145" s="10"/>
     </row>
     <row r="146" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A146" s="115"/>
-      <c r="B146" s="116"/>
-      <c r="C146" s="113"/>
+      <c r="A146" s="125"/>
+      <c r="B146" s="111"/>
+      <c r="C146" s="121"/>
       <c r="D146" s="9" t="s">
         <v>21</v>
       </c>
@@ -9700,9 +9700,9 @@
       <c r="S146" s="61"/>
     </row>
     <row r="147" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A147" s="115"/>
-      <c r="B147" s="116"/>
-      <c r="C147" s="113"/>
+      <c r="A147" s="125"/>
+      <c r="B147" s="111"/>
+      <c r="C147" s="121"/>
       <c r="D147" s="48" t="s">
         <v>62</v>
       </c>
@@ -9751,9 +9751,9 @@
       <c r="S147" s="10"/>
     </row>
     <row r="148" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A148" s="115"/>
-      <c r="B148" s="116"/>
-      <c r="C148" s="113"/>
+      <c r="A148" s="125"/>
+      <c r="B148" s="111"/>
+      <c r="C148" s="121"/>
       <c r="D148" s="9" t="s">
         <v>23</v>
       </c>
@@ -9802,9 +9802,9 @@
       <c r="S148" s="61"/>
     </row>
     <row r="149" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A149" s="115"/>
-      <c r="B149" s="116"/>
-      <c r="C149" s="113"/>
+      <c r="A149" s="125"/>
+      <c r="B149" s="111"/>
+      <c r="C149" s="121"/>
       <c r="D149" s="48" t="s">
         <v>63</v>
       </c>
@@ -9866,9 +9866,9 @@
       </c>
     </row>
     <row r="150" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A150" s="115"/>
-      <c r="B150" s="116"/>
-      <c r="C150" s="113"/>
+      <c r="A150" s="125"/>
+      <c r="B150" s="111"/>
+      <c r="C150" s="121"/>
       <c r="D150" s="9" t="s">
         <v>20</v>
       </c>
@@ -9917,9 +9917,9 @@
       <c r="S150" s="61"/>
     </row>
     <row r="151" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A151" s="115"/>
-      <c r="B151" s="116"/>
-      <c r="C151" s="113"/>
+      <c r="A151" s="125"/>
+      <c r="B151" s="111"/>
+      <c r="C151" s="121"/>
       <c r="D151" s="9" t="s">
         <v>24</v>
       </c>
@@ -9942,9 +9942,9 @@
       </c>
     </row>
     <row r="152" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A152" s="115"/>
-      <c r="B152" s="116"/>
-      <c r="C152" s="113"/>
+      <c r="A152" s="125"/>
+      <c r="B152" s="111"/>
+      <c r="C152" s="121"/>
       <c r="D152" s="49" t="s">
         <v>64</v>
       </c>
@@ -10009,9 +10009,9 @@
       </c>
     </row>
     <row r="153" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A153" s="115"/>
-      <c r="B153" s="116"/>
-      <c r="C153" s="113"/>
+      <c r="A153" s="125"/>
+      <c r="B153" s="111"/>
+      <c r="C153" s="121"/>
       <c r="D153" s="52" t="s">
         <v>67</v>
       </c>
@@ -10113,17 +10113,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A22:A31"/>
-    <mergeCell ref="A8:C11"/>
-    <mergeCell ref="B13:C15"/>
-    <mergeCell ref="B22:B27"/>
-    <mergeCell ref="A13:A19"/>
-    <mergeCell ref="B16:C19"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C30:C31"/>
     <mergeCell ref="C127:C139"/>
     <mergeCell ref="C140:C153"/>
     <mergeCell ref="A34:A60"/>
@@ -10140,6 +10129,17 @@
     <mergeCell ref="C34:C46"/>
     <mergeCell ref="B47:B60"/>
     <mergeCell ref="C47:C60"/>
+    <mergeCell ref="A22:A31"/>
+    <mergeCell ref="A8:C11"/>
+    <mergeCell ref="B13:C15"/>
+    <mergeCell ref="B22:B27"/>
+    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="B16:C19"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C30:C31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="58" fitToHeight="5" orientation="landscape" r:id="rId1"/>
@@ -10153,9 +10153,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AA233"/>
+  <dimension ref="A3:AA233"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -10173,11 +10173,6 @@
     <col min="23" max="23" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>136</v>
-      </c>
-    </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>102</v>

</xml_diff>